<commit_message>
slow going, but getting there
</commit_message>
<xml_diff>
--- a/tests/simple.xlsx
+++ b/tests/simple.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="0" windowWidth="25605" windowHeight="14715" tabRatio="861" activeTab="11"/>
+    <workbookView xWindow="900" yWindow="0" windowWidth="25605" windowHeight="14715" tabRatio="861" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -12,9 +12,9 @@
     <sheet name="Population size" sheetId="4" r:id="rId3"/>
     <sheet name="HIV prevalence" sheetId="15" r:id="rId4"/>
     <sheet name="Other epidemiology" sheetId="6" r:id="rId5"/>
-    <sheet name="Cascade" sheetId="18" r:id="rId6"/>
-    <sheet name="Optional indicators" sheetId="5" r:id="rId7"/>
-    <sheet name="Testing &amp; treatment" sheetId="7" r:id="rId8"/>
+    <sheet name="Optional indicators" sheetId="5" r:id="rId6"/>
+    <sheet name="Testing &amp; treatment" sheetId="7" r:id="rId7"/>
+    <sheet name="Cascade" sheetId="18" r:id="rId8"/>
     <sheet name="Sexual behavior" sheetId="8" r:id="rId9"/>
     <sheet name="Injecting behavior" sheetId="9" r:id="rId10"/>
     <sheet name="Partnerships &amp; transitions" sheetId="10" r:id="rId11"/>
@@ -884,12 +884,6 @@
     <xf numFmtId="9" fontId="1" fillId="8" borderId="2" xfId="104" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="113"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="113" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -910,6 +904,12 @@
     </xf>
     <xf numFmtId="165" fontId="16" fillId="10" borderId="2" xfId="113" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="114">
@@ -2290,15 +2290,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32"/>
+      <c r="A2" s="41"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32"/>
+      <c r="A3" s="41"/>
     </row>
     <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -3037,7 +3037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
@@ -5229,1616 +5229,6 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y67"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-    </row>
-    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="37">
-        <v>2000</v>
-      </c>
-      <c r="D2" s="37">
-        <v>2001</v>
-      </c>
-      <c r="E2" s="37">
-        <v>2002</v>
-      </c>
-      <c r="F2" s="37">
-        <v>2003</v>
-      </c>
-      <c r="G2" s="37">
-        <v>2004</v>
-      </c>
-      <c r="H2" s="37">
-        <v>2005</v>
-      </c>
-      <c r="I2" s="37">
-        <v>2006</v>
-      </c>
-      <c r="J2" s="37">
-        <v>2007</v>
-      </c>
-      <c r="K2" s="37">
-        <v>2008</v>
-      </c>
-      <c r="L2" s="37">
-        <v>2009</v>
-      </c>
-      <c r="M2" s="37">
-        <v>2010</v>
-      </c>
-      <c r="N2" s="37">
-        <v>2011</v>
-      </c>
-      <c r="O2" s="37">
-        <v>2012</v>
-      </c>
-      <c r="P2" s="37">
-        <v>2013</v>
-      </c>
-      <c r="Q2" s="37">
-        <v>2014</v>
-      </c>
-      <c r="R2" s="37">
-        <v>2015</v>
-      </c>
-      <c r="S2" s="37">
-        <v>2016</v>
-      </c>
-      <c r="T2" s="37">
-        <v>2017</v>
-      </c>
-      <c r="U2" s="37">
-        <v>2018</v>
-      </c>
-      <c r="V2" s="37">
-        <v>2019</v>
-      </c>
-      <c r="W2" s="37">
-        <v>2020</v>
-      </c>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="35"/>
-      <c r="V3" s="35"/>
-      <c r="W3" s="35"/>
-      <c r="X3" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y3" s="39">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="35"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35"/>
-      <c r="V4" s="35"/>
-      <c r="W4" s="35"/>
-      <c r="X4" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y4" s="39">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="33"/>
-      <c r="S8" s="33"/>
-      <c r="T8" s="33"/>
-      <c r="U8" s="33"/>
-      <c r="V8" s="33"/>
-      <c r="W8" s="33"/>
-      <c r="X8" s="33"/>
-      <c r="Y8" s="33"/>
-    </row>
-    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="37">
-        <v>2000</v>
-      </c>
-      <c r="D9" s="37">
-        <v>2001</v>
-      </c>
-      <c r="E9" s="37">
-        <v>2002</v>
-      </c>
-      <c r="F9" s="37">
-        <v>2003</v>
-      </c>
-      <c r="G9" s="37">
-        <v>2004</v>
-      </c>
-      <c r="H9" s="37">
-        <v>2005</v>
-      </c>
-      <c r="I9" s="37">
-        <v>2006</v>
-      </c>
-      <c r="J9" s="37">
-        <v>2007</v>
-      </c>
-      <c r="K9" s="37">
-        <v>2008</v>
-      </c>
-      <c r="L9" s="37">
-        <v>2009</v>
-      </c>
-      <c r="M9" s="37">
-        <v>2010</v>
-      </c>
-      <c r="N9" s="37">
-        <v>2011</v>
-      </c>
-      <c r="O9" s="37">
-        <v>2012</v>
-      </c>
-      <c r="P9" s="37">
-        <v>2013</v>
-      </c>
-      <c r="Q9" s="37">
-        <v>2014</v>
-      </c>
-      <c r="R9" s="37">
-        <v>2015</v>
-      </c>
-      <c r="S9" s="37">
-        <v>2016</v>
-      </c>
-      <c r="T9" s="37">
-        <v>2017</v>
-      </c>
-      <c r="U9" s="37">
-        <v>2018</v>
-      </c>
-      <c r="V9" s="37">
-        <v>2019</v>
-      </c>
-      <c r="W9" s="37">
-        <v>2020</v>
-      </c>
-      <c r="X9" s="33"/>
-      <c r="Y9" s="37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="35"/>
-      <c r="S10" s="35"/>
-      <c r="T10" s="35"/>
-      <c r="U10" s="35"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="35"/>
-      <c r="X10" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y10" s="39">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="35"/>
-      <c r="T11" s="35"/>
-      <c r="U11" s="35"/>
-      <c r="V11" s="35"/>
-      <c r="W11" s="35"/>
-      <c r="X11" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y11" s="39">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="33"/>
-      <c r="R15" s="33"/>
-      <c r="S15" s="33"/>
-      <c r="T15" s="33"/>
-      <c r="U15" s="33"/>
-      <c r="V15" s="33"/>
-      <c r="W15" s="33"/>
-      <c r="X15" s="33"/>
-      <c r="Y15" s="33"/>
-    </row>
-    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="37">
-        <v>2000</v>
-      </c>
-      <c r="D16" s="37">
-        <v>2001</v>
-      </c>
-      <c r="E16" s="37">
-        <v>2002</v>
-      </c>
-      <c r="F16" s="37">
-        <v>2003</v>
-      </c>
-      <c r="G16" s="37">
-        <v>2004</v>
-      </c>
-      <c r="H16" s="37">
-        <v>2005</v>
-      </c>
-      <c r="I16" s="37">
-        <v>2006</v>
-      </c>
-      <c r="J16" s="37">
-        <v>2007</v>
-      </c>
-      <c r="K16" s="37">
-        <v>2008</v>
-      </c>
-      <c r="L16" s="37">
-        <v>2009</v>
-      </c>
-      <c r="M16" s="37">
-        <v>2010</v>
-      </c>
-      <c r="N16" s="37">
-        <v>2011</v>
-      </c>
-      <c r="O16" s="37">
-        <v>2012</v>
-      </c>
-      <c r="P16" s="37">
-        <v>2013</v>
-      </c>
-      <c r="Q16" s="37">
-        <v>2014</v>
-      </c>
-      <c r="R16" s="37">
-        <v>2015</v>
-      </c>
-      <c r="S16" s="37">
-        <v>2016</v>
-      </c>
-      <c r="T16" s="37">
-        <v>2017</v>
-      </c>
-      <c r="U16" s="37">
-        <v>2018</v>
-      </c>
-      <c r="V16" s="37">
-        <v>2019</v>
-      </c>
-      <c r="W16" s="37">
-        <v>2020</v>
-      </c>
-      <c r="X16" s="33"/>
-      <c r="Y16" s="37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
-      <c r="B17" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
-      <c r="X17" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y17" s="39">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
-      <c r="X18" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y18" s="39">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
-      <c r="R22" s="33"/>
-      <c r="S22" s="33"/>
-      <c r="T22" s="33"/>
-      <c r="U22" s="33"/>
-      <c r="V22" s="33"/>
-      <c r="W22" s="33"/>
-      <c r="X22" s="33"/>
-      <c r="Y22" s="33"/>
-    </row>
-    <row r="23" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="37">
-        <v>2000</v>
-      </c>
-      <c r="D23" s="37">
-        <v>2001</v>
-      </c>
-      <c r="E23" s="37">
-        <v>2002</v>
-      </c>
-      <c r="F23" s="37">
-        <v>2003</v>
-      </c>
-      <c r="G23" s="37">
-        <v>2004</v>
-      </c>
-      <c r="H23" s="37">
-        <v>2005</v>
-      </c>
-      <c r="I23" s="37">
-        <v>2006</v>
-      </c>
-      <c r="J23" s="37">
-        <v>2007</v>
-      </c>
-      <c r="K23" s="37">
-        <v>2008</v>
-      </c>
-      <c r="L23" s="37">
-        <v>2009</v>
-      </c>
-      <c r="M23" s="37">
-        <v>2010</v>
-      </c>
-      <c r="N23" s="37">
-        <v>2011</v>
-      </c>
-      <c r="O23" s="37">
-        <v>2012</v>
-      </c>
-      <c r="P23" s="37">
-        <v>2013</v>
-      </c>
-      <c r="Q23" s="37">
-        <v>2014</v>
-      </c>
-      <c r="R23" s="37">
-        <v>2015</v>
-      </c>
-      <c r="S23" s="37">
-        <v>2016</v>
-      </c>
-      <c r="T23" s="37">
-        <v>2017</v>
-      </c>
-      <c r="U23" s="37">
-        <v>2018</v>
-      </c>
-      <c r="V23" s="37">
-        <v>2019</v>
-      </c>
-      <c r="W23" s="37">
-        <v>2020</v>
-      </c>
-      <c r="X23" s="33"/>
-      <c r="Y23" s="37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
-      <c r="B24" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="35"/>
-      <c r="P24" s="35"/>
-      <c r="Q24" s="35"/>
-      <c r="R24" s="35"/>
-      <c r="S24" s="35"/>
-      <c r="T24" s="35"/>
-      <c r="U24" s="35"/>
-      <c r="V24" s="35"/>
-      <c r="W24" s="35"/>
-      <c r="X24" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y24" s="39">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
-      <c r="B25" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="35"/>
-      <c r="P25" s="35"/>
-      <c r="Q25" s="35"/>
-      <c r="R25" s="35"/>
-      <c r="S25" s="35"/>
-      <c r="T25" s="35"/>
-      <c r="U25" s="35"/>
-      <c r="V25" s="35"/>
-      <c r="W25" s="35"/>
-      <c r="X25" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y25" s="39">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="33"/>
-      <c r="Q29" s="33"/>
-      <c r="R29" s="33"/>
-      <c r="S29" s="33"/>
-      <c r="T29" s="33"/>
-      <c r="U29" s="33"/>
-      <c r="V29" s="33"/>
-      <c r="W29" s="33"/>
-      <c r="X29" s="33"/>
-      <c r="Y29" s="33"/>
-    </row>
-    <row r="30" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="37">
-        <v>2000</v>
-      </c>
-      <c r="D30" s="37">
-        <v>2001</v>
-      </c>
-      <c r="E30" s="37">
-        <v>2002</v>
-      </c>
-      <c r="F30" s="37">
-        <v>2003</v>
-      </c>
-      <c r="G30" s="37">
-        <v>2004</v>
-      </c>
-      <c r="H30" s="37">
-        <v>2005</v>
-      </c>
-      <c r="I30" s="37">
-        <v>2006</v>
-      </c>
-      <c r="J30" s="37">
-        <v>2007</v>
-      </c>
-      <c r="K30" s="37">
-        <v>2008</v>
-      </c>
-      <c r="L30" s="37">
-        <v>2009</v>
-      </c>
-      <c r="M30" s="37">
-        <v>2010</v>
-      </c>
-      <c r="N30" s="37">
-        <v>2011</v>
-      </c>
-      <c r="O30" s="37">
-        <v>2012</v>
-      </c>
-      <c r="P30" s="37">
-        <v>2013</v>
-      </c>
-      <c r="Q30" s="37">
-        <v>2014</v>
-      </c>
-      <c r="R30" s="37">
-        <v>2015</v>
-      </c>
-      <c r="S30" s="37">
-        <v>2016</v>
-      </c>
-      <c r="T30" s="37">
-        <v>2017</v>
-      </c>
-      <c r="U30" s="37">
-        <v>2018</v>
-      </c>
-      <c r="V30" s="37">
-        <v>2019</v>
-      </c>
-      <c r="W30" s="37">
-        <v>2020</v>
-      </c>
-      <c r="X30" s="33"/>
-      <c r="Y30" s="37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
-      <c r="B31" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="39"/>
-      <c r="N31" s="39"/>
-      <c r="O31" s="39"/>
-      <c r="P31" s="39"/>
-      <c r="Q31" s="39"/>
-      <c r="R31" s="39"/>
-      <c r="S31" s="39"/>
-      <c r="T31" s="39"/>
-      <c r="U31" s="39"/>
-      <c r="V31" s="39"/>
-      <c r="W31" s="39"/>
-      <c r="X31" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y31" s="39">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="33"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="33"/>
-      <c r="N35" s="33"/>
-      <c r="O35" s="33"/>
-      <c r="P35" s="33"/>
-      <c r="Q35" s="33"/>
-      <c r="R35" s="33"/>
-      <c r="S35" s="33"/>
-      <c r="T35" s="33"/>
-      <c r="U35" s="33"/>
-      <c r="V35" s="33"/>
-      <c r="W35" s="33"/>
-      <c r="X35" s="33"/>
-      <c r="Y35" s="33"/>
-    </row>
-    <row r="36" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="37">
-        <v>2000</v>
-      </c>
-      <c r="D36" s="37">
-        <v>2001</v>
-      </c>
-      <c r="E36" s="37">
-        <v>2002</v>
-      </c>
-      <c r="F36" s="37">
-        <v>2003</v>
-      </c>
-      <c r="G36" s="37">
-        <v>2004</v>
-      </c>
-      <c r="H36" s="37">
-        <v>2005</v>
-      </c>
-      <c r="I36" s="37">
-        <v>2006</v>
-      </c>
-      <c r="J36" s="37">
-        <v>2007</v>
-      </c>
-      <c r="K36" s="37">
-        <v>2008</v>
-      </c>
-      <c r="L36" s="37">
-        <v>2009</v>
-      </c>
-      <c r="M36" s="37">
-        <v>2010</v>
-      </c>
-      <c r="N36" s="37">
-        <v>2011</v>
-      </c>
-      <c r="O36" s="37">
-        <v>2012</v>
-      </c>
-      <c r="P36" s="37">
-        <v>2013</v>
-      </c>
-      <c r="Q36" s="37">
-        <v>2014</v>
-      </c>
-      <c r="R36" s="37">
-        <v>2015</v>
-      </c>
-      <c r="S36" s="37">
-        <v>2016</v>
-      </c>
-      <c r="T36" s="37">
-        <v>2017</v>
-      </c>
-      <c r="U36" s="37">
-        <v>2018</v>
-      </c>
-      <c r="V36" s="37">
-        <v>2019</v>
-      </c>
-      <c r="W36" s="37">
-        <v>2020</v>
-      </c>
-      <c r="X36" s="33"/>
-      <c r="Y36" s="37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
-      <c r="B37" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="39"/>
-      <c r="K37" s="39"/>
-      <c r="L37" s="39"/>
-      <c r="M37" s="39"/>
-      <c r="N37" s="39"/>
-      <c r="O37" s="39"/>
-      <c r="P37" s="39"/>
-      <c r="Q37" s="39"/>
-      <c r="R37" s="39"/>
-      <c r="S37" s="39"/>
-      <c r="T37" s="39"/>
-      <c r="U37" s="39"/>
-      <c r="V37" s="39"/>
-      <c r="W37" s="39"/>
-      <c r="X37" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y37" s="39">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="33"/>
-      <c r="J41" s="33"/>
-      <c r="K41" s="33"/>
-      <c r="L41" s="33"/>
-      <c r="M41" s="33"/>
-      <c r="N41" s="33"/>
-      <c r="O41" s="33"/>
-      <c r="P41" s="33"/>
-      <c r="Q41" s="33"/>
-      <c r="R41" s="33"/>
-      <c r="S41" s="33"/>
-      <c r="T41" s="33"/>
-      <c r="U41" s="33"/>
-      <c r="V41" s="33"/>
-      <c r="W41" s="33"/>
-      <c r="X41" s="33"/>
-      <c r="Y41" s="33"/>
-    </row>
-    <row r="42" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="33"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="37">
-        <v>2000</v>
-      </c>
-      <c r="D42" s="37">
-        <v>2001</v>
-      </c>
-      <c r="E42" s="37">
-        <v>2002</v>
-      </c>
-      <c r="F42" s="37">
-        <v>2003</v>
-      </c>
-      <c r="G42" s="37">
-        <v>2004</v>
-      </c>
-      <c r="H42" s="37">
-        <v>2005</v>
-      </c>
-      <c r="I42" s="37">
-        <v>2006</v>
-      </c>
-      <c r="J42" s="37">
-        <v>2007</v>
-      </c>
-      <c r="K42" s="37">
-        <v>2008</v>
-      </c>
-      <c r="L42" s="37">
-        <v>2009</v>
-      </c>
-      <c r="M42" s="37">
-        <v>2010</v>
-      </c>
-      <c r="N42" s="37">
-        <v>2011</v>
-      </c>
-      <c r="O42" s="37">
-        <v>2012</v>
-      </c>
-      <c r="P42" s="37">
-        <v>2013</v>
-      </c>
-      <c r="Q42" s="37">
-        <v>2014</v>
-      </c>
-      <c r="R42" s="37">
-        <v>2015</v>
-      </c>
-      <c r="S42" s="37">
-        <v>2016</v>
-      </c>
-      <c r="T42" s="37">
-        <v>2017</v>
-      </c>
-      <c r="U42" s="37">
-        <v>2018</v>
-      </c>
-      <c r="V42" s="37">
-        <v>2019</v>
-      </c>
-      <c r="W42" s="37">
-        <v>2020</v>
-      </c>
-      <c r="X42" s="33"/>
-      <c r="Y42" s="37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="33"/>
-      <c r="B43" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="40"/>
-      <c r="F43" s="40"/>
-      <c r="G43" s="40"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
-      <c r="K43" s="40"/>
-      <c r="L43" s="40"/>
-      <c r="M43" s="40"/>
-      <c r="N43" s="40"/>
-      <c r="O43" s="40"/>
-      <c r="P43" s="40"/>
-      <c r="Q43" s="40"/>
-      <c r="R43" s="40"/>
-      <c r="S43" s="40"/>
-      <c r="T43" s="40"/>
-      <c r="U43" s="40"/>
-      <c r="V43" s="40"/>
-      <c r="W43" s="40"/>
-      <c r="X43" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y43" s="41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="33"/>
-      <c r="J47" s="33"/>
-      <c r="K47" s="33"/>
-      <c r="L47" s="33"/>
-      <c r="M47" s="33"/>
-      <c r="N47" s="33"/>
-      <c r="O47" s="33"/>
-      <c r="P47" s="33"/>
-      <c r="Q47" s="33"/>
-      <c r="R47" s="33"/>
-      <c r="S47" s="33"/>
-      <c r="T47" s="33"/>
-      <c r="U47" s="33"/>
-      <c r="V47" s="33"/>
-      <c r="W47" s="33"/>
-      <c r="X47" s="33"/>
-      <c r="Y47" s="33"/>
-    </row>
-    <row r="48" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="33"/>
-      <c r="B48" s="33"/>
-      <c r="C48" s="37">
-        <v>2000</v>
-      </c>
-      <c r="D48" s="37">
-        <v>2001</v>
-      </c>
-      <c r="E48" s="37">
-        <v>2002</v>
-      </c>
-      <c r="F48" s="37">
-        <v>2003</v>
-      </c>
-      <c r="G48" s="37">
-        <v>2004</v>
-      </c>
-      <c r="H48" s="37">
-        <v>2005</v>
-      </c>
-      <c r="I48" s="37">
-        <v>2006</v>
-      </c>
-      <c r="J48" s="37">
-        <v>2007</v>
-      </c>
-      <c r="K48" s="37">
-        <v>2008</v>
-      </c>
-      <c r="L48" s="37">
-        <v>2009</v>
-      </c>
-      <c r="M48" s="37">
-        <v>2010</v>
-      </c>
-      <c r="N48" s="37">
-        <v>2011</v>
-      </c>
-      <c r="O48" s="37">
-        <v>2012</v>
-      </c>
-      <c r="P48" s="37">
-        <v>2013</v>
-      </c>
-      <c r="Q48" s="37">
-        <v>2014</v>
-      </c>
-      <c r="R48" s="37">
-        <v>2015</v>
-      </c>
-      <c r="S48" s="37">
-        <v>2016</v>
-      </c>
-      <c r="T48" s="37">
-        <v>2017</v>
-      </c>
-      <c r="U48" s="37">
-        <v>2018</v>
-      </c>
-      <c r="V48" s="37">
-        <v>2019</v>
-      </c>
-      <c r="W48" s="37">
-        <v>2020</v>
-      </c>
-      <c r="X48" s="33"/>
-      <c r="Y48" s="37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="33"/>
-      <c r="B49" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="39"/>
-      <c r="H49" s="39"/>
-      <c r="I49" s="39"/>
-      <c r="J49" s="39"/>
-      <c r="K49" s="39"/>
-      <c r="L49" s="39"/>
-      <c r="M49" s="39"/>
-      <c r="N49" s="39"/>
-      <c r="O49" s="39"/>
-      <c r="P49" s="39"/>
-      <c r="Q49" s="39"/>
-      <c r="R49" s="39"/>
-      <c r="S49" s="39"/>
-      <c r="T49" s="39"/>
-      <c r="U49" s="39"/>
-      <c r="V49" s="39"/>
-      <c r="W49" s="39"/>
-      <c r="X49" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y49" s="39">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="53" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="B53" s="33"/>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="33"/>
-      <c r="H53" s="33"/>
-      <c r="I53" s="33"/>
-      <c r="J53" s="33"/>
-      <c r="K53" s="33"/>
-      <c r="L53" s="33"/>
-      <c r="M53" s="33"/>
-      <c r="N53" s="33"/>
-      <c r="O53" s="33"/>
-      <c r="P53" s="33"/>
-      <c r="Q53" s="33"/>
-      <c r="R53" s="33"/>
-      <c r="S53" s="33"/>
-      <c r="T53" s="33"/>
-      <c r="U53" s="33"/>
-      <c r="V53" s="33"/>
-      <c r="W53" s="33"/>
-      <c r="X53" s="33"/>
-      <c r="Y53" s="33"/>
-    </row>
-    <row r="54" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="33"/>
-      <c r="B54" s="33"/>
-      <c r="C54" s="37">
-        <v>2000</v>
-      </c>
-      <c r="D54" s="37">
-        <v>2001</v>
-      </c>
-      <c r="E54" s="37">
-        <v>2002</v>
-      </c>
-      <c r="F54" s="37">
-        <v>2003</v>
-      </c>
-      <c r="G54" s="37">
-        <v>2004</v>
-      </c>
-      <c r="H54" s="37">
-        <v>2005</v>
-      </c>
-      <c r="I54" s="37">
-        <v>2006</v>
-      </c>
-      <c r="J54" s="37">
-        <v>2007</v>
-      </c>
-      <c r="K54" s="37">
-        <v>2008</v>
-      </c>
-      <c r="L54" s="37">
-        <v>2009</v>
-      </c>
-      <c r="M54" s="37">
-        <v>2010</v>
-      </c>
-      <c r="N54" s="37">
-        <v>2011</v>
-      </c>
-      <c r="O54" s="37">
-        <v>2012</v>
-      </c>
-      <c r="P54" s="37">
-        <v>2013</v>
-      </c>
-      <c r="Q54" s="37">
-        <v>2014</v>
-      </c>
-      <c r="R54" s="37">
-        <v>2015</v>
-      </c>
-      <c r="S54" s="37">
-        <v>2016</v>
-      </c>
-      <c r="T54" s="37">
-        <v>2017</v>
-      </c>
-      <c r="U54" s="37">
-        <v>2018</v>
-      </c>
-      <c r="V54" s="37">
-        <v>2019</v>
-      </c>
-      <c r="W54" s="37">
-        <v>2020</v>
-      </c>
-      <c r="X54" s="33"/>
-      <c r="Y54" s="37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="33"/>
-      <c r="B55" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="39"/>
-      <c r="I55" s="39"/>
-      <c r="J55" s="39"/>
-      <c r="K55" s="39"/>
-      <c r="L55" s="39"/>
-      <c r="M55" s="39"/>
-      <c r="N55" s="39"/>
-      <c r="O55" s="39"/>
-      <c r="P55" s="39"/>
-      <c r="Q55" s="39"/>
-      <c r="R55" s="39"/>
-      <c r="S55" s="39"/>
-      <c r="T55" s="39"/>
-      <c r="U55" s="39"/>
-      <c r="V55" s="39"/>
-      <c r="W55" s="39"/>
-      <c r="X55" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y55" s="39">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="59" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="B59" s="33"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="33"/>
-      <c r="H59" s="33"/>
-      <c r="I59" s="33"/>
-      <c r="J59" s="33"/>
-      <c r="K59" s="33"/>
-      <c r="L59" s="33"/>
-      <c r="M59" s="33"/>
-      <c r="N59" s="33"/>
-      <c r="O59" s="33"/>
-      <c r="P59" s="33"/>
-      <c r="Q59" s="33"/>
-      <c r="R59" s="33"/>
-      <c r="S59" s="33"/>
-      <c r="T59" s="33"/>
-      <c r="U59" s="33"/>
-      <c r="V59" s="33"/>
-      <c r="W59" s="33"/>
-      <c r="X59" s="33"/>
-      <c r="Y59" s="33"/>
-    </row>
-    <row r="60" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="33"/>
-      <c r="B60" s="33"/>
-      <c r="C60" s="37">
-        <v>2000</v>
-      </c>
-      <c r="D60" s="37">
-        <v>2001</v>
-      </c>
-      <c r="E60" s="37">
-        <v>2002</v>
-      </c>
-      <c r="F60" s="37">
-        <v>2003</v>
-      </c>
-      <c r="G60" s="37">
-        <v>2004</v>
-      </c>
-      <c r="H60" s="37">
-        <v>2005</v>
-      </c>
-      <c r="I60" s="37">
-        <v>2006</v>
-      </c>
-      <c r="J60" s="37">
-        <v>2007</v>
-      </c>
-      <c r="K60" s="37">
-        <v>2008</v>
-      </c>
-      <c r="L60" s="37">
-        <v>2009</v>
-      </c>
-      <c r="M60" s="37">
-        <v>2010</v>
-      </c>
-      <c r="N60" s="37">
-        <v>2011</v>
-      </c>
-      <c r="O60" s="37">
-        <v>2012</v>
-      </c>
-      <c r="P60" s="37">
-        <v>2013</v>
-      </c>
-      <c r="Q60" s="37">
-        <v>2014</v>
-      </c>
-      <c r="R60" s="37">
-        <v>2015</v>
-      </c>
-      <c r="S60" s="37">
-        <v>2016</v>
-      </c>
-      <c r="T60" s="37">
-        <v>2017</v>
-      </c>
-      <c r="U60" s="37">
-        <v>2018</v>
-      </c>
-      <c r="V60" s="37">
-        <v>2019</v>
-      </c>
-      <c r="W60" s="37">
-        <v>2020</v>
-      </c>
-      <c r="X60" s="33"/>
-      <c r="Y60" s="37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="33"/>
-      <c r="B61" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="39"/>
-      <c r="I61" s="39"/>
-      <c r="J61" s="39"/>
-      <c r="K61" s="39"/>
-      <c r="L61" s="39"/>
-      <c r="M61" s="39"/>
-      <c r="N61" s="39"/>
-      <c r="O61" s="39"/>
-      <c r="P61" s="39"/>
-      <c r="Q61" s="39"/>
-      <c r="R61" s="39"/>
-      <c r="S61" s="39"/>
-      <c r="T61" s="39"/>
-      <c r="U61" s="39"/>
-      <c r="V61" s="39"/>
-      <c r="W61" s="39"/>
-      <c r="X61" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y61" s="39">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="65" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="B65" s="33"/>
-      <c r="C65" s="33"/>
-      <c r="D65" s="33"/>
-      <c r="E65" s="33"/>
-      <c r="F65" s="33"/>
-      <c r="G65" s="33"/>
-      <c r="H65" s="33"/>
-      <c r="I65" s="33"/>
-      <c r="J65" s="33"/>
-      <c r="K65" s="33"/>
-      <c r="L65" s="33"/>
-      <c r="M65" s="33"/>
-      <c r="N65" s="33"/>
-      <c r="O65" s="33"/>
-      <c r="P65" s="33"/>
-      <c r="Q65" s="33"/>
-      <c r="R65" s="33"/>
-      <c r="S65" s="33"/>
-      <c r="T65" s="33"/>
-      <c r="U65" s="33"/>
-      <c r="V65" s="33"/>
-      <c r="W65" s="33"/>
-      <c r="X65" s="33"/>
-      <c r="Y65" s="33"/>
-    </row>
-    <row r="66" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="33"/>
-      <c r="B66" s="33"/>
-      <c r="C66" s="37">
-        <v>2000</v>
-      </c>
-      <c r="D66" s="37">
-        <v>2001</v>
-      </c>
-      <c r="E66" s="37">
-        <v>2002</v>
-      </c>
-      <c r="F66" s="37">
-        <v>2003</v>
-      </c>
-      <c r="G66" s="37">
-        <v>2004</v>
-      </c>
-      <c r="H66" s="37">
-        <v>2005</v>
-      </c>
-      <c r="I66" s="37">
-        <v>2006</v>
-      </c>
-      <c r="J66" s="37">
-        <v>2007</v>
-      </c>
-      <c r="K66" s="37">
-        <v>2008</v>
-      </c>
-      <c r="L66" s="37">
-        <v>2009</v>
-      </c>
-      <c r="M66" s="37">
-        <v>2010</v>
-      </c>
-      <c r="N66" s="37">
-        <v>2011</v>
-      </c>
-      <c r="O66" s="37">
-        <v>2012</v>
-      </c>
-      <c r="P66" s="37">
-        <v>2013</v>
-      </c>
-      <c r="Q66" s="37">
-        <v>2014</v>
-      </c>
-      <c r="R66" s="37">
-        <v>2015</v>
-      </c>
-      <c r="S66" s="37">
-        <v>2016</v>
-      </c>
-      <c r="T66" s="37">
-        <v>2017</v>
-      </c>
-      <c r="U66" s="37">
-        <v>2018</v>
-      </c>
-      <c r="V66" s="37">
-        <v>2019</v>
-      </c>
-      <c r="W66" s="37">
-        <v>2020</v>
-      </c>
-      <c r="X66" s="33"/>
-      <c r="Y66" s="37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="67" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="33"/>
-      <c r="B67" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C67" s="39"/>
-      <c r="D67" s="39"/>
-      <c r="E67" s="39"/>
-      <c r="F67" s="39"/>
-      <c r="G67" s="39"/>
-      <c r="H67" s="39"/>
-      <c r="I67" s="39"/>
-      <c r="J67" s="39"/>
-      <c r="K67" s="39"/>
-      <c r="L67" s="39"/>
-      <c r="M67" s="39"/>
-      <c r="N67" s="39"/>
-      <c r="O67" s="39"/>
-      <c r="P67" s="39"/>
-      <c r="Q67" s="39"/>
-      <c r="R67" s="39"/>
-      <c r="S67" s="39"/>
-      <c r="T67" s="39"/>
-      <c r="U67" s="39"/>
-      <c r="V67" s="39"/>
-      <c r="W67" s="39"/>
-      <c r="X67" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y67" s="39">
-        <v>0.85</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y39"/>
   <sheetViews>
     <sheetView topLeftCell="F4" workbookViewId="0">
@@ -7599,7 +5989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y41"/>
   <sheetViews>
@@ -8487,6 +6877,1616 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+    </row>
+    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D2" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E2" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F2" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G2" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H2" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I2" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J2" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K2" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L2" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M2" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N2" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O2" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P2" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q2" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R2" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S2" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T2" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U2" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V2" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W2" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
+      <c r="B3" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33"/>
+      <c r="V3" s="33"/>
+      <c r="W3" s="33"/>
+      <c r="X3" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y3" s="37">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="31"/>
+      <c r="B4" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y4" s="37">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="31"/>
+      <c r="V8" s="31"/>
+      <c r="W8" s="31"/>
+      <c r="X8" s="31"/>
+      <c r="Y8" s="31"/>
+    </row>
+    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D9" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E9" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F9" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G9" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H9" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I9" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J9" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K9" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L9" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M9" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N9" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O9" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P9" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q9" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R9" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S9" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T9" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U9" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V9" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W9" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X9" s="31"/>
+      <c r="Y9" s="35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="33"/>
+      <c r="T10" s="33"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="33"/>
+      <c r="X10" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y10" s="37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
+      <c r="B11" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="33"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="33"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="33"/>
+      <c r="X11" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y11" s="37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="31"/>
+      <c r="U15" s="31"/>
+      <c r="V15" s="31"/>
+      <c r="W15" s="31"/>
+      <c r="X15" s="31"/>
+      <c r="Y15" s="31"/>
+    </row>
+    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D16" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E16" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F16" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G16" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H16" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I16" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J16" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K16" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L16" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M16" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N16" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O16" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P16" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q16" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R16" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S16" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T16" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U16" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V16" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W16" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X16" s="31"/>
+      <c r="Y16" s="35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="31"/>
+      <c r="B17" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="33"/>
+      <c r="T17" s="33"/>
+      <c r="U17" s="33"/>
+      <c r="V17" s="33"/>
+      <c r="W17" s="33"/>
+      <c r="X17" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y17" s="37">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="31"/>
+      <c r="B18" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="33"/>
+      <c r="U18" s="33"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="33"/>
+      <c r="X18" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y18" s="37">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="31"/>
+      <c r="W22" s="31"/>
+      <c r="X22" s="31"/>
+      <c r="Y22" s="31"/>
+    </row>
+    <row r="23" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D23" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E23" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F23" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G23" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H23" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I23" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J23" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K23" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L23" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M23" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N23" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O23" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P23" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q23" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R23" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S23" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T23" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U23" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V23" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W23" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X23" s="31"/>
+      <c r="Y23" s="35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="31"/>
+      <c r="B24" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33"/>
+      <c r="Q24" s="33"/>
+      <c r="R24" s="33"/>
+      <c r="S24" s="33"/>
+      <c r="T24" s="33"/>
+      <c r="U24" s="33"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="33"/>
+      <c r="X24" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y24" s="37">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="31"/>
+      <c r="B25" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="33"/>
+      <c r="Q25" s="33"/>
+      <c r="R25" s="33"/>
+      <c r="S25" s="33"/>
+      <c r="T25" s="33"/>
+      <c r="U25" s="33"/>
+      <c r="V25" s="33"/>
+      <c r="W25" s="33"/>
+      <c r="X25" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y25" s="37">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="31"/>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="31"/>
+      <c r="S29" s="31"/>
+      <c r="T29" s="31"/>
+      <c r="U29" s="31"/>
+      <c r="V29" s="31"/>
+      <c r="W29" s="31"/>
+      <c r="X29" s="31"/>
+      <c r="Y29" s="31"/>
+    </row>
+    <row r="30" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="31"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D30" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E30" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F30" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G30" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H30" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I30" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J30" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K30" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L30" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M30" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N30" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O30" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P30" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q30" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R30" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S30" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T30" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U30" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V30" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W30" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X30" s="31"/>
+      <c r="Y30" s="35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="31"/>
+      <c r="B31" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="37"/>
+      <c r="M31" s="37"/>
+      <c r="N31" s="37"/>
+      <c r="O31" s="37"/>
+      <c r="P31" s="37"/>
+      <c r="Q31" s="37"/>
+      <c r="R31" s="37"/>
+      <c r="S31" s="37"/>
+      <c r="T31" s="37"/>
+      <c r="U31" s="37"/>
+      <c r="V31" s="37"/>
+      <c r="W31" s="37"/>
+      <c r="X31" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y31" s="37">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="31"/>
+      <c r="P35" s="31"/>
+      <c r="Q35" s="31"/>
+      <c r="R35" s="31"/>
+      <c r="S35" s="31"/>
+      <c r="T35" s="31"/>
+      <c r="U35" s="31"/>
+      <c r="V35" s="31"/>
+      <c r="W35" s="31"/>
+      <c r="X35" s="31"/>
+      <c r="Y35" s="31"/>
+    </row>
+    <row r="36" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D36" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E36" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F36" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G36" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H36" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I36" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J36" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K36" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L36" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M36" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N36" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O36" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P36" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q36" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R36" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S36" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T36" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U36" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V36" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W36" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X36" s="31"/>
+      <c r="Y36" s="35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="31"/>
+      <c r="B37" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="37"/>
+      <c r="P37" s="37"/>
+      <c r="Q37" s="37"/>
+      <c r="R37" s="37"/>
+      <c r="S37" s="37"/>
+      <c r="T37" s="37"/>
+      <c r="U37" s="37"/>
+      <c r="V37" s="37"/>
+      <c r="W37" s="37"/>
+      <c r="X37" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y37" s="37">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="S41" s="31"/>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+    </row>
+    <row r="42" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D42" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E42" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F42" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G42" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H42" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I42" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J42" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K42" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L42" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M42" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N42" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O42" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P42" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q42" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R42" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S42" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T42" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U42" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V42" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W42" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X42" s="31"/>
+      <c r="Y42" s="35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="31"/>
+      <c r="B43" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
+      <c r="K43" s="38"/>
+      <c r="L43" s="38"/>
+      <c r="M43" s="38"/>
+      <c r="N43" s="38"/>
+      <c r="O43" s="38"/>
+      <c r="P43" s="38"/>
+      <c r="Q43" s="38"/>
+      <c r="R43" s="38"/>
+      <c r="S43" s="38"/>
+      <c r="T43" s="38"/>
+      <c r="U43" s="38"/>
+      <c r="V43" s="38"/>
+      <c r="W43" s="38"/>
+      <c r="X43" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y43" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" s="31"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
+      <c r="K47" s="31"/>
+      <c r="L47" s="31"/>
+      <c r="M47" s="31"/>
+      <c r="N47" s="31"/>
+      <c r="O47" s="31"/>
+      <c r="P47" s="31"/>
+      <c r="Q47" s="31"/>
+      <c r="R47" s="31"/>
+      <c r="S47" s="31"/>
+      <c r="T47" s="31"/>
+      <c r="U47" s="31"/>
+      <c r="V47" s="31"/>
+      <c r="W47" s="31"/>
+      <c r="X47" s="31"/>
+      <c r="Y47" s="31"/>
+    </row>
+    <row r="48" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="31"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D48" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E48" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F48" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G48" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H48" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I48" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J48" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K48" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L48" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M48" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N48" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O48" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P48" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q48" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R48" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S48" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T48" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U48" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V48" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W48" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X48" s="31"/>
+      <c r="Y48" s="35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="31"/>
+      <c r="B49" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="37"/>
+      <c r="L49" s="37"/>
+      <c r="M49" s="37"/>
+      <c r="N49" s="37"/>
+      <c r="O49" s="37"/>
+      <c r="P49" s="37"/>
+      <c r="Q49" s="37"/>
+      <c r="R49" s="37"/>
+      <c r="S49" s="37"/>
+      <c r="T49" s="37"/>
+      <c r="U49" s="37"/>
+      <c r="V49" s="37"/>
+      <c r="W49" s="37"/>
+      <c r="X49" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y49" s="37">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="31"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="31"/>
+      <c r="K53" s="31"/>
+      <c r="L53" s="31"/>
+      <c r="M53" s="31"/>
+      <c r="N53" s="31"/>
+      <c r="O53" s="31"/>
+      <c r="P53" s="31"/>
+      <c r="Q53" s="31"/>
+      <c r="R53" s="31"/>
+      <c r="S53" s="31"/>
+      <c r="T53" s="31"/>
+      <c r="U53" s="31"/>
+      <c r="V53" s="31"/>
+      <c r="W53" s="31"/>
+      <c r="X53" s="31"/>
+      <c r="Y53" s="31"/>
+    </row>
+    <row r="54" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="31"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D54" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E54" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F54" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G54" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H54" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I54" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J54" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K54" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L54" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M54" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N54" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O54" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P54" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q54" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R54" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S54" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T54" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U54" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V54" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W54" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X54" s="31"/>
+      <c r="Y54" s="35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="31"/>
+      <c r="B55" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="37"/>
+      <c r="K55" s="37"/>
+      <c r="L55" s="37"/>
+      <c r="M55" s="37"/>
+      <c r="N55" s="37"/>
+      <c r="O55" s="37"/>
+      <c r="P55" s="37"/>
+      <c r="Q55" s="37"/>
+      <c r="R55" s="37"/>
+      <c r="S55" s="37"/>
+      <c r="T55" s="37"/>
+      <c r="U55" s="37"/>
+      <c r="V55" s="37"/>
+      <c r="W55" s="37"/>
+      <c r="X55" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y55" s="37">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="31"/>
+      <c r="G59" s="31"/>
+      <c r="H59" s="31"/>
+      <c r="I59" s="31"/>
+      <c r="J59" s="31"/>
+      <c r="K59" s="31"/>
+      <c r="L59" s="31"/>
+      <c r="M59" s="31"/>
+      <c r="N59" s="31"/>
+      <c r="O59" s="31"/>
+      <c r="P59" s="31"/>
+      <c r="Q59" s="31"/>
+      <c r="R59" s="31"/>
+      <c r="S59" s="31"/>
+      <c r="T59" s="31"/>
+      <c r="U59" s="31"/>
+      <c r="V59" s="31"/>
+      <c r="W59" s="31"/>
+      <c r="X59" s="31"/>
+      <c r="Y59" s="31"/>
+    </row>
+    <row r="60" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="31"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D60" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E60" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F60" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G60" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H60" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I60" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J60" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K60" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L60" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M60" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N60" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O60" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P60" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q60" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R60" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S60" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T60" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U60" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V60" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W60" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X60" s="31"/>
+      <c r="Y60" s="35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="31"/>
+      <c r="B61" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="37"/>
+      <c r="K61" s="37"/>
+      <c r="L61" s="37"/>
+      <c r="M61" s="37"/>
+      <c r="N61" s="37"/>
+      <c r="O61" s="37"/>
+      <c r="P61" s="37"/>
+      <c r="Q61" s="37"/>
+      <c r="R61" s="37"/>
+      <c r="S61" s="37"/>
+      <c r="T61" s="37"/>
+      <c r="U61" s="37"/>
+      <c r="V61" s="37"/>
+      <c r="W61" s="37"/>
+      <c r="X61" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y61" s="37">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B65" s="31"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="31"/>
+      <c r="F65" s="31"/>
+      <c r="G65" s="31"/>
+      <c r="H65" s="31"/>
+      <c r="I65" s="31"/>
+      <c r="J65" s="31"/>
+      <c r="K65" s="31"/>
+      <c r="L65" s="31"/>
+      <c r="M65" s="31"/>
+      <c r="N65" s="31"/>
+      <c r="O65" s="31"/>
+      <c r="P65" s="31"/>
+      <c r="Q65" s="31"/>
+      <c r="R65" s="31"/>
+      <c r="S65" s="31"/>
+      <c r="T65" s="31"/>
+      <c r="U65" s="31"/>
+      <c r="V65" s="31"/>
+      <c r="W65" s="31"/>
+      <c r="X65" s="31"/>
+      <c r="Y65" s="31"/>
+    </row>
+    <row r="66" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="31"/>
+      <c r="B66" s="31"/>
+      <c r="C66" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D66" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E66" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F66" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G66" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H66" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I66" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J66" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K66" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L66" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M66" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N66" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O66" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P66" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q66" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R66" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S66" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T66" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U66" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V66" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W66" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X66" s="31"/>
+      <c r="Y66" s="35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="31"/>
+      <c r="B67" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C67" s="37"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="37"/>
+      <c r="J67" s="37"/>
+      <c r="K67" s="37"/>
+      <c r="L67" s="37"/>
+      <c r="M67" s="37"/>
+      <c r="N67" s="37"/>
+      <c r="O67" s="37"/>
+      <c r="P67" s="37"/>
+      <c r="Q67" s="37"/>
+      <c r="R67" s="37"/>
+      <c r="S67" s="37"/>
+      <c r="T67" s="37"/>
+      <c r="U67" s="37"/>
+      <c r="V67" s="37"/>
+      <c r="W67" s="37"/>
+      <c r="X67" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y67" s="37">
+        <v>0.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y45"/>

</xml_diff>

<commit_message>
remove prop aware fromcascade sheet, add it and proptreat to optional
</commit_message>
<xml_diff>
--- a/tests/simple.xlsx
+++ b/tests/simple.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="0" windowWidth="25605" windowHeight="14715" tabRatio="861" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="861" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -20,7 +20,12 @@
     <sheet name="Partnerships &amp; transitions" sheetId="10" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -131,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="120">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -488,6 +493,48 @@
   </si>
   <si>
     <t>Proportion of people on ART with viral suppression (%)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Diagnosed </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PLHIV </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">on treatment </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>(%)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -495,8 +542,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
@@ -712,12 +759,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="114">
+  <cellStyleXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -827,8 +874,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -911,14 +962,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="113" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="114">
+  <cellStyles count="118">
     <cellStyle name="Comma 2" xfId="4"/>
     <cellStyle name="Comma 3" xfId="2"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="15"/>
     <cellStyle name="Followed Hyperlink 11" xfId="16"/>
     <cellStyle name="Followed Hyperlink 12" xfId="17"/>
@@ -1020,6 +1074,8 @@
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Normal 3" xfId="6"/>
@@ -2284,34 +2340,34 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="89.7109375" customWidth="1"/>
+    <col min="1" max="1" width="89.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="12.75" customHeight="1">
       <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" s="41"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" s="41"/>
     </row>
-    <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="14">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="67.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="14">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="14">
       <c r="A7" s="21" t="s">
         <v>92</v>
       </c>
@@ -2337,17 +2393,17 @@
       <selection activeCell="X1" sqref="X1:AG1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="25" width="8.85546875" customWidth="1"/>
+    <col min="1" max="25" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -2415,7 +2471,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2448,7 +2504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2481,15 +2537,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="8" spans="1:25" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -2557,7 +2613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2590,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2623,15 +2679,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="13" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="14" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="15" spans="1:25" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -2699,7 +2755,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:25" ht="13.5" customHeight="1">
       <c r="B17" s="22" t="s">
         <v>14</v>
       </c>
@@ -2731,9 +2787,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="2:25" ht="13.5" customHeight="1"/>
+    <row r="19" spans="2:25" ht="13.5" customHeight="1"/>
+    <row r="20" spans="2:25" ht="13.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2752,21 +2808,21 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="6" width="8.85546875" customWidth="1"/>
+    <col min="1" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="6" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13.5" customHeight="1">
       <c r="C2" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2776,7 +2832,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2786,7 +2842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2794,26 +2850,26 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13.5" customHeight="1">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="13.5" customHeight="1">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="13.5" customHeight="1">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="13.5" customHeight="1">
       <c r="C9" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2823,7 +2879,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="13.5" customHeight="1">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2833,7 +2889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="13.5" customHeight="1">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2841,26 +2897,26 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="13.5" customHeight="1">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="13.5" customHeight="1">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="13.5" customHeight="1">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="13.5" customHeight="1">
       <c r="C16" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2870,7 +2926,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="13.5" customHeight="1">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2878,7 +2934,7 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="13.5" customHeight="1">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2886,26 +2942,26 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="13.5" customHeight="1">
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="13.5" customHeight="1">
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="13.5" customHeight="1">
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="13.5" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="13.5" customHeight="1">
       <c r="C23" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2915,7 +2971,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="13.5" customHeight="1">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2923,7 +2979,7 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="13.5" customHeight="1">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2931,14 +2987,14 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="13.5" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="13.5" customHeight="1">
       <c r="C30" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2948,7 +3004,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="13.5" customHeight="1">
       <c r="B31" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2956,14 +3012,14 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="35" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="13.5" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>112</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="13.5" customHeight="1">
       <c r="C36" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2973,7 +3029,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="13.5" customHeight="1">
       <c r="B37" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2981,7 +3037,7 @@
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="13.5" customHeight="1">
       <c r="B38" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2989,14 +3045,14 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="42" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="13.5" customHeight="1">
       <c r="A42" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="13.5" customHeight="1">
       <c r="C43" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3006,7 +3062,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="13.5" customHeight="1">
       <c r="B44" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3014,7 +3070,7 @@
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="13.5" customHeight="1">
       <c r="B45" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3041,14 +3097,14 @@
       <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="6" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="6" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="13.5" customHeight="1">
       <c r="A1" s="25" t="s">
         <v>49</v>
       </c>
@@ -3057,7 +3113,7 @@
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.5" customHeight="1">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="27" t="s">
@@ -3070,7 +3126,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.5" customHeight="1">
       <c r="A3" s="24"/>
       <c r="B3" s="26" t="s">
         <v>50</v>
@@ -3085,7 +3141,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.5" customHeight="1">
       <c r="A4" s="24"/>
       <c r="B4" s="26" t="s">
         <v>51</v>
@@ -3100,7 +3156,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.5" customHeight="1">
       <c r="A5" s="24"/>
       <c r="B5" s="26" t="s">
         <v>52</v>
@@ -3115,7 +3171,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.5" customHeight="1">
       <c r="A6" s="24"/>
       <c r="B6" s="26" t="s">
         <v>53</v>
@@ -3130,7 +3186,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.5" customHeight="1">
       <c r="A7" s="24"/>
       <c r="B7" s="26" t="s">
         <v>54</v>
@@ -3145,7 +3201,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.5" customHeight="1">
       <c r="A8" s="24"/>
       <c r="B8" s="26" t="s">
         <v>55</v>
@@ -3160,7 +3216,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.5" customHeight="1">
       <c r="A9" s="24"/>
       <c r="B9" s="26" t="s">
         <v>56</v>
@@ -3175,16 +3231,16 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.5" customHeight="1">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="13.5" customHeight="1">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="13.5" customHeight="1">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="13.5" customHeight="1">
       <c r="A13" s="25" t="s">
         <v>57</v>
       </c>
@@ -3193,7 +3249,7 @@
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="13.5" customHeight="1">
       <c r="A14" s="24"/>
       <c r="B14" s="24"/>
       <c r="C14" s="27" t="s">
@@ -3206,7 +3262,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="13.5" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="26" t="s">
         <v>58</v>
@@ -3221,7 +3277,7 @@
         <v>48.02</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="13.5" customHeight="1">
       <c r="A16" s="24"/>
       <c r="B16" s="26" t="s">
         <v>59</v>
@@ -3236,7 +3292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="13.5" customHeight="1">
       <c r="A17" s="24"/>
       <c r="B17" s="26" t="s">
         <v>60</v>
@@ -3251,7 +3307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="13.5" customHeight="1">
       <c r="A18" s="24"/>
       <c r="B18" s="26" t="s">
         <v>61</v>
@@ -3266,7 +3322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="13.5" customHeight="1">
       <c r="A19" s="24"/>
       <c r="B19" s="26" t="s">
         <v>62</v>
@@ -3281,7 +3337,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="13.5" customHeight="1">
       <c r="A20" s="24"/>
       <c r="B20" s="26" t="s">
         <v>63</v>
@@ -3296,16 +3352,16 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="13.5" customHeight="1">
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="13.5" customHeight="1">
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="13.5" customHeight="1">
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="13.5" customHeight="1">
       <c r="A24" s="25" t="s">
         <v>64</v>
       </c>
@@ -3314,7 +3370,7 @@
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
     </row>
-    <row r="25" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="13.5" customHeight="1">
       <c r="A25" s="24"/>
       <c r="B25" s="24"/>
       <c r="C25" s="27" t="s">
@@ -3327,7 +3383,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="13.5" customHeight="1">
       <c r="A26" s="24"/>
       <c r="B26" s="26" t="s">
         <v>65</v>
@@ -3342,7 +3398,7 @@
         <v>9.76</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="13.5" customHeight="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26" t="s">
         <v>60</v>
@@ -3357,7 +3413,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="13.5" customHeight="1">
       <c r="A28" s="24"/>
       <c r="B28" s="26" t="s">
         <v>99</v>
@@ -3372,7 +3428,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="13.5" customHeight="1">
       <c r="A29" s="24"/>
       <c r="B29" s="26" t="s">
         <v>66</v>
@@ -3387,7 +3443,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="13.5" customHeight="1">
       <c r="A30" s="24"/>
       <c r="B30" s="26" t="s">
         <v>67</v>
@@ -3402,16 +3458,16 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="13.5" customHeight="1">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="13.5" customHeight="1">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="13.5" customHeight="1">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="13.5" customHeight="1">
       <c r="A34" s="25" t="s">
         <v>68</v>
       </c>
@@ -3420,7 +3476,7 @@
       <c r="D34" s="24"/>
       <c r="E34" s="24"/>
     </row>
-    <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="13.5" customHeight="1">
       <c r="A35" s="24"/>
       <c r="B35" s="24"/>
       <c r="C35" s="27" t="s">
@@ -3433,7 +3489,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="13.5" customHeight="1">
       <c r="A36" s="24"/>
       <c r="B36" s="26" t="s">
         <v>69</v>
@@ -3448,7 +3504,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="13.5" customHeight="1">
       <c r="A37" s="24"/>
       <c r="B37" s="26" t="s">
         <v>70</v>
@@ -3463,7 +3519,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="13.5" customHeight="1">
       <c r="A38" s="24"/>
       <c r="B38" s="26" t="s">
         <v>71</v>
@@ -3478,7 +3534,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="13.5" customHeight="1">
       <c r="A39" s="24"/>
       <c r="B39" s="26" t="s">
         <v>72</v>
@@ -3493,16 +3549,16 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="13.5" customHeight="1">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="13.5" customHeight="1">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="13.5" customHeight="1">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="13.5" customHeight="1">
       <c r="A43" s="25" t="s">
         <v>73</v>
       </c>
@@ -3511,7 +3567,7 @@
       <c r="D43" s="24"/>
       <c r="E43" s="24"/>
     </row>
-    <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="13.5" customHeight="1">
       <c r="A44" s="24"/>
       <c r="B44" s="24"/>
       <c r="C44" s="27" t="s">
@@ -3524,7 +3580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="13.5" customHeight="1">
       <c r="A45" s="24"/>
       <c r="B45" s="26" t="s">
         <v>58</v>
@@ -3539,7 +3595,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="13.5" customHeight="1">
       <c r="A46" s="24"/>
       <c r="B46" s="26" t="s">
         <v>59</v>
@@ -3554,7 +3610,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="13.5" customHeight="1">
       <c r="A47" s="24"/>
       <c r="B47" s="26" t="s">
         <v>74</v>
@@ -3569,7 +3625,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="13.5" customHeight="1">
       <c r="A48" s="24"/>
       <c r="B48" s="26" t="s">
         <v>61</v>
@@ -3584,7 +3640,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="13.5" customHeight="1">
       <c r="A49" s="24"/>
       <c r="B49" s="26" t="s">
         <v>62</v>
@@ -3599,7 +3655,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="13.5" customHeight="1">
       <c r="A50" s="24"/>
       <c r="B50" s="26" t="s">
         <v>63</v>
@@ -3614,7 +3670,7 @@
         <v>0.432</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="13.5" customHeight="1">
       <c r="A51" s="24"/>
       <c r="B51" s="26" t="s">
         <v>75</v>
@@ -3629,7 +3685,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="13.5" customHeight="1">
       <c r="A52" s="24"/>
       <c r="B52" s="26" t="s">
         <v>76</v>
@@ -3644,16 +3700,16 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="13.5" customHeight="1">
       <c r="B53" s="3"/>
     </row>
-    <row r="54" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="13.5" customHeight="1">
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="13.5" customHeight="1">
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="13.5" customHeight="1">
       <c r="A56" s="25" t="s">
         <v>100</v>
       </c>
@@ -3662,7 +3718,7 @@
       <c r="D56" s="24"/>
       <c r="E56" s="24"/>
     </row>
-    <row r="57" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="13.5" customHeight="1">
       <c r="A57" s="24"/>
       <c r="B57" s="24"/>
       <c r="C57" s="27" t="s">
@@ -3675,7 +3731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="13.5" customHeight="1">
       <c r="A58" s="24"/>
       <c r="B58" s="26" t="s">
         <v>77</v>
@@ -3693,7 +3749,7 @@
       <c r="H58" s="23"/>
       <c r="I58" s="23"/>
     </row>
-    <row r="59" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="13.5" customHeight="1">
       <c r="A59" s="24"/>
       <c r="B59" s="26" t="s">
         <v>78</v>
@@ -3711,7 +3767,7 @@
       <c r="H59" s="23"/>
       <c r="I59" s="23"/>
     </row>
-    <row r="60" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="13.5" customHeight="1">
       <c r="A60" s="24"/>
       <c r="B60" s="26" t="s">
         <v>79</v>
@@ -3729,7 +3785,7 @@
       <c r="H60" s="23"/>
       <c r="I60" s="23"/>
     </row>
-    <row r="61" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="13.5" customHeight="1">
       <c r="A61" s="24"/>
       <c r="B61" s="26" t="s">
         <v>94</v>
@@ -3747,7 +3803,7 @@
       <c r="H61" s="23"/>
       <c r="I61" s="23"/>
     </row>
-    <row r="62" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="13.5" customHeight="1">
       <c r="A62" s="24"/>
       <c r="B62" s="26" t="s">
         <v>80</v>
@@ -3765,7 +3821,7 @@
       <c r="H62" s="23"/>
       <c r="I62" s="23"/>
     </row>
-    <row r="63" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="13.5" customHeight="1">
       <c r="A63" s="24"/>
       <c r="B63" s="26" t="s">
         <v>81</v>
@@ -3783,7 +3839,7 @@
       <c r="H63" s="23"/>
       <c r="I63" s="23"/>
     </row>
-    <row r="64" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="13.5" customHeight="1">
       <c r="A64" s="24"/>
       <c r="B64" s="26" t="s">
         <v>82</v>
@@ -3801,7 +3857,7 @@
       <c r="H64" s="23"/>
       <c r="I64" s="23"/>
     </row>
-    <row r="65" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="13.5" customHeight="1">
       <c r="A65" s="24"/>
       <c r="B65" s="26" t="s">
         <v>97</v>
@@ -3819,7 +3875,7 @@
       <c r="H65" s="23"/>
       <c r="I65" s="23"/>
     </row>
-    <row r="66" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="13.5" customHeight="1">
       <c r="A66" s="24"/>
       <c r="B66" s="26" t="s">
         <v>98</v>
@@ -3834,12 +3890,12 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="13.5" customHeight="1">
       <c r="B67" s="3"/>
     </row>
-    <row r="68" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="13.5" customHeight="1"/>
+    <row r="69" spans="1:9" ht="13.5" customHeight="1"/>
+    <row r="70" spans="1:9" ht="13.5" customHeight="1">
       <c r="A70" s="25" t="s">
         <v>83</v>
       </c>
@@ -3848,7 +3904,7 @@
       <c r="D70" s="24"/>
       <c r="E70" s="24"/>
     </row>
-    <row r="71" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="13.5" customHeight="1">
       <c r="A71" s="24"/>
       <c r="B71" s="24"/>
       <c r="C71" s="27" t="s">
@@ -3861,7 +3917,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="13.5" customHeight="1">
       <c r="A72" s="24"/>
       <c r="B72" s="26" t="s">
         <v>84</v>
@@ -3876,7 +3932,7 @@
         <v>0.20499999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="13.5" customHeight="1">
       <c r="A73" s="24"/>
       <c r="B73" s="26" t="s">
         <v>85</v>
@@ -3891,7 +3947,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="13.5" customHeight="1">
       <c r="A74" s="24"/>
       <c r="B74" s="26" t="s">
         <v>86</v>
@@ -3906,7 +3962,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="13.5" customHeight="1">
       <c r="A75" s="24"/>
       <c r="B75" s="26" t="s">
         <v>87</v>
@@ -3921,7 +3977,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="13.5" customHeight="1">
       <c r="A76" s="24"/>
       <c r="B76" s="26" t="s">
         <v>88</v>
@@ -3936,7 +3992,7 @@
         <v>0.47399999999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="15" customHeight="1">
       <c r="A77" s="24"/>
       <c r="B77" s="26" t="s">
         <v>89</v>
@@ -3951,7 +4007,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="15" customHeight="1">
       <c r="A78" s="24"/>
       <c r="B78" s="26" t="s">
         <v>90</v>
@@ -3985,16 +4041,16 @@
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
-    <col min="5" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="1" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="5" max="6" width="8.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -4002,7 +4058,7 @@
       <c r="D1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="13.5" customHeight="1">
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4028,7 +4084,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="13.5" customHeight="1">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -4057,7 +4113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="13.5" customHeight="1">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -4086,47 +4142,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="13.5" customHeight="1">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="13.5" customHeight="1">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="13.5" customHeight="1">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="13.5" customHeight="1">
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="13.5" customHeight="1">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="13.5" customHeight="1">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="13.5" customHeight="1">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="13.5" customHeight="1">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="13.5" customHeight="1">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="G13" s="3"/>
@@ -4149,17 +4205,17 @@
       <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="26" width="8.85546875" customWidth="1"/>
+    <col min="1" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="13.5" customHeight="1">
       <c r="D2" s="5">
         <v>2000</v>
       </c>
@@ -4227,7 +4283,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4261,7 +4317,7 @@
       </c>
       <c r="Z3" s="12"/>
     </row>
-    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4303,7 +4359,7 @@
       </c>
       <c r="Z4" s="12"/>
     </row>
-    <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="13.5" customHeight="1">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4337,8 +4393,8 @@
       </c>
       <c r="Z5" s="12"/>
     </row>
-    <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:26" ht="13.5" customHeight="1">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4372,7 +4428,7 @@
       </c>
       <c r="Z7" s="12"/>
     </row>
-    <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="13.5" customHeight="1">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4414,7 +4470,7 @@
       </c>
       <c r="Z8" s="12"/>
     </row>
-    <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="13.5" customHeight="1">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4448,7 +4504,7 @@
       </c>
       <c r="Z9" s="12"/>
     </row>
-    <row r="10" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:26" ht="13.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4468,17 +4524,17 @@
       <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="26" width="8.85546875" customWidth="1"/>
+    <col min="1" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="13.5" customHeight="1">
       <c r="D2" s="7">
         <v>2000</v>
       </c>
@@ -4546,7 +4602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4580,7 +4636,7 @@
       </c>
       <c r="Z3" s="10"/>
     </row>
-    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4620,7 +4676,7 @@
       </c>
       <c r="Z4" s="14"/>
     </row>
-    <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="13.5" customHeight="1">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4654,8 +4710,8 @@
       </c>
       <c r="Z5" s="10"/>
     </row>
-    <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:26" ht="13.5" customHeight="1">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4689,7 +4745,7 @@
       </c>
       <c r="Z7" s="10"/>
     </row>
-    <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="13.5" customHeight="1">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4729,7 +4785,7 @@
       </c>
       <c r="Z8" s="10"/>
     </row>
-    <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="13.5" customHeight="1">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4783,17 +4839,17 @@
       <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="25" width="8.85546875" customWidth="1"/>
+    <col min="1" max="25" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -4861,7 +4917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4896,7 +4952,7 @@
       </c>
       <c r="Y3" s="10"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4931,15 +4987,15 @@
       </c>
       <c r="Y4" s="10"/>
     </row>
-    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="8" spans="1:25" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -5007,7 +5063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5040,7 +5096,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5073,15 +5129,15 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="13" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="14" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="15" spans="1:25" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -5149,7 +5205,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:25" ht="13.5" customHeight="1">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5182,7 +5238,7 @@
       </c>
       <c r="Y17" s="10"/>
     </row>
-    <row r="18" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:25" ht="13.5" customHeight="1">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5229,23 +5285,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y39"/>
+  <dimension ref="A1:Y54"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="25" width="8.85546875" customWidth="1"/>
+    <col min="1" max="25" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -5313,7 +5369,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -5343,15 +5399,15 @@
       </c>
       <c r="Y3" s="9"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="5" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="13.5" customHeight="1">
       <c r="C8" s="5">
         <v>2000</v>
       </c>
@@ -5419,7 +5475,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
@@ -5449,15 +5505,15 @@
       </c>
       <c r="Y9" s="9"/>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="11" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="12" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="13" spans="1:25" ht="13.5" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="13.5" customHeight="1">
       <c r="C14" s="5">
         <v>2000</v>
       </c>
@@ -5525,7 +5581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="13.5" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
@@ -5555,15 +5611,15 @@
       </c>
       <c r="Y15" s="9"/>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="17" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="18" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="19" spans="1:25" ht="13.5" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="13.5" customHeight="1">
       <c r="C20" s="5">
         <v>2000</v>
       </c>
@@ -5631,7 +5687,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="13.5" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
@@ -5661,15 +5717,15 @@
       </c>
       <c r="Y21" s="9"/>
     </row>
-    <row r="22" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="23" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="24" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="25" spans="1:25" ht="13.5" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="13.5" customHeight="1">
       <c r="C26" s="7">
         <v>2000</v>
       </c>
@@ -5737,7 +5793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="13.5" customHeight="1">
       <c r="B27" s="7" t="s">
         <v>14</v>
       </c>
@@ -5767,15 +5823,15 @@
       </c>
       <c r="Y27" s="9"/>
     </row>
-    <row r="28" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="29" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="30" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="C32" s="5">
         <v>2000</v>
       </c>
@@ -5843,7 +5899,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" ht="13.5" customHeight="1">
       <c r="B33" s="5" t="s">
         <v>14</v>
       </c>
@@ -5873,15 +5929,15 @@
       </c>
       <c r="Y33" s="9"/>
     </row>
-    <row r="34" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="35" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="36" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="37" spans="1:25" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="13.5" customHeight="1">
       <c r="C38" s="5">
         <v>2000</v>
       </c>
@@ -5949,7 +6005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="13.5" customHeight="1">
       <c r="B39" s="5" t="s">
         <v>14</v>
       </c>
@@ -5979,8 +6035,277 @@
       </c>
       <c r="Y39" s="9"/>
     </row>
+    <row r="43" spans="1:25" ht="14">
+      <c r="A43" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="31"/>
+      <c r="M43" s="31"/>
+      <c r="N43" s="31"/>
+      <c r="O43" s="31"/>
+      <c r="P43" s="31"/>
+      <c r="Q43" s="31"/>
+      <c r="R43" s="31"/>
+      <c r="S43" s="31"/>
+      <c r="T43" s="31"/>
+      <c r="U43" s="31"/>
+      <c r="V43" s="31"/>
+      <c r="W43" s="31"/>
+      <c r="X43" s="31"/>
+      <c r="Y43" s="31"/>
+    </row>
+    <row r="44" spans="1:25" ht="14">
+      <c r="A44" s="31"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D44" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E44" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F44" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G44" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H44" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I44" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J44" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K44" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L44" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M44" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N44" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O44" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P44" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q44" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R44" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S44" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T44" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U44" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V44" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W44" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X44" s="31"/>
+      <c r="Y44" s="35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" ht="14">
+      <c r="A45" s="31"/>
+      <c r="B45" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="37"/>
+      <c r="M45" s="37"/>
+      <c r="N45" s="37"/>
+      <c r="O45" s="37"/>
+      <c r="P45" s="37"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="37"/>
+      <c r="S45" s="37"/>
+      <c r="T45" s="37"/>
+      <c r="U45" s="37"/>
+      <c r="V45" s="37"/>
+      <c r="W45" s="37"/>
+      <c r="X45" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y45" s="37"/>
+    </row>
+    <row r="46" spans="1:25" ht="12"/>
+    <row r="47" spans="1:25" ht="12"/>
+    <row r="48" spans="1:25" ht="12"/>
+    <row r="49" spans="1:25" ht="14">
+      <c r="A49" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="31"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="31"/>
+      <c r="O49" s="31"/>
+      <c r="P49" s="31"/>
+      <c r="Q49" s="31"/>
+      <c r="R49" s="31"/>
+      <c r="S49" s="31"/>
+      <c r="T49" s="31"/>
+      <c r="U49" s="31"/>
+      <c r="V49" s="31"/>
+      <c r="W49" s="31"/>
+      <c r="X49" s="31"/>
+      <c r="Y49" s="31"/>
+    </row>
+    <row r="50" spans="1:25" ht="14">
+      <c r="A50" s="31"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D50" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E50" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F50" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G50" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H50" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I50" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J50" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K50" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L50" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M50" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N50" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O50" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P50" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q50" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R50" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S50" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T50" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U50" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V50" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W50" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X50" s="31"/>
+      <c r="Y50" s="35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" ht="14">
+      <c r="A51" s="31"/>
+      <c r="B51" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="37"/>
+      <c r="N51" s="37"/>
+      <c r="O51" s="37"/>
+      <c r="P51" s="37"/>
+      <c r="Q51" s="37"/>
+      <c r="R51" s="37"/>
+      <c r="S51" s="37"/>
+      <c r="T51" s="37"/>
+      <c r="U51" s="37"/>
+      <c r="V51" s="37"/>
+      <c r="W51" s="37"/>
+      <c r="X51" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y51" s="37"/>
+    </row>
+    <row r="52" spans="1:25" ht="12"/>
+    <row r="53" spans="1:25" ht="12"/>
+    <row r="54" spans="1:25" ht="12"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5997,17 +6322,17 @@
       <selection activeCell="AA31" sqref="AA31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="25" width="8.85546875" customWidth="1"/>
+    <col min="1" max="25" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -6075,7 +6400,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -6108,7 +6433,7 @@
       </c>
       <c r="Y3" s="15"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -6141,15 +6466,15 @@
       </c>
       <c r="Y4" s="15"/>
     </row>
-    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="8" spans="1:25" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -6217,7 +6542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1">
       <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
@@ -6249,15 +6574,15 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="12" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="13" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="14" spans="1:25" ht="13.5" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="13.5" customHeight="1">
       <c r="C15" s="5">
         <v>2000</v>
       </c>
@@ -6325,7 +6650,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
@@ -6365,15 +6690,15 @@
       </c>
       <c r="Y16" s="6"/>
     </row>
-    <row r="17" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="18" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="19" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="20" spans="1:25" ht="13.5" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="13.5" customHeight="1">
       <c r="C21" s="5">
         <v>2000</v>
       </c>
@@ -6441,7 +6766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="13.5" customHeight="1">
       <c r="B22" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -6474,7 +6799,7 @@
       </c>
       <c r="Y22" s="15"/>
     </row>
-    <row r="23" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="13.5" customHeight="1">
       <c r="B23" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -6507,15 +6832,15 @@
       </c>
       <c r="Y23" s="15"/>
     </row>
-    <row r="24" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="25" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="26" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="27" spans="1:25" ht="13.5" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" ht="13.5" customHeight="1">
       <c r="C28" s="5">
         <v>2000</v>
       </c>
@@ -6583,7 +6908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="B29" s="5" t="s">
         <v>14</v>
       </c>
@@ -6623,15 +6948,15 @@
       </c>
       <c r="Y29" s="6"/>
     </row>
-    <row r="30" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="31" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="32" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="33" spans="1:25" ht="13.5" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" ht="13.5" customHeight="1">
       <c r="C34" s="5">
         <v>2000</v>
       </c>
@@ -6699,7 +7024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" ht="13.5" customHeight="1">
       <c r="B35" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -6756,15 +7081,15 @@
       </c>
       <c r="Y35" s="9"/>
     </row>
-    <row r="36" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="37" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="38" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="39" spans="1:25" ht="13.5" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" ht="13.5" customHeight="1">
       <c r="C40" s="5">
         <v>2000</v>
       </c>
@@ -6832,7 +7157,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" ht="13.5" customHeight="1">
       <c r="B41" s="5" t="s">
         <v>14</v>
       </c>
@@ -6879,15 +7204,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y67"/>
+  <dimension ref="A1:Y61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="14">
       <c r="A1" s="34" t="s">
         <v>106</v>
       </c>
@@ -6916,7 +7241,7 @@
       <c r="X1" s="31"/>
       <c r="Y1" s="31"/>
     </row>
-    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="14">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="35">
@@ -6987,7 +7312,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="14">
       <c r="A3" s="31"/>
       <c r="B3" s="32" t="s">
         <v>95</v>
@@ -7020,7 +7345,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="14">
       <c r="A4" s="31"/>
       <c r="B4" s="32" t="s">
         <v>96</v>
@@ -7053,7 +7378,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="14">
       <c r="A8" s="34" t="s">
         <v>101</v>
       </c>
@@ -7082,7 +7407,7 @@
       <c r="X8" s="31"/>
       <c r="Y8" s="31"/>
     </row>
-    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="14">
       <c r="A9" s="31"/>
       <c r="B9" s="31"/>
       <c r="C9" s="35">
@@ -7153,7 +7478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="14">
       <c r="A10" s="31"/>
       <c r="B10" s="32" t="s">
         <v>95</v>
@@ -7186,7 +7511,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="14">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
         <v>96</v>
@@ -7219,7 +7544,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="14">
       <c r="A15" s="34" t="s">
         <v>107</v>
       </c>
@@ -7248,7 +7573,7 @@
       <c r="X15" s="31"/>
       <c r="Y15" s="31"/>
     </row>
-    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="14">
       <c r="A16" s="31"/>
       <c r="B16" s="31"/>
       <c r="C16" s="35">
@@ -7319,7 +7644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="14">
       <c r="A17" s="31"/>
       <c r="B17" s="32" t="s">
         <v>95</v>
@@ -7352,7 +7677,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="14">
       <c r="A18" s="31"/>
       <c r="B18" s="32" t="s">
         <v>96</v>
@@ -7385,7 +7710,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="14">
       <c r="A22" s="34" t="s">
         <v>108</v>
       </c>
@@ -7414,7 +7739,7 @@
       <c r="X22" s="31"/>
       <c r="Y22" s="31"/>
     </row>
-    <row r="23" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="14">
       <c r="A23" s="31"/>
       <c r="B23" s="31"/>
       <c r="C23" s="35">
@@ -7485,7 +7810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="14">
       <c r="A24" s="31"/>
       <c r="B24" s="32" t="s">
         <v>95</v>
@@ -7518,7 +7843,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="14">
       <c r="A25" s="31"/>
       <c r="B25" s="32" t="s">
         <v>96</v>
@@ -7551,7 +7876,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="14">
       <c r="A29" s="34" t="s">
         <v>113</v>
       </c>
@@ -7580,7 +7905,7 @@
       <c r="X29" s="31"/>
       <c r="Y29" s="31"/>
     </row>
-    <row r="30" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="14">
       <c r="A30" s="31"/>
       <c r="B30" s="31"/>
       <c r="C30" s="35">
@@ -7651,7 +7976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="14">
       <c r="A31" s="31"/>
       <c r="B31" s="35" t="s">
         <v>30</v>
@@ -7684,7 +8009,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" ht="14">
       <c r="A35" s="34" t="s">
         <v>102</v>
       </c>
@@ -7713,7 +8038,7 @@
       <c r="X35" s="31"/>
       <c r="Y35" s="31"/>
     </row>
-    <row r="36" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" ht="14">
       <c r="A36" s="31"/>
       <c r="B36" s="31"/>
       <c r="C36" s="35">
@@ -7784,7 +8109,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" ht="14">
       <c r="A37" s="31"/>
       <c r="B37" s="35" t="s">
         <v>30</v>
@@ -7817,7 +8142,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" ht="14">
       <c r="A41" s="34" t="s">
         <v>114</v>
       </c>
@@ -7846,7 +8171,7 @@
       <c r="X41" s="31"/>
       <c r="Y41" s="31"/>
     </row>
-    <row r="42" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" ht="14">
       <c r="A42" s="31"/>
       <c r="B42" s="31"/>
       <c r="C42" s="35">
@@ -7917,7 +8242,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" ht="14">
       <c r="A43" s="31"/>
       <c r="B43" s="35" t="s">
         <v>30</v>
@@ -7950,7 +8275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" ht="14">
       <c r="A47" s="34" t="s">
         <v>115</v>
       </c>
@@ -7979,7 +8304,7 @@
       <c r="X47" s="31"/>
       <c r="Y47" s="31"/>
     </row>
-    <row r="48" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" ht="14">
       <c r="A48" s="31"/>
       <c r="B48" s="31"/>
       <c r="C48" s="35">
@@ -8050,7 +8375,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" ht="14">
       <c r="A49" s="31"/>
       <c r="B49" s="35" t="s">
         <v>30</v>
@@ -8083,9 +8408,9 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" ht="14">
       <c r="A53" s="34" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B53" s="31"/>
       <c r="C53" s="31"/>
@@ -8112,7 +8437,7 @@
       <c r="X53" s="31"/>
       <c r="Y53" s="31"/>
     </row>
-    <row r="54" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" ht="14">
       <c r="A54" s="31"/>
       <c r="B54" s="31"/>
       <c r="C54" s="35">
@@ -8183,7 +8508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" ht="14">
       <c r="A55" s="31"/>
       <c r="B55" s="35" t="s">
         <v>30</v>
@@ -8216,9 +8541,9 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="59" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" ht="14">
       <c r="A59" s="34" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B59" s="31"/>
       <c r="C59" s="31"/>
@@ -8245,7 +8570,7 @@
       <c r="X59" s="31"/>
       <c r="Y59" s="31"/>
     </row>
-    <row r="60" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" ht="14">
       <c r="A60" s="31"/>
       <c r="B60" s="31"/>
       <c r="C60" s="35">
@@ -8316,7 +8641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" ht="14">
       <c r="A61" s="31"/>
       <c r="B61" s="35" t="s">
         <v>30</v>
@@ -8349,141 +8674,14 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="B65" s="31"/>
-      <c r="C65" s="31"/>
-      <c r="D65" s="31"/>
-      <c r="E65" s="31"/>
-      <c r="F65" s="31"/>
-      <c r="G65" s="31"/>
-      <c r="H65" s="31"/>
-      <c r="I65" s="31"/>
-      <c r="J65" s="31"/>
-      <c r="K65" s="31"/>
-      <c r="L65" s="31"/>
-      <c r="M65" s="31"/>
-      <c r="N65" s="31"/>
-      <c r="O65" s="31"/>
-      <c r="P65" s="31"/>
-      <c r="Q65" s="31"/>
-      <c r="R65" s="31"/>
-      <c r="S65" s="31"/>
-      <c r="T65" s="31"/>
-      <c r="U65" s="31"/>
-      <c r="V65" s="31"/>
-      <c r="W65" s="31"/>
-      <c r="X65" s="31"/>
-      <c r="Y65" s="31"/>
-    </row>
-    <row r="66" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="31"/>
-      <c r="B66" s="31"/>
-      <c r="C66" s="35">
-        <v>2000</v>
-      </c>
-      <c r="D66" s="35">
-        <v>2001</v>
-      </c>
-      <c r="E66" s="35">
-        <v>2002</v>
-      </c>
-      <c r="F66" s="35">
-        <v>2003</v>
-      </c>
-      <c r="G66" s="35">
-        <v>2004</v>
-      </c>
-      <c r="H66" s="35">
-        <v>2005</v>
-      </c>
-      <c r="I66" s="35">
-        <v>2006</v>
-      </c>
-      <c r="J66" s="35">
-        <v>2007</v>
-      </c>
-      <c r="K66" s="35">
-        <v>2008</v>
-      </c>
-      <c r="L66" s="35">
-        <v>2009</v>
-      </c>
-      <c r="M66" s="35">
-        <v>2010</v>
-      </c>
-      <c r="N66" s="35">
-        <v>2011</v>
-      </c>
-      <c r="O66" s="35">
-        <v>2012</v>
-      </c>
-      <c r="P66" s="35">
-        <v>2013</v>
-      </c>
-      <c r="Q66" s="35">
-        <v>2014</v>
-      </c>
-      <c r="R66" s="35">
-        <v>2015</v>
-      </c>
-      <c r="S66" s="35">
-        <v>2016</v>
-      </c>
-      <c r="T66" s="35">
-        <v>2017</v>
-      </c>
-      <c r="U66" s="35">
-        <v>2018</v>
-      </c>
-      <c r="V66" s="35">
-        <v>2019</v>
-      </c>
-      <c r="W66" s="35">
-        <v>2020</v>
-      </c>
-      <c r="X66" s="31"/>
-      <c r="Y66" s="35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="67" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="31"/>
-      <c r="B67" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="C67" s="37"/>
-      <c r="D67" s="37"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="37"/>
-      <c r="G67" s="37"/>
-      <c r="H67" s="37"/>
-      <c r="I67" s="37"/>
-      <c r="J67" s="37"/>
-      <c r="K67" s="37"/>
-      <c r="L67" s="37"/>
-      <c r="M67" s="37"/>
-      <c r="N67" s="37"/>
-      <c r="O67" s="37"/>
-      <c r="P67" s="37"/>
-      <c r="Q67" s="37"/>
-      <c r="R67" s="37"/>
-      <c r="S67" s="37"/>
-      <c r="T67" s="37"/>
-      <c r="U67" s="37"/>
-      <c r="V67" s="37"/>
-      <c r="W67" s="37"/>
-      <c r="X67" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y67" s="37">
-        <v>0.85</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8495,17 +8693,17 @@
       <selection activeCell="AA53" sqref="AA53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="25" width="8.85546875" customWidth="1"/>
+    <col min="1" max="25" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -8573,7 +8771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -8606,7 +8804,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -8639,15 +8837,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="8" spans="1:25" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -8715,7 +8913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -8749,7 +8947,7 @@
         <v>12.000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -8783,15 +8981,15 @@
         <v>6.0000000000000009</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="13" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="14" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="15" spans="1:25" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -8859,7 +9057,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="13.5" customHeight="1">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -8892,7 +9090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="13.5" customHeight="1">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -8925,15 +9123,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="20" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="21" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="22" spans="1:25" ht="13.5" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="13.5" customHeight="1">
       <c r="C23" s="5">
         <v>2000</v>
       </c>
@@ -9001,7 +9199,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="13.5" customHeight="1">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9034,7 +9232,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="13.5" customHeight="1">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9067,15 +9265,15 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="27" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="28" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="13.5" customHeight="1">
       <c r="C30" s="5">
         <v>2000</v>
       </c>
@@ -9143,7 +9341,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="B31" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9176,7 +9374,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="B32" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9209,15 +9407,15 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="34" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="35" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="36" spans="1:25" ht="13.5" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" ht="13.5" customHeight="1">
       <c r="C37" s="5">
         <v>2000</v>
       </c>
@@ -9285,7 +9483,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="13.5" customHeight="1">
       <c r="B38" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9318,7 +9516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="13.5" customHeight="1">
       <c r="B39" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9351,15 +9549,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="41" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="42" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="43" spans="1:25" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" ht="13.5" customHeight="1">
       <c r="C44" s="5">
         <v>2000</v>
       </c>
@@ -9427,7 +9625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" ht="13.5" customHeight="1">
       <c r="B45" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>

</xml_diff>

<commit_message>
switched order, added propcare param
</commit_message>
<xml_diff>
--- a/tests/simple.xlsx
+++ b/tests/simple.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="861" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14715" tabRatio="861" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -12,15 +12,15 @@
     <sheet name="Population size" sheetId="4" r:id="rId3"/>
     <sheet name="HIV prevalence" sheetId="15" r:id="rId4"/>
     <sheet name="Other epidemiology" sheetId="6" r:id="rId5"/>
-    <sheet name="Optional indicators" sheetId="5" r:id="rId6"/>
-    <sheet name="Testing &amp; treatment" sheetId="7" r:id="rId7"/>
+    <sheet name="Testing &amp; treatment" sheetId="7" r:id="rId6"/>
+    <sheet name="Optional indicators" sheetId="5" r:id="rId7"/>
     <sheet name="Cascade" sheetId="18" r:id="rId8"/>
     <sheet name="Sexual behavior" sheetId="8" r:id="rId9"/>
     <sheet name="Injecting behavior" sheetId="9" r:id="rId10"/>
     <sheet name="Partnerships &amp; transitions" sheetId="10" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="121">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -495,46 +495,10 @@
     <t>Proportion of people on ART with viral suppression (%)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">Diagnosed </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">PLHIV </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">on treatment </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>(%)</t>
-    </r>
+    <t>Diagnosed PLHIV in care (%)</t>
+  </si>
+  <si>
+    <t>PLHIV in care on treatment (%)</t>
   </si>
 </sst>
 </file>
@@ -542,8 +506,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
@@ -762,9 +726,9 @@
   <cellStyleXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -956,13 +920,13 @@
     <xf numFmtId="165" fontId="16" fillId="10" borderId="2" xfId="113" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="113" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="113" applyFont="1"/>
   </cellXfs>
   <cellStyles count="118">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2340,34 +2304,34 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="89.6640625" customWidth="1"/>
+    <col min="1" max="1" width="89.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="12.75" customHeight="1">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="41"/>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="41"/>
-    </row>
-    <row r="4" spans="1:1" ht="14">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="42"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="42"/>
+    </row>
+    <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:1" ht="67.5" customHeight="1">
+    <row r="5" spans="1:1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="14">
+    <row r="6" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:1" ht="14">
+    <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>92</v>
       </c>
@@ -2393,17 +2357,17 @@
       <selection activeCell="X1" sqref="X1:AG1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="25" width="8.83203125" customWidth="1"/>
+    <col min="1" max="25" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -2471,7 +2435,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2504,7 +2468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2537,15 +2501,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="6" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1">
+    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -2613,7 +2577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2646,7 +2610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2679,15 +2643,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1">
+    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -2755,7 +2719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:25" ht="13.5" customHeight="1">
+    <row r="17" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
         <v>14</v>
       </c>
@@ -2787,9 +2751,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:25" ht="13.5" customHeight="1"/>
-    <row r="19" spans="2:25" ht="13.5" customHeight="1"/>
-    <row r="20" spans="2:25" ht="13.5" customHeight="1"/>
+    <row r="18" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2808,21 +2772,21 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="6" width="8.83203125" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="6" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.5" customHeight="1">
+    <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" ht="13.5" customHeight="1">
+    <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2832,7 +2796,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.5" customHeight="1">
+    <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2842,7 +2806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.5" customHeight="1">
+    <row r="4" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2850,26 +2814,26 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="13.5" customHeight="1">
+    <row r="5" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="13.5" customHeight="1">
+    <row r="6" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="13.5" customHeight="1">
+    <row r="7" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="13.5" customHeight="1">
+    <row r="8" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="13.5" customHeight="1">
+    <row r="9" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2879,7 +2843,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13.5" customHeight="1">
+    <row r="10" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2889,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.5" customHeight="1">
+    <row r="11" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2897,26 +2861,26 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" ht="13.5" customHeight="1">
+    <row r="12" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" ht="13.5" customHeight="1">
+    <row r="13" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="13.5" customHeight="1">
+    <row r="14" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="13.5" customHeight="1">
+    <row r="15" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1">
+    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2926,7 +2890,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="13.5" customHeight="1">
+    <row r="17" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2934,7 +2898,7 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" ht="13.5" customHeight="1">
+    <row r="18" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2942,26 +2906,26 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" ht="13.5" customHeight="1">
+    <row r="19" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="13.5" customHeight="1">
+    <row r="20" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="13.5" customHeight="1">
+    <row r="21" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="13.5" customHeight="1">
+    <row r="22" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" ht="13.5" customHeight="1">
+    <row r="23" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2971,7 +2935,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="13.5" customHeight="1">
+    <row r="24" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2979,7 +2943,7 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" ht="13.5" customHeight="1">
+    <row r="25" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2987,14 +2951,14 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="13.5" customHeight="1">
+    <row r="29" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="13.5" customHeight="1">
+    <row r="30" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3004,7 +2968,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="13.5" customHeight="1">
+    <row r="31" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3012,14 +2976,14 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="35" spans="1:4" ht="13.5" customHeight="1">
+    <row r="35" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>112</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" ht="13.5" customHeight="1">
+    <row r="36" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3029,7 +2993,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="13.5" customHeight="1">
+    <row r="37" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3037,7 +3001,7 @@
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" ht="13.5" customHeight="1">
+    <row r="38" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3045,14 +3009,14 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="42" spans="1:4" ht="13.5" customHeight="1">
+    <row r="42" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" ht="13.5" customHeight="1">
+    <row r="43" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3062,7 +3026,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="13.5" customHeight="1">
+    <row r="44" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3070,7 +3034,7 @@
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" ht="13.5" customHeight="1">
+    <row r="45" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3097,14 +3061,14 @@
       <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="6" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="6" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1">
+    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>49</v>
       </c>
@@ -3113,7 +3077,7 @@
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1">
+    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="27" t="s">
@@ -3126,7 +3090,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1">
+    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="26" t="s">
         <v>50</v>
@@ -3141,7 +3105,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1">
+    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
       <c r="B4" s="26" t="s">
         <v>51</v>
@@ -3156,7 +3120,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1">
+    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="26" t="s">
         <v>52</v>
@@ -3171,7 +3135,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1">
+    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="26" t="s">
         <v>53</v>
@@ -3186,7 +3150,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1">
+    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="26" t="s">
         <v>54</v>
@@ -3201,7 +3165,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1">
+    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="26" t="s">
         <v>55</v>
@@ -3216,7 +3180,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1">
+    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="26" t="s">
         <v>56</v>
@@ -3231,16 +3195,16 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1">
+    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="13.5" customHeight="1">
+    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="13.5" customHeight="1">
+    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="13.5" customHeight="1">
+    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>57</v>
       </c>
@@ -3249,7 +3213,7 @@
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1">
+    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="24"/>
       <c r="C14" s="27" t="s">
@@ -3262,7 +3226,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1">
+    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="26" t="s">
         <v>58</v>
@@ -3277,7 +3241,7 @@
         <v>48.02</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="13.5" customHeight="1">
+    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="26" t="s">
         <v>59</v>
@@ -3292,7 +3256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="13.5" customHeight="1">
+    <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="26" t="s">
         <v>60</v>
@@ -3307,7 +3271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="13.5" customHeight="1">
+    <row r="18" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="26" t="s">
         <v>61</v>
@@ -3322,7 +3286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="13.5" customHeight="1">
+    <row r="19" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
       <c r="B19" s="26" t="s">
         <v>62</v>
@@ -3337,7 +3301,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="13.5" customHeight="1">
+    <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="26" t="s">
         <v>63</v>
@@ -3352,16 +3316,16 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="13.5" customHeight="1">
+    <row r="21" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="13.5" customHeight="1">
+    <row r="22" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="13.5" customHeight="1">
+    <row r="23" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="13.5" customHeight="1">
+    <row r="24" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>64</v>
       </c>
@@ -3370,7 +3334,7 @@
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
     </row>
-    <row r="25" spans="1:5" ht="13.5" customHeight="1">
+    <row r="25" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
       <c r="B25" s="24"/>
       <c r="C25" s="27" t="s">
@@ -3383,7 +3347,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="13.5" customHeight="1">
+    <row r="26" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
       <c r="B26" s="26" t="s">
         <v>65</v>
@@ -3398,7 +3362,7 @@
         <v>9.76</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="13.5" customHeight="1">
+    <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
       <c r="B27" s="26" t="s">
         <v>60</v>
@@ -3413,7 +3377,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="13.5" customHeight="1">
+    <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24"/>
       <c r="B28" s="26" t="s">
         <v>99</v>
@@ -3428,7 +3392,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="13.5" customHeight="1">
+    <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24"/>
       <c r="B29" s="26" t="s">
         <v>66</v>
@@ -3443,7 +3407,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="13.5" customHeight="1">
+    <row r="30" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
       <c r="B30" s="26" t="s">
         <v>67</v>
@@ -3458,16 +3422,16 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="13.5" customHeight="1">
+    <row r="31" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="13.5" customHeight="1">
+    <row r="32" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="13.5" customHeight="1">
+    <row r="33" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="1:5" ht="13.5" customHeight="1">
+    <row r="34" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>68</v>
       </c>
@@ -3476,7 +3440,7 @@
       <c r="D34" s="24"/>
       <c r="E34" s="24"/>
     </row>
-    <row r="35" spans="1:5" ht="13.5" customHeight="1">
+    <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="24"/>
       <c r="B35" s="24"/>
       <c r="C35" s="27" t="s">
@@ -3489,7 +3453,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="13.5" customHeight="1">
+    <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
       <c r="B36" s="26" t="s">
         <v>69</v>
@@ -3504,7 +3468,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="13.5" customHeight="1">
+    <row r="37" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24"/>
       <c r="B37" s="26" t="s">
         <v>70</v>
@@ -3519,7 +3483,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="13.5" customHeight="1">
+    <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="24"/>
       <c r="B38" s="26" t="s">
         <v>71</v>
@@ -3534,7 +3498,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="13.5" customHeight="1">
+    <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24"/>
       <c r="B39" s="26" t="s">
         <v>72</v>
@@ -3549,16 +3513,16 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="13.5" customHeight="1">
+    <row r="40" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="1:5" ht="13.5" customHeight="1">
+    <row r="41" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="1:5" ht="13.5" customHeight="1">
+    <row r="42" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="1:5" ht="13.5" customHeight="1">
+    <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>73</v>
       </c>
@@ -3567,7 +3531,7 @@
       <c r="D43" s="24"/>
       <c r="E43" s="24"/>
     </row>
-    <row r="44" spans="1:5" ht="13.5" customHeight="1">
+    <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="24"/>
       <c r="B44" s="24"/>
       <c r="C44" s="27" t="s">
@@ -3580,7 +3544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="13.5" customHeight="1">
+    <row r="45" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="24"/>
       <c r="B45" s="26" t="s">
         <v>58</v>
@@ -3595,7 +3559,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="13.5" customHeight="1">
+    <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="24"/>
       <c r="B46" s="26" t="s">
         <v>59</v>
@@ -3610,7 +3574,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="13.5" customHeight="1">
+    <row r="47" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="24"/>
       <c r="B47" s="26" t="s">
         <v>74</v>
@@ -3625,7 +3589,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="13.5" customHeight="1">
+    <row r="48" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="24"/>
       <c r="B48" s="26" t="s">
         <v>61</v>
@@ -3640,7 +3604,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="13.5" customHeight="1">
+    <row r="49" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="24"/>
       <c r="B49" s="26" t="s">
         <v>62</v>
@@ -3655,7 +3619,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="13.5" customHeight="1">
+    <row r="50" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="24"/>
       <c r="B50" s="26" t="s">
         <v>63</v>
@@ -3670,7 +3634,7 @@
         <v>0.432</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="13.5" customHeight="1">
+    <row r="51" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="24"/>
       <c r="B51" s="26" t="s">
         <v>75</v>
@@ -3685,7 +3649,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="13.5" customHeight="1">
+    <row r="52" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="24"/>
       <c r="B52" s="26" t="s">
         <v>76</v>
@@ -3700,16 +3664,16 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="13.5" customHeight="1">
+    <row r="53" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="3"/>
     </row>
-    <row r="54" spans="1:9" ht="13.5" customHeight="1">
+    <row r="54" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:9" ht="13.5" customHeight="1">
+    <row r="55" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:9" ht="13.5" customHeight="1">
+    <row r="56" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="25" t="s">
         <v>100</v>
       </c>
@@ -3718,7 +3682,7 @@
       <c r="D56" s="24"/>
       <c r="E56" s="24"/>
     </row>
-    <row r="57" spans="1:9" ht="13.5" customHeight="1">
+    <row r="57" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="24"/>
       <c r="B57" s="24"/>
       <c r="C57" s="27" t="s">
@@ -3731,7 +3695,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="13.5" customHeight="1">
+    <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="24"/>
       <c r="B58" s="26" t="s">
         <v>77</v>
@@ -3749,7 +3713,7 @@
       <c r="H58" s="23"/>
       <c r="I58" s="23"/>
     </row>
-    <row r="59" spans="1:9" ht="13.5" customHeight="1">
+    <row r="59" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="24"/>
       <c r="B59" s="26" t="s">
         <v>78</v>
@@ -3767,7 +3731,7 @@
       <c r="H59" s="23"/>
       <c r="I59" s="23"/>
     </row>
-    <row r="60" spans="1:9" ht="13.5" customHeight="1">
+    <row r="60" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="24"/>
       <c r="B60" s="26" t="s">
         <v>79</v>
@@ -3785,7 +3749,7 @@
       <c r="H60" s="23"/>
       <c r="I60" s="23"/>
     </row>
-    <row r="61" spans="1:9" ht="13.5" customHeight="1">
+    <row r="61" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="24"/>
       <c r="B61" s="26" t="s">
         <v>94</v>
@@ -3803,7 +3767,7 @@
       <c r="H61" s="23"/>
       <c r="I61" s="23"/>
     </row>
-    <row r="62" spans="1:9" ht="13.5" customHeight="1">
+    <row r="62" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="24"/>
       <c r="B62" s="26" t="s">
         <v>80</v>
@@ -3821,7 +3785,7 @@
       <c r="H62" s="23"/>
       <c r="I62" s="23"/>
     </row>
-    <row r="63" spans="1:9" ht="13.5" customHeight="1">
+    <row r="63" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="24"/>
       <c r="B63" s="26" t="s">
         <v>81</v>
@@ -3839,7 +3803,7 @@
       <c r="H63" s="23"/>
       <c r="I63" s="23"/>
     </row>
-    <row r="64" spans="1:9" ht="13.5" customHeight="1">
+    <row r="64" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="24"/>
       <c r="B64" s="26" t="s">
         <v>82</v>
@@ -3857,7 +3821,7 @@
       <c r="H64" s="23"/>
       <c r="I64" s="23"/>
     </row>
-    <row r="65" spans="1:9" ht="13.5" customHeight="1">
+    <row r="65" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="24"/>
       <c r="B65" s="26" t="s">
         <v>97</v>
@@ -3875,7 +3839,7 @@
       <c r="H65" s="23"/>
       <c r="I65" s="23"/>
     </row>
-    <row r="66" spans="1:9" ht="13.5" customHeight="1">
+    <row r="66" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="24"/>
       <c r="B66" s="26" t="s">
         <v>98</v>
@@ -3890,12 +3854,12 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="13.5" customHeight="1">
+    <row r="67" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="3"/>
     </row>
-    <row r="68" spans="1:9" ht="13.5" customHeight="1"/>
-    <row r="69" spans="1:9" ht="13.5" customHeight="1"/>
-    <row r="70" spans="1:9" ht="13.5" customHeight="1">
+    <row r="68" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="25" t="s">
         <v>83</v>
       </c>
@@ -3904,7 +3868,7 @@
       <c r="D70" s="24"/>
       <c r="E70" s="24"/>
     </row>
-    <row r="71" spans="1:9" ht="13.5" customHeight="1">
+    <row r="71" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="24"/>
       <c r="B71" s="24"/>
       <c r="C71" s="27" t="s">
@@ -3917,7 +3881,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="13.5" customHeight="1">
+    <row r="72" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="24"/>
       <c r="B72" s="26" t="s">
         <v>84</v>
@@ -3932,7 +3896,7 @@
         <v>0.20499999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="13.5" customHeight="1">
+    <row r="73" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="24"/>
       <c r="B73" s="26" t="s">
         <v>85</v>
@@ -3947,7 +3911,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="13.5" customHeight="1">
+    <row r="74" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="24"/>
       <c r="B74" s="26" t="s">
         <v>86</v>
@@ -3962,7 +3926,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="13.5" customHeight="1">
+    <row r="75" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="24"/>
       <c r="B75" s="26" t="s">
         <v>87</v>
@@ -3977,7 +3941,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="13.5" customHeight="1">
+    <row r="76" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="24"/>
       <c r="B76" s="26" t="s">
         <v>88</v>
@@ -3992,7 +3956,7 @@
         <v>0.47399999999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15" customHeight="1">
+    <row r="77" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="24"/>
       <c r="B77" s="26" t="s">
         <v>89</v>
@@ -4007,7 +3971,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15" customHeight="1">
+    <row r="78" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="24"/>
       <c r="B78" s="26" t="s">
         <v>90</v>
@@ -4041,16 +4005,16 @@
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.6640625" customWidth="1"/>
-    <col min="5" max="6" width="8.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="5" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" customHeight="1">
+    <row r="1" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -4058,7 +4022,7 @@
       <c r="D1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="13.5" customHeight="1">
+    <row r="2" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4084,7 +4048,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.5" customHeight="1">
+    <row r="3" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -4113,7 +4077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13.5" customHeight="1">
+    <row r="4" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -4142,47 +4106,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.5" customHeight="1">
+    <row r="5" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="13.5" customHeight="1">
+    <row r="6" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="13.5" customHeight="1">
+    <row r="7" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="13.5" customHeight="1">
+    <row r="8" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="13.5" customHeight="1">
+    <row r="9" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="13.5" customHeight="1">
+    <row r="10" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="13.5" customHeight="1">
+    <row r="11" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="13.5" customHeight="1">
+    <row r="12" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="13.5" customHeight="1">
+    <row r="13" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="G13" s="3"/>
@@ -4205,17 +4169,17 @@
       <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="26" width="8.83203125" customWidth="1"/>
+    <col min="1" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.5" customHeight="1">
+    <row r="1" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="13.5" customHeight="1">
+    <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="5">
         <v>2000</v>
       </c>
@@ -4283,7 +4247,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13.5" customHeight="1">
+    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4317,7 +4281,7 @@
       </c>
       <c r="Z3" s="12"/>
     </row>
-    <row r="4" spans="1:26" ht="13.5" customHeight="1">
+    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4359,7 +4323,7 @@
       </c>
       <c r="Z4" s="12"/>
     </row>
-    <row r="5" spans="1:26" ht="13.5" customHeight="1">
+    <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4393,8 +4357,8 @@
       </c>
       <c r="Z5" s="12"/>
     </row>
-    <row r="6" spans="1:26" ht="13.5" customHeight="1"/>
-    <row r="7" spans="1:26" ht="13.5" customHeight="1">
+    <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4428,7 +4392,7 @@
       </c>
       <c r="Z7" s="12"/>
     </row>
-    <row r="8" spans="1:26" ht="13.5" customHeight="1">
+    <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4470,7 +4434,7 @@
       </c>
       <c r="Z8" s="12"/>
     </row>
-    <row r="9" spans="1:26" ht="13.5" customHeight="1">
+    <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4504,7 +4468,7 @@
       </c>
       <c r="Z9" s="12"/>
     </row>
-    <row r="10" spans="1:26" ht="13.5" customHeight="1"/>
+    <row r="10" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4524,17 +4488,17 @@
       <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="26" width="8.83203125" customWidth="1"/>
+    <col min="1" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.5" customHeight="1">
+    <row r="1" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="13.5" customHeight="1">
+    <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="7">
         <v>2000</v>
       </c>
@@ -4602,7 +4566,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13.5" customHeight="1">
+    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4636,7 +4600,7 @@
       </c>
       <c r="Z3" s="10"/>
     </row>
-    <row r="4" spans="1:26" ht="13.5" customHeight="1">
+    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4676,7 +4640,7 @@
       </c>
       <c r="Z4" s="14"/>
     </row>
-    <row r="5" spans="1:26" ht="13.5" customHeight="1">
+    <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4710,8 +4674,8 @@
       </c>
       <c r="Z5" s="10"/>
     </row>
-    <row r="6" spans="1:26" ht="13.5" customHeight="1"/>
-    <row r="7" spans="1:26" ht="13.5" customHeight="1">
+    <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4745,7 +4709,7 @@
       </c>
       <c r="Z7" s="10"/>
     </row>
-    <row r="8" spans="1:26" ht="13.5" customHeight="1">
+    <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4785,7 +4749,7 @@
       </c>
       <c r="Z8" s="10"/>
     </row>
-    <row r="9" spans="1:26" ht="13.5" customHeight="1">
+    <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4839,17 +4803,17 @@
       <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="25" width="8.83203125" customWidth="1"/>
+    <col min="1" max="25" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -4917,7 +4881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4952,7 +4916,7 @@
       </c>
       <c r="Y3" s="10"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4987,15 +4951,15 @@
       </c>
       <c r="Y4" s="10"/>
     </row>
-    <row r="5" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="6" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1">
+    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -5063,7 +5027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5096,7 +5060,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5129,15 +5093,15 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1">
+    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -5205,7 +5169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:25" ht="13.5" customHeight="1">
+    <row r="17" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5238,7 +5202,7 @@
       </c>
       <c r="Y17" s="10"/>
     </row>
-    <row r="18" spans="2:25" ht="13.5" customHeight="1">
+    <row r="18" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5284,24 +5248,912 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y41"/>
+  <sheetViews>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AA31" sqref="AA31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="25" width="8.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E2" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F2" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G2" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H2" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I2" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J2" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K2" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L2" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M2" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N2" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O2" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P2" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R2" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S2" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T2" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U2" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V2" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W2" s="5">
+        <v>2020</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="str">
+        <f>Populations!$C$3</f>
+        <v>M 15-49</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15">
+        <v>6.4500000000000002E-2</v>
+      </c>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y3" s="15"/>
+    </row>
+    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="str">
+        <f>Populations!$C$4</f>
+        <v>F 15-49</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15">
+        <v>6.4500000000000002E-2</v>
+      </c>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y4" s="15"/>
+    </row>
+    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E9" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F9" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G9" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H9" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I9" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J9" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K9" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L9" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M9" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N9" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O9" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P9" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R9" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S9" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T9" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U9" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V9" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W9" s="5">
+        <v>2020</v>
+      </c>
+      <c r="Y9" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y10" s="16">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E15" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F15" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G15" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H15" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I15" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J15" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K15" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L15" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M15" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N15" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O15" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P15" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R15" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S15" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T15" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U15" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V15" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W15" s="5">
+        <v>2020</v>
+      </c>
+      <c r="Y15" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6">
+        <v>50</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6">
+        <v>600</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6">
+        <v>1900</v>
+      </c>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6">
+        <v>3200</v>
+      </c>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y16" s="6"/>
+    </row>
+    <row r="17" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D21" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E21" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F21" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G21" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H21" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I21" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J21" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K21" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L21" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M21" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N21" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O21" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P21" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R21" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S21" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T21" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U21" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V21" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W21" s="5">
+        <v>2020</v>
+      </c>
+      <c r="Y21" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="str">
+        <f>Populations!$C$3</f>
+        <v>M 15-49</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15">
+        <v>0</v>
+      </c>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y22" s="15"/>
+    </row>
+    <row r="23" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="str">
+        <f>Populations!$C$4</f>
+        <v>F 15-49</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15">
+        <v>0</v>
+      </c>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y23" s="15"/>
+    </row>
+    <row r="24" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E28" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F28" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G28" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H28" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I28" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J28" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K28" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L28" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M28" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N28" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O28" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P28" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q28" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R28" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S28" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T28" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U28" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V28" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W28" s="5">
+        <v>2020</v>
+      </c>
+      <c r="Y28" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="10">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="M29" s="10">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="N29" s="10">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="O29" s="10">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="P29" s="10">
+        <v>0.86</v>
+      </c>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y29" s="6"/>
+    </row>
+    <row r="30" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D34" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E34" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F34" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G34" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H34" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I34" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J34" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K34" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L34" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M34" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N34" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O34" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P34" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q34" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R34" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S34" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T34" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U34" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V34" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W34" s="5">
+        <v>2020</v>
+      </c>
+      <c r="Y34" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="str">
+        <f>Populations!$C$4</f>
+        <v>F 15-49</v>
+      </c>
+      <c r="C35" s="9">
+        <v>4.5925296336727484E-2</v>
+      </c>
+      <c r="D35" s="9">
+        <v>4.5324022610802442E-2</v>
+      </c>
+      <c r="E35" s="9">
+        <v>4.5258178531301665E-2</v>
+      </c>
+      <c r="F35" s="9">
+        <v>4.5643569591584512E-2</v>
+      </c>
+      <c r="G35" s="9">
+        <v>4.6393022020567463E-2</v>
+      </c>
+      <c r="H35" s="9">
+        <v>4.7380532618388635E-2</v>
+      </c>
+      <c r="I35" s="9">
+        <v>4.8776034491919598E-2</v>
+      </c>
+      <c r="J35" s="9">
+        <v>5.0081489017354618E-2</v>
+      </c>
+      <c r="K35" s="9">
+        <v>5.1207019154705748E-2</v>
+      </c>
+      <c r="L35" s="9">
+        <v>5.2116086916866047E-2</v>
+      </c>
+      <c r="M35" s="9">
+        <v>5.278448936292468E-2</v>
+      </c>
+      <c r="N35" s="9">
+        <v>5.2115181359517093E-2</v>
+      </c>
+      <c r="O35" s="9">
+        <v>5.2484499496074824E-2</v>
+      </c>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="9"/>
+      <c r="U35" s="9"/>
+      <c r="V35" s="9"/>
+      <c r="W35" s="9"/>
+      <c r="X35" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y35" s="9"/>
+    </row>
+    <row r="36" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D40" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E40" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F40" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G40" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H40" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I40" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J40" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K40" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L40" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M40" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N40" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O40" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P40" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q40" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R40" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S40" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T40" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U40" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V40" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W40" s="5">
+        <v>2020</v>
+      </c>
+      <c r="Y40" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
+      <c r="R41" s="15"/>
+      <c r="S41" s="15"/>
+      <c r="T41" s="15"/>
+      <c r="U41" s="15"/>
+      <c r="V41" s="15"/>
+      <c r="W41" s="15"/>
+      <c r="X41" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y41" s="18">
+        <f>14/100*87/100</f>
+        <v>0.12180000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y54"/>
+  <dimension ref="A1:Y57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="25" width="8.83203125" customWidth="1"/>
+    <col min="1" max="25" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -5369,7 +6221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -5399,15 +6251,15 @@
       </c>
       <c r="Y3" s="9"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="5" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="6" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1">
+    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="5">
         <v>2000</v>
       </c>
@@ -5475,7 +6327,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
@@ -5505,15 +6357,15 @@
       </c>
       <c r="Y9" s="9"/>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1">
+    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="5">
         <v>2000</v>
       </c>
@@ -5581,7 +6433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1">
+    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
@@ -5611,15 +6463,15 @@
       </c>
       <c r="Y15" s="9"/>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="17" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="18" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="19" spans="1:25" ht="13.5" customHeight="1">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="13.5" customHeight="1">
+    <row r="20" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="5">
         <v>2000</v>
       </c>
@@ -5687,7 +6539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="13.5" customHeight="1">
+    <row r="21" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
@@ -5717,15 +6569,15 @@
       </c>
       <c r="Y21" s="9"/>
     </row>
-    <row r="22" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="23" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="24" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="25" spans="1:25" ht="13.5" customHeight="1">
+    <row r="22" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="13.5" customHeight="1">
+    <row r="26" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="7">
         <v>2000</v>
       </c>
@@ -5793,7 +6645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="13.5" customHeight="1">
+    <row r="27" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>14</v>
       </c>
@@ -5823,15 +6675,15 @@
       </c>
       <c r="Y27" s="9"/>
     </row>
-    <row r="28" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="29" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="30" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="31" spans="1:25" ht="13.5" customHeight="1">
+    <row r="28" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="13.5" customHeight="1">
+    <row r="32" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="5">
         <v>2000</v>
       </c>
@@ -5899,7 +6751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="13.5" customHeight="1">
+    <row r="33" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>14</v>
       </c>
@@ -5929,15 +6781,15 @@
       </c>
       <c r="Y33" s="9"/>
     </row>
-    <row r="34" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="35" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="36" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="37" spans="1:25" ht="13.5" customHeight="1">
+    <row r="34" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="13.5" customHeight="1">
+    <row r="38" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="5">
         <v>2000</v>
       </c>
@@ -6005,7 +6857,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="13.5" customHeight="1">
+    <row r="39" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>14</v>
       </c>
@@ -6035,7 +6887,7 @@
       </c>
       <c r="Y39" s="9"/>
     </row>
-    <row r="43" spans="1:25" ht="14">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="34" t="s">
         <v>116</v>
       </c>
@@ -6064,7 +6916,7 @@
       <c r="X43" s="31"/>
       <c r="Y43" s="31"/>
     </row>
-    <row r="44" spans="1:25" ht="14">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="31"/>
       <c r="B44" s="31"/>
       <c r="C44" s="35">
@@ -6135,7 +6987,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="14">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="31"/>
       <c r="B45" s="35" t="s">
         <v>30</v>
@@ -6166,11 +7018,11 @@
       </c>
       <c r="Y45" s="37"/>
     </row>
-    <row r="46" spans="1:25" ht="12"/>
-    <row r="47" spans="1:25" ht="12"/>
-    <row r="48" spans="1:25" ht="12"/>
-    <row r="49" spans="1:25" ht="14">
-      <c r="A49" s="42" t="s">
+    <row r="46" spans="1:25" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:25" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:25" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A49" s="40" t="s">
         <v>119</v>
       </c>
       <c r="B49" s="31"/>
@@ -6198,7 +7050,7 @@
       <c r="X49" s="31"/>
       <c r="Y49" s="31"/>
     </row>
-    <row r="50" spans="1:25" ht="14">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" s="31"/>
       <c r="B50" s="31"/>
       <c r="C50" s="35">
@@ -6269,7 +7121,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:25" ht="14">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="31"/>
       <c r="B51" s="35" t="s">
         <v>30</v>
@@ -6300,900 +7152,143 @@
       </c>
       <c r="Y51" s="37"/>
     </row>
-    <row r="52" spans="1:25" ht="12"/>
-    <row r="53" spans="1:25" ht="12"/>
-    <row r="54" spans="1:25" ht="12"/>
+    <row r="52" spans="1:25" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:25" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:25" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" s="31"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
+      <c r="H55" s="31"/>
+      <c r="I55" s="31"/>
+      <c r="J55" s="31"/>
+      <c r="K55" s="31"/>
+      <c r="L55" s="31"/>
+      <c r="M55" s="31"/>
+      <c r="N55" s="31"/>
+      <c r="O55" s="31"/>
+      <c r="P55" s="31"/>
+      <c r="Q55" s="31"/>
+      <c r="R55" s="31"/>
+      <c r="S55" s="31"/>
+      <c r="T55" s="31"/>
+      <c r="U55" s="31"/>
+      <c r="V55" s="31"/>
+      <c r="W55" s="31"/>
+      <c r="X55" s="31"/>
+      <c r="Y55" s="31"/>
+    </row>
+    <row r="56" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="31"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D56" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E56" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F56" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G56" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H56" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I56" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J56" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K56" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L56" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M56" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N56" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O56" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P56" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q56" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R56" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S56" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T56" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U56" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V56" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W56" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X56" s="31"/>
+      <c r="Y56" s="35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="31"/>
+      <c r="B57" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="37"/>
+      <c r="L57" s="37"/>
+      <c r="M57" s="37"/>
+      <c r="N57" s="37"/>
+      <c r="O57" s="37"/>
+      <c r="P57" s="37"/>
+      <c r="Q57" s="37"/>
+      <c r="R57" s="37"/>
+      <c r="S57" s="37"/>
+      <c r="T57" s="37"/>
+      <c r="U57" s="37"/>
+      <c r="V57" s="37"/>
+      <c r="W57" s="37"/>
+      <c r="X57" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y57" s="37"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y41"/>
-  <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AA31" sqref="AA31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="25" width="8.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1">
-      <c r="C2" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D2" s="5">
-        <v>2001</v>
-      </c>
-      <c r="E2" s="5">
-        <v>2002</v>
-      </c>
-      <c r="F2" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G2" s="5">
-        <v>2004</v>
-      </c>
-      <c r="H2" s="5">
-        <v>2005</v>
-      </c>
-      <c r="I2" s="5">
-        <v>2006</v>
-      </c>
-      <c r="J2" s="5">
-        <v>2007</v>
-      </c>
-      <c r="K2" s="5">
-        <v>2008</v>
-      </c>
-      <c r="L2" s="5">
-        <v>2009</v>
-      </c>
-      <c r="M2" s="5">
-        <v>2010</v>
-      </c>
-      <c r="N2" s="5">
-        <v>2011</v>
-      </c>
-      <c r="O2" s="5">
-        <v>2012</v>
-      </c>
-      <c r="P2" s="5">
-        <v>2013</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>2014</v>
-      </c>
-      <c r="R2" s="5">
-        <v>2015</v>
-      </c>
-      <c r="S2" s="5">
-        <v>2016</v>
-      </c>
-      <c r="T2" s="5">
-        <v>2017</v>
-      </c>
-      <c r="U2" s="5">
-        <v>2018</v>
-      </c>
-      <c r="V2" s="5">
-        <v>2019</v>
-      </c>
-      <c r="W2" s="5">
-        <v>2020</v>
-      </c>
-      <c r="Y2" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1">
-      <c r="B3" s="7" t="str">
-        <f>Populations!$C$3</f>
-        <v>M 15-49</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15">
-        <v>6.4500000000000002E-2</v>
-      </c>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y3" s="15"/>
-    </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1">
-      <c r="B4" s="7" t="str">
-        <f>Populations!$C$4</f>
-        <v>F 15-49</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15">
-        <v>6.4500000000000002E-2</v>
-      </c>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y4" s="15"/>
-    </row>
-    <row r="5" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="6" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1">
-      <c r="C9" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D9" s="5">
-        <v>2001</v>
-      </c>
-      <c r="E9" s="5">
-        <v>2002</v>
-      </c>
-      <c r="F9" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G9" s="5">
-        <v>2004</v>
-      </c>
-      <c r="H9" s="5">
-        <v>2005</v>
-      </c>
-      <c r="I9" s="5">
-        <v>2006</v>
-      </c>
-      <c r="J9" s="5">
-        <v>2007</v>
-      </c>
-      <c r="K9" s="5">
-        <v>2008</v>
-      </c>
-      <c r="L9" s="5">
-        <v>2009</v>
-      </c>
-      <c r="M9" s="5">
-        <v>2010</v>
-      </c>
-      <c r="N9" s="5">
-        <v>2011</v>
-      </c>
-      <c r="O9" s="5">
-        <v>2012</v>
-      </c>
-      <c r="P9" s="5">
-        <v>2013</v>
-      </c>
-      <c r="Q9" s="5">
-        <v>2014</v>
-      </c>
-      <c r="R9" s="5">
-        <v>2015</v>
-      </c>
-      <c r="S9" s="5">
-        <v>2016</v>
-      </c>
-      <c r="T9" s="5">
-        <v>2017</v>
-      </c>
-      <c r="U9" s="5">
-        <v>2018</v>
-      </c>
-      <c r="V9" s="5">
-        <v>2019</v>
-      </c>
-      <c r="W9" s="5">
-        <v>2020</v>
-      </c>
-      <c r="Y9" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1">
-      <c r="B10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y10" s="16">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="C15" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D15" s="5">
-        <v>2001</v>
-      </c>
-      <c r="E15" s="5">
-        <v>2002</v>
-      </c>
-      <c r="F15" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G15" s="5">
-        <v>2004</v>
-      </c>
-      <c r="H15" s="5">
-        <v>2005</v>
-      </c>
-      <c r="I15" s="5">
-        <v>2006</v>
-      </c>
-      <c r="J15" s="5">
-        <v>2007</v>
-      </c>
-      <c r="K15" s="5">
-        <v>2008</v>
-      </c>
-      <c r="L15" s="5">
-        <v>2009</v>
-      </c>
-      <c r="M15" s="5">
-        <v>2010</v>
-      </c>
-      <c r="N15" s="5">
-        <v>2011</v>
-      </c>
-      <c r="O15" s="5">
-        <v>2012</v>
-      </c>
-      <c r="P15" s="5">
-        <v>2013</v>
-      </c>
-      <c r="Q15" s="5">
-        <v>2014</v>
-      </c>
-      <c r="R15" s="5">
-        <v>2015</v>
-      </c>
-      <c r="S15" s="5">
-        <v>2016</v>
-      </c>
-      <c r="T15" s="5">
-        <v>2017</v>
-      </c>
-      <c r="U15" s="5">
-        <v>2018</v>
-      </c>
-      <c r="V15" s="5">
-        <v>2019</v>
-      </c>
-      <c r="W15" s="5">
-        <v>2020</v>
-      </c>
-      <c r="Y15" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1">
-      <c r="B16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="6">
-        <v>0</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6">
-        <v>50</v>
-      </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6">
-        <v>600</v>
-      </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6">
-        <v>1900</v>
-      </c>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6">
-        <v>3200</v>
-      </c>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6"/>
-      <c r="W16" s="6"/>
-      <c r="X16" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y16" s="6"/>
-    </row>
-    <row r="17" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="18" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="19" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="20" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" ht="13.5" customHeight="1">
-      <c r="C21" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D21" s="5">
-        <v>2001</v>
-      </c>
-      <c r="E21" s="5">
-        <v>2002</v>
-      </c>
-      <c r="F21" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G21" s="5">
-        <v>2004</v>
-      </c>
-      <c r="H21" s="5">
-        <v>2005</v>
-      </c>
-      <c r="I21" s="5">
-        <v>2006</v>
-      </c>
-      <c r="J21" s="5">
-        <v>2007</v>
-      </c>
-      <c r="K21" s="5">
-        <v>2008</v>
-      </c>
-      <c r="L21" s="5">
-        <v>2009</v>
-      </c>
-      <c r="M21" s="5">
-        <v>2010</v>
-      </c>
-      <c r="N21" s="5">
-        <v>2011</v>
-      </c>
-      <c r="O21" s="5">
-        <v>2012</v>
-      </c>
-      <c r="P21" s="5">
-        <v>2013</v>
-      </c>
-      <c r="Q21" s="5">
-        <v>2014</v>
-      </c>
-      <c r="R21" s="5">
-        <v>2015</v>
-      </c>
-      <c r="S21" s="5">
-        <v>2016</v>
-      </c>
-      <c r="T21" s="5">
-        <v>2017</v>
-      </c>
-      <c r="U21" s="5">
-        <v>2018</v>
-      </c>
-      <c r="V21" s="5">
-        <v>2019</v>
-      </c>
-      <c r="W21" s="5">
-        <v>2020</v>
-      </c>
-      <c r="Y21" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" ht="13.5" customHeight="1">
-      <c r="B22" s="7" t="str">
-        <f>Populations!$C$3</f>
-        <v>M 15-49</v>
-      </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15">
-        <v>0</v>
-      </c>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="15"/>
-      <c r="U22" s="15"/>
-      <c r="V22" s="15"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y22" s="15"/>
-    </row>
-    <row r="23" spans="1:25" ht="13.5" customHeight="1">
-      <c r="B23" s="7" t="str">
-        <f>Populations!$C$4</f>
-        <v>F 15-49</v>
-      </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15">
-        <v>0</v>
-      </c>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="15"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y23" s="15"/>
-    </row>
-    <row r="24" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="25" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="26" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="27" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A27" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" ht="13.5" customHeight="1">
-      <c r="C28" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D28" s="5">
-        <v>2001</v>
-      </c>
-      <c r="E28" s="5">
-        <v>2002</v>
-      </c>
-      <c r="F28" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G28" s="5">
-        <v>2004</v>
-      </c>
-      <c r="H28" s="5">
-        <v>2005</v>
-      </c>
-      <c r="I28" s="5">
-        <v>2006</v>
-      </c>
-      <c r="J28" s="5">
-        <v>2007</v>
-      </c>
-      <c r="K28" s="5">
-        <v>2008</v>
-      </c>
-      <c r="L28" s="5">
-        <v>2009</v>
-      </c>
-      <c r="M28" s="5">
-        <v>2010</v>
-      </c>
-      <c r="N28" s="5">
-        <v>2011</v>
-      </c>
-      <c r="O28" s="5">
-        <v>2012</v>
-      </c>
-      <c r="P28" s="5">
-        <v>2013</v>
-      </c>
-      <c r="Q28" s="5">
-        <v>2014</v>
-      </c>
-      <c r="R28" s="5">
-        <v>2015</v>
-      </c>
-      <c r="S28" s="5">
-        <v>2016</v>
-      </c>
-      <c r="T28" s="5">
-        <v>2017</v>
-      </c>
-      <c r="U28" s="5">
-        <v>2018</v>
-      </c>
-      <c r="V28" s="5">
-        <v>2019</v>
-      </c>
-      <c r="W28" s="5">
-        <v>2020</v>
-      </c>
-      <c r="Y28" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" ht="13.5" customHeight="1">
-      <c r="B29" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="10">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="M29" s="10">
-        <v>0.82099999999999995</v>
-      </c>
-      <c r="N29" s="10">
-        <v>0.82299999999999995</v>
-      </c>
-      <c r="O29" s="10">
-        <v>0.85799999999999998</v>
-      </c>
-      <c r="P29" s="10">
-        <v>0.86</v>
-      </c>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6"/>
-      <c r="U29" s="6"/>
-      <c r="V29" s="6"/>
-      <c r="W29" s="6"/>
-      <c r="X29" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y29" s="6"/>
-    </row>
-    <row r="30" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="31" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="32" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="33" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25" ht="13.5" customHeight="1">
-      <c r="C34" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D34" s="5">
-        <v>2001</v>
-      </c>
-      <c r="E34" s="5">
-        <v>2002</v>
-      </c>
-      <c r="F34" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G34" s="5">
-        <v>2004</v>
-      </c>
-      <c r="H34" s="5">
-        <v>2005</v>
-      </c>
-      <c r="I34" s="5">
-        <v>2006</v>
-      </c>
-      <c r="J34" s="5">
-        <v>2007</v>
-      </c>
-      <c r="K34" s="5">
-        <v>2008</v>
-      </c>
-      <c r="L34" s="5">
-        <v>2009</v>
-      </c>
-      <c r="M34" s="5">
-        <v>2010</v>
-      </c>
-      <c r="N34" s="5">
-        <v>2011</v>
-      </c>
-      <c r="O34" s="5">
-        <v>2012</v>
-      </c>
-      <c r="P34" s="5">
-        <v>2013</v>
-      </c>
-      <c r="Q34" s="5">
-        <v>2014</v>
-      </c>
-      <c r="R34" s="5">
-        <v>2015</v>
-      </c>
-      <c r="S34" s="5">
-        <v>2016</v>
-      </c>
-      <c r="T34" s="5">
-        <v>2017</v>
-      </c>
-      <c r="U34" s="5">
-        <v>2018</v>
-      </c>
-      <c r="V34" s="5">
-        <v>2019</v>
-      </c>
-      <c r="W34" s="5">
-        <v>2020</v>
-      </c>
-      <c r="Y34" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25" ht="13.5" customHeight="1">
-      <c r="B35" s="7" t="str">
-        <f>Populations!$C$4</f>
-        <v>F 15-49</v>
-      </c>
-      <c r="C35" s="9">
-        <v>4.5925296336727484E-2</v>
-      </c>
-      <c r="D35" s="9">
-        <v>4.5324022610802442E-2</v>
-      </c>
-      <c r="E35" s="9">
-        <v>4.5258178531301665E-2</v>
-      </c>
-      <c r="F35" s="9">
-        <v>4.5643569591584512E-2</v>
-      </c>
-      <c r="G35" s="9">
-        <v>4.6393022020567463E-2</v>
-      </c>
-      <c r="H35" s="9">
-        <v>4.7380532618388635E-2</v>
-      </c>
-      <c r="I35" s="9">
-        <v>4.8776034491919598E-2</v>
-      </c>
-      <c r="J35" s="9">
-        <v>5.0081489017354618E-2</v>
-      </c>
-      <c r="K35" s="9">
-        <v>5.1207019154705748E-2</v>
-      </c>
-      <c r="L35" s="9">
-        <v>5.2116086916866047E-2</v>
-      </c>
-      <c r="M35" s="9">
-        <v>5.278448936292468E-2</v>
-      </c>
-      <c r="N35" s="9">
-        <v>5.2115181359517093E-2</v>
-      </c>
-      <c r="O35" s="9">
-        <v>5.2484499496074824E-2</v>
-      </c>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="9"/>
-      <c r="T35" s="9"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="9"/>
-      <c r="W35" s="9"/>
-      <c r="X35" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y35" s="9"/>
-    </row>
-    <row r="36" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="37" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="38" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="39" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A39" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25" ht="13.5" customHeight="1">
-      <c r="C40" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D40" s="5">
-        <v>2001</v>
-      </c>
-      <c r="E40" s="5">
-        <v>2002</v>
-      </c>
-      <c r="F40" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G40" s="5">
-        <v>2004</v>
-      </c>
-      <c r="H40" s="5">
-        <v>2005</v>
-      </c>
-      <c r="I40" s="5">
-        <v>2006</v>
-      </c>
-      <c r="J40" s="5">
-        <v>2007</v>
-      </c>
-      <c r="K40" s="5">
-        <v>2008</v>
-      </c>
-      <c r="L40" s="5">
-        <v>2009</v>
-      </c>
-      <c r="M40" s="5">
-        <v>2010</v>
-      </c>
-      <c r="N40" s="5">
-        <v>2011</v>
-      </c>
-      <c r="O40" s="5">
-        <v>2012</v>
-      </c>
-      <c r="P40" s="5">
-        <v>2013</v>
-      </c>
-      <c r="Q40" s="5">
-        <v>2014</v>
-      </c>
-      <c r="R40" s="5">
-        <v>2015</v>
-      </c>
-      <c r="S40" s="5">
-        <v>2016</v>
-      </c>
-      <c r="T40" s="5">
-        <v>2017</v>
-      </c>
-      <c r="U40" s="5">
-        <v>2018</v>
-      </c>
-      <c r="V40" s="5">
-        <v>2019</v>
-      </c>
-      <c r="W40" s="5">
-        <v>2020</v>
-      </c>
-      <c r="Y40" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" ht="13.5" customHeight="1">
-      <c r="B41" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="15"/>
-      <c r="S41" s="15"/>
-      <c r="T41" s="15"/>
-      <c r="U41" s="15"/>
-      <c r="V41" s="15"/>
-      <c r="W41" s="15"/>
-      <c r="X41" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y41" s="18">
-        <f>14/100*87/100</f>
-        <v>0.12180000000000002</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7210,9 +7305,9 @@
       <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="14">
+    <row r="1" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>106</v>
       </c>
@@ -7241,7 +7336,7 @@
       <c r="X1" s="31"/>
       <c r="Y1" s="31"/>
     </row>
-    <row r="2" spans="1:25" ht="14">
+    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="35">
@@ -7312,7 +7407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="14">
+    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
       <c r="B3" s="32" t="s">
         <v>95</v>
@@ -7345,7 +7440,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="14">
+    <row r="4" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" s="32" t="s">
         <v>96</v>
@@ -7378,7 +7473,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="14">
+    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>101</v>
       </c>
@@ -7407,7 +7502,7 @@
       <c r="X8" s="31"/>
       <c r="Y8" s="31"/>
     </row>
-    <row r="9" spans="1:25" ht="14">
+    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="31"/>
       <c r="C9" s="35">
@@ -7478,7 +7573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="14">
+    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
       <c r="B10" s="32" t="s">
         <v>95</v>
@@ -7511,7 +7606,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="14">
+    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
         <v>96</v>
@@ -7544,7 +7639,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="14">
+    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>107</v>
       </c>
@@ -7573,7 +7668,7 @@
       <c r="X15" s="31"/>
       <c r="Y15" s="31"/>
     </row>
-    <row r="16" spans="1:25" ht="14">
+    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
       <c r="B16" s="31"/>
       <c r="C16" s="35">
@@ -7644,7 +7739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="14">
+    <row r="17" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
       <c r="B17" s="32" t="s">
         <v>95</v>
@@ -7677,7 +7772,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="14">
+    <row r="18" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="31"/>
       <c r="B18" s="32" t="s">
         <v>96</v>
@@ -7710,7 +7805,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="14">
+    <row r="22" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
         <v>108</v>
       </c>
@@ -7739,7 +7834,7 @@
       <c r="X22" s="31"/>
       <c r="Y22" s="31"/>
     </row>
-    <row r="23" spans="1:25" ht="14">
+    <row r="23" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
       <c r="B23" s="31"/>
       <c r="C23" s="35">
@@ -7810,7 +7905,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="14">
+    <row r="24" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
       <c r="B24" s="32" t="s">
         <v>95</v>
@@ -7843,7 +7938,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="14">
+    <row r="25" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
       <c r="B25" s="32" t="s">
         <v>96</v>
@@ -7876,7 +7971,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="14">
+    <row r="29" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
         <v>113</v>
       </c>
@@ -7905,7 +8000,7 @@
       <c r="X29" s="31"/>
       <c r="Y29" s="31"/>
     </row>
-    <row r="30" spans="1:25" ht="14">
+    <row r="30" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
       <c r="B30" s="31"/>
       <c r="C30" s="35">
@@ -7976,7 +8071,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="14">
+    <row r="31" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
       <c r="B31" s="35" t="s">
         <v>30</v>
@@ -8009,7 +8104,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="14">
+    <row r="35" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="34" t="s">
         <v>102</v>
       </c>
@@ -8038,7 +8133,7 @@
       <c r="X35" s="31"/>
       <c r="Y35" s="31"/>
     </row>
-    <row r="36" spans="1:25" ht="14">
+    <row r="36" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="31"/>
       <c r="B36" s="31"/>
       <c r="C36" s="35">
@@ -8109,7 +8204,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="14">
+    <row r="37" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="31"/>
       <c r="B37" s="35" t="s">
         <v>30</v>
@@ -8142,7 +8237,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="14">
+    <row r="41" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="34" t="s">
         <v>114</v>
       </c>
@@ -8171,7 +8266,7 @@
       <c r="X41" s="31"/>
       <c r="Y41" s="31"/>
     </row>
-    <row r="42" spans="1:25" ht="14">
+    <row r="42" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="31"/>
       <c r="B42" s="31"/>
       <c r="C42" s="35">
@@ -8242,7 +8337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="14">
+    <row r="43" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="31"/>
       <c r="B43" s="35" t="s">
         <v>30</v>
@@ -8275,7 +8370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="14">
+    <row r="47" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="34" t="s">
         <v>115</v>
       </c>
@@ -8304,7 +8399,7 @@
       <c r="X47" s="31"/>
       <c r="Y47" s="31"/>
     </row>
-    <row r="48" spans="1:25" ht="14">
+    <row r="48" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="31"/>
       <c r="B48" s="31"/>
       <c r="C48" s="35">
@@ -8375,7 +8470,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="14">
+    <row r="49" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="31"/>
       <c r="B49" s="35" t="s">
         <v>30</v>
@@ -8408,7 +8503,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="14">
+    <row r="53" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="34" t="s">
         <v>117</v>
       </c>
@@ -8437,7 +8532,7 @@
       <c r="X53" s="31"/>
       <c r="Y53" s="31"/>
     </row>
-    <row r="54" spans="1:25" ht="14">
+    <row r="54" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="31"/>
       <c r="B54" s="31"/>
       <c r="C54" s="35">
@@ -8508,7 +8603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="14">
+    <row r="55" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="31"/>
       <c r="B55" s="35" t="s">
         <v>30</v>
@@ -8541,7 +8636,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="59" spans="1:25" ht="14">
+    <row r="59" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="34" t="s">
         <v>118</v>
       </c>
@@ -8570,7 +8665,7 @@
       <c r="X59" s="31"/>
       <c r="Y59" s="31"/>
     </row>
-    <row r="60" spans="1:25" ht="14">
+    <row r="60" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="31"/>
       <c r="B60" s="31"/>
       <c r="C60" s="35">
@@ -8641,7 +8736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:25" ht="14">
+    <row r="61" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="31"/>
       <c r="B61" s="35" t="s">
         <v>30</v>
@@ -8693,17 +8788,17 @@
       <selection activeCell="AA53" sqref="AA53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="25" width="8.83203125" customWidth="1"/>
+    <col min="1" max="25" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -8771,7 +8866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -8804,7 +8899,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -8837,15 +8932,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="6" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1">
+    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -8913,7 +9008,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -8947,7 +9042,7 @@
         <v>12.000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -8981,15 +9076,15 @@
         <v>6.0000000000000009</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1">
+    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -9057,7 +9152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="13.5" customHeight="1">
+    <row r="17" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9090,7 +9185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="13.5" customHeight="1">
+    <row r="18" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9123,15 +9218,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="20" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="21" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="22" spans="1:25" ht="13.5" customHeight="1">
+    <row r="19" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="13.5" customHeight="1">
+    <row r="23" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="5">
         <v>2000</v>
       </c>
@@ -9199,7 +9294,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="13.5" customHeight="1">
+    <row r="24" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9232,7 +9327,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="13.5" customHeight="1">
+    <row r="25" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9265,15 +9360,15 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="27" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="28" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="29" spans="1:25" ht="13.5" customHeight="1">
+    <row r="26" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="13.5" customHeight="1">
+    <row r="30" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="5">
         <v>2000</v>
       </c>
@@ -9341,7 +9436,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="13.5" customHeight="1">
+    <row r="31" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9374,7 +9469,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="13.5" customHeight="1">
+    <row r="32" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9407,15 +9502,15 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="34" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="35" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="36" spans="1:25" ht="13.5" customHeight="1">
+    <row r="33" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="13.5" customHeight="1">
+    <row r="37" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="5">
         <v>2000</v>
       </c>
@@ -9483,7 +9578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="13.5" customHeight="1">
+    <row r="38" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9516,7 +9611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="13.5" customHeight="1">
+    <row r="39" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9549,15 +9644,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="41" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="42" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="43" spans="1:25" ht="13.5" customHeight="1">
+    <row r="40" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="13.5" customHeight="1">
+    <row r="44" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44" s="5">
         <v>2000</v>
       </c>
@@ -9625,7 +9720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="13.5" customHeight="1">
+    <row r="45" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>

</xml_diff>

<commit_message>
remove proportion pmtct option from spreadsheets
</commit_message>
<xml_diff>
--- a/tests/simple.xlsx
+++ b/tests/simple.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14715" tabRatio="861" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="861" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Partnerships &amp; transitions" sheetId="10" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -81,18 +81,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="L29" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Laura Grobicki:
-This value refers to number of pregnant women tested for HIV and who receive PMTCT</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="Y41" authorId="0">
       <text>
         <r>
@@ -240,9 +228,6 @@
     <t>Average number of acts with casual partners per person per year</t>
   </si>
   <si>
-    <t>Number (or percentage) of women on PMTCT (Option B/B+)</t>
-  </si>
-  <si>
     <t>Average percentage of people who receptively shared a needle/syringe at last injection</t>
   </si>
   <si>
@@ -499,6 +484,9 @@
   </si>
   <si>
     <t>PLHIV in care on treatment (%)</t>
+  </si>
+  <si>
+    <t>Number of women on PMTCT (Option B/B+)</t>
   </si>
 </sst>
 </file>
@@ -506,8 +494,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
@@ -723,12 +711,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="118">
+  <cellStyleXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -842,6 +830,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -928,7 +918,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="118">
+  <cellStyles count="120">
     <cellStyle name="Comma 2" xfId="4"/>
     <cellStyle name="Comma 3" xfId="2"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
@@ -937,6 +927,7 @@
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="15"/>
     <cellStyle name="Followed Hyperlink 11" xfId="16"/>
     <cellStyle name="Followed Hyperlink 12" xfId="17"/>
@@ -1040,6 +1031,7 @@
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Normal 3" xfId="6"/>
@@ -2304,36 +2296,36 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="89.7109375" customWidth="1"/>
+    <col min="1" max="1" width="89.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="12.75" customHeight="1">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" s="42"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" s="42"/>
     </row>
-    <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="14">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="67.5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="14">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="14">
       <c r="A7" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2357,17 +2349,17 @@
       <selection activeCell="X1" sqref="X1:AG1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="25" width="8.85546875" customWidth="1"/>
+    <col min="1" max="25" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -2435,7 +2427,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2468,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2501,15 +2493,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="8" spans="1:25" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -2577,7 +2569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2610,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2643,15 +2635,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="13" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="14" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="15" spans="1:25" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="13.5" customHeight="1">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -2719,7 +2711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:25" ht="13.5" customHeight="1">
       <c r="B17" s="22" t="s">
         <v>14</v>
       </c>
@@ -2751,9 +2743,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="2:25" ht="13.5" customHeight="1"/>
+    <row r="19" spans="2:25" ht="13.5" customHeight="1"/>
+    <row r="20" spans="2:25" ht="13.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2772,21 +2764,21 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="6" width="8.85546875" customWidth="1"/>
+    <col min="1" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="6" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13.5" customHeight="1">
       <c r="C2" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2796,7 +2788,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2806,7 +2798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2814,26 +2806,26 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13.5" customHeight="1">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="13.5" customHeight="1">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="13.5" customHeight="1">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="13.5" customHeight="1">
       <c r="C9" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2843,7 +2835,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="13.5" customHeight="1">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2853,7 +2845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="13.5" customHeight="1">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2861,26 +2853,26 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="13.5" customHeight="1">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="13.5" customHeight="1">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="13.5" customHeight="1">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="13.5" customHeight="1">
       <c r="C16" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2890,7 +2882,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="13.5" customHeight="1">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2898,7 +2890,7 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="13.5" customHeight="1">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2906,26 +2898,26 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="13.5" customHeight="1">
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="13.5" customHeight="1">
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="13.5" customHeight="1">
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="13.5" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="13.5" customHeight="1">
       <c r="C23" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2935,7 +2927,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="13.5" customHeight="1">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2943,7 +2935,7 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="13.5" customHeight="1">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2951,14 +2943,14 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="13.5" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="13.5" customHeight="1">
       <c r="C30" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2968,7 +2960,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="13.5" customHeight="1">
       <c r="B31" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2976,14 +2968,14 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="35" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="13.5" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="13.5" customHeight="1">
       <c r="C36" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2993,7 +2985,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="13.5" customHeight="1">
       <c r="B37" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3001,7 +2993,7 @@
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="13.5" customHeight="1">
       <c r="B38" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3009,14 +3001,14 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="42" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="13.5" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="13.5" customHeight="1">
       <c r="C43" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3026,7 +3018,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="13.5" customHeight="1">
       <c r="B44" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3034,7 +3026,7 @@
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="13.5" customHeight="1">
       <c r="B45" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3061,23 +3053,23 @@
       <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="6" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="6" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="13.5" customHeight="1">
       <c r="A1" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.5" customHeight="1">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="27" t="s">
@@ -3090,10 +3082,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.5" customHeight="1">
       <c r="A3" s="24"/>
       <c r="B3" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="28">
         <v>4.0000000000000002E-4</v>
@@ -3105,10 +3097,10 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.5" customHeight="1">
       <c r="A4" s="24"/>
       <c r="B4" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="28">
         <v>8.0000000000000004E-4</v>
@@ -3120,10 +3112,10 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.5" customHeight="1">
       <c r="A5" s="24"/>
       <c r="B5" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="28">
         <v>1.38E-2</v>
@@ -3135,10 +3127,10 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.5" customHeight="1">
       <c r="A6" s="24"/>
       <c r="B6" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="28">
         <v>1.1000000000000001E-3</v>
@@ -3150,10 +3142,10 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.5" customHeight="1">
       <c r="A7" s="24"/>
       <c r="B7" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="28">
         <v>8.0000000000000002E-3</v>
@@ -3165,10 +3157,10 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.5" customHeight="1">
       <c r="A8" s="24"/>
       <c r="B8" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="28">
         <v>0.36699999999999999</v>
@@ -3180,10 +3172,10 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.5" customHeight="1">
       <c r="A9" s="24"/>
       <c r="B9" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="28">
         <v>0.20499999999999999</v>
@@ -3195,25 +3187,25 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.5" customHeight="1">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="13.5" customHeight="1">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="13.5" customHeight="1">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="13.5" customHeight="1">
       <c r="A13" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="13.5" customHeight="1">
       <c r="A14" s="24"/>
       <c r="B14" s="24"/>
       <c r="C14" s="27" t="s">
@@ -3226,10 +3218,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="13.5" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="29">
         <v>26.03</v>
@@ -3241,10 +3233,10 @@
         <v>48.02</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="13.5" customHeight="1">
       <c r="A16" s="24"/>
       <c r="B16" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="29">
         <v>1</v>
@@ -3256,10 +3248,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="13.5" customHeight="1">
       <c r="A17" s="24"/>
       <c r="B17" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="29">
         <v>1</v>
@@ -3271,10 +3263,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="13.5" customHeight="1">
       <c r="A18" s="24"/>
       <c r="B18" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="29">
         <v>1</v>
@@ -3286,10 +3278,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="13.5" customHeight="1">
       <c r="A19" s="24"/>
       <c r="B19" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="29">
         <v>3.49</v>
@@ -3301,10 +3293,10 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="13.5" customHeight="1">
       <c r="A20" s="24"/>
       <c r="B20" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="29">
         <v>7.17</v>
@@ -3316,25 +3308,25 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="13.5" customHeight="1">
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="13.5" customHeight="1">
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="13.5" customHeight="1">
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="13.5" customHeight="1">
       <c r="A24" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
     </row>
-    <row r="25" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="13.5" customHeight="1">
       <c r="A25" s="24"/>
       <c r="B25" s="24"/>
       <c r="C25" s="27" t="s">
@@ -3347,10 +3339,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="13.5" customHeight="1">
       <c r="A26" s="24"/>
       <c r="B26" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C26" s="30">
         <v>4.1399999999999997</v>
@@ -3362,10 +3354,10 @@
         <v>9.76</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="13.5" customHeight="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="30">
         <v>1.05</v>
@@ -3377,10 +3369,10 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="13.5" customHeight="1">
       <c r="A28" s="24"/>
       <c r="B28" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="30">
         <v>0.33</v>
@@ -3392,10 +3384,10 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="13.5" customHeight="1">
       <c r="A29" s="24"/>
       <c r="B29" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29" s="30">
         <v>0.27</v>
@@ -3407,10 +3399,10 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="13.5" customHeight="1">
       <c r="A30" s="24"/>
       <c r="B30" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C30" s="30">
         <v>0.67</v>
@@ -3422,25 +3414,25 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="13.5" customHeight="1">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="13.5" customHeight="1">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="13.5" customHeight="1">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="13.5" customHeight="1">
       <c r="A34" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34" s="24"/>
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
       <c r="E34" s="24"/>
     </row>
-    <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="13.5" customHeight="1">
       <c r="A35" s="24"/>
       <c r="B35" s="24"/>
       <c r="C35" s="27" t="s">
@@ -3453,10 +3445,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="13.5" customHeight="1">
       <c r="A36" s="24"/>
       <c r="B36" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C36" s="30">
         <v>0.45</v>
@@ -3468,10 +3460,10 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="13.5" customHeight="1">
       <c r="A37" s="24"/>
       <c r="B37" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C37" s="30">
         <v>0.7</v>
@@ -3483,10 +3475,10 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="13.5" customHeight="1">
       <c r="A38" s="24"/>
       <c r="B38" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C38" s="30">
         <v>0.47</v>
@@ -3498,10 +3490,10 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="13.5" customHeight="1">
       <c r="A39" s="24"/>
       <c r="B39" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="30">
         <v>1.52</v>
@@ -3513,25 +3505,25 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="13.5" customHeight="1">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="13.5" customHeight="1">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="13.5" customHeight="1">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="13.5" customHeight="1">
       <c r="A43" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B43" s="24"/>
       <c r="C43" s="24"/>
       <c r="D43" s="24"/>
       <c r="E43" s="24"/>
     </row>
-    <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="13.5" customHeight="1">
       <c r="A44" s="24"/>
       <c r="B44" s="24"/>
       <c r="C44" s="27" t="s">
@@ -3544,10 +3536,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="13.5" customHeight="1">
       <c r="A45" s="24"/>
       <c r="B45" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C45" s="28">
         <v>3.5999999999999999E-3</v>
@@ -3559,10 +3551,10 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="13.5" customHeight="1">
       <c r="A46" s="24"/>
       <c r="B46" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C46" s="28">
         <v>3.5999999999999999E-3</v>
@@ -3574,10 +3566,10 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="13.5" customHeight="1">
       <c r="A47" s="24"/>
       <c r="B47" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C47" s="28">
         <v>5.7999999999999996E-3</v>
@@ -3589,10 +3581,10 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="13.5" customHeight="1">
       <c r="A48" s="24"/>
       <c r="B48" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C48" s="28">
         <v>8.8000000000000005E-3</v>
@@ -3604,10 +3596,10 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="13.5" customHeight="1">
       <c r="A49" s="24"/>
       <c r="B49" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C49" s="28">
         <v>5.8999999999999997E-2</v>
@@ -3619,10 +3611,10 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="13.5" customHeight="1">
       <c r="A50" s="24"/>
       <c r="B50" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C50" s="28">
         <v>0.32300000000000001</v>
@@ -3634,10 +3626,10 @@
         <v>0.432</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="13.5" customHeight="1">
       <c r="A51" s="24"/>
       <c r="B51" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C51" s="28">
         <v>0.23</v>
@@ -3649,10 +3641,10 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="13.5" customHeight="1">
       <c r="A52" s="24"/>
       <c r="B52" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C52" s="28">
         <v>2.17</v>
@@ -3664,25 +3656,25 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="13.5" customHeight="1">
       <c r="B53" s="3"/>
     </row>
-    <row r="54" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="13.5" customHeight="1">
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="13.5" customHeight="1">
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="13.5" customHeight="1">
       <c r="A56" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B56" s="24"/>
       <c r="C56" s="24"/>
       <c r="D56" s="24"/>
       <c r="E56" s="24"/>
     </row>
-    <row r="57" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="13.5" customHeight="1">
       <c r="A57" s="24"/>
       <c r="B57" s="24"/>
       <c r="C57" s="27" t="s">
@@ -3695,10 +3687,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="13.5" customHeight="1">
       <c r="A58" s="24"/>
       <c r="B58" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C58" s="30">
         <v>0.95</v>
@@ -3713,10 +3705,10 @@
       <c r="H58" s="23"/>
       <c r="I58" s="23"/>
     </row>
-    <row r="59" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="13.5" customHeight="1">
       <c r="A59" s="24"/>
       <c r="B59" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C59" s="30">
         <v>0.57999999999999996</v>
@@ -3731,10 +3723,10 @@
       <c r="H59" s="23"/>
       <c r="I59" s="23"/>
     </row>
-    <row r="60" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="13.5" customHeight="1">
       <c r="A60" s="24"/>
       <c r="B60" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C60" s="30">
         <v>0</v>
@@ -3749,10 +3741,10 @@
       <c r="H60" s="23"/>
       <c r="I60" s="23"/>
     </row>
-    <row r="61" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="13.5" customHeight="1">
       <c r="A61" s="24"/>
       <c r="B61" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C61" s="30">
         <v>2.65</v>
@@ -3767,10 +3759,10 @@
       <c r="H61" s="23"/>
       <c r="I61" s="23"/>
     </row>
-    <row r="62" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="13.5" customHeight="1">
       <c r="A62" s="24"/>
       <c r="B62" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C62" s="30">
         <v>0.54</v>
@@ -3785,10 +3777,10 @@
       <c r="H62" s="23"/>
       <c r="I62" s="23"/>
     </row>
-    <row r="63" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="13.5" customHeight="1">
       <c r="A63" s="24"/>
       <c r="B63" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C63" s="30">
         <v>0.9</v>
@@ -3803,10 +3795,10 @@
       <c r="H63" s="23"/>
       <c r="I63" s="23"/>
     </row>
-    <row r="64" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="13.5" customHeight="1">
       <c r="A64" s="24"/>
       <c r="B64" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C64" s="30">
         <v>0.73</v>
@@ -3821,10 +3813,10 @@
       <c r="H64" s="23"/>
       <c r="I64" s="23"/>
     </row>
-    <row r="65" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="13.5" customHeight="1">
       <c r="A65" s="24"/>
       <c r="B65" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C65" s="30">
         <v>0.5</v>
@@ -3839,10 +3831,10 @@
       <c r="H65" s="23"/>
       <c r="I65" s="23"/>
     </row>
-    <row r="66" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="13.5" customHeight="1">
       <c r="A66" s="24"/>
       <c r="B66" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C66" s="30">
         <v>0.92</v>
@@ -3854,21 +3846,21 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="13.5" customHeight="1">
       <c r="B67" s="3"/>
     </row>
-    <row r="68" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="13.5" customHeight="1"/>
+    <row r="69" spans="1:9" ht="13.5" customHeight="1"/>
+    <row r="70" spans="1:9" ht="13.5" customHeight="1">
       <c r="A70" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B70" s="24"/>
       <c r="C70" s="24"/>
       <c r="D70" s="24"/>
       <c r="E70" s="24"/>
     </row>
-    <row r="71" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="13.5" customHeight="1">
       <c r="A71" s="24"/>
       <c r="B71" s="24"/>
       <c r="C71" s="27" t="s">
@@ -3881,10 +3873,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="13.5" customHeight="1">
       <c r="A72" s="24"/>
       <c r="B72" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C72" s="29">
         <v>0.14599999999999999</v>
@@ -3896,10 +3888,10 @@
         <v>0.20499999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="13.5" customHeight="1">
       <c r="A73" s="24"/>
       <c r="B73" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C73" s="29">
         <v>8.0000000000000002E-3</v>
@@ -3911,10 +3903,10 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="13.5" customHeight="1">
       <c r="A74" s="24"/>
       <c r="B74" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C74" s="29">
         <v>0.02</v>
@@ -3926,10 +3918,10 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="13.5" customHeight="1">
       <c r="A75" s="24"/>
       <c r="B75" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C75" s="29">
         <v>7.0000000000000007E-2</v>
@@ -3941,10 +3933,10 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="13.5" customHeight="1">
       <c r="A76" s="24"/>
       <c r="B76" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C76" s="29">
         <v>0.26500000000000001</v>
@@ -3956,10 +3948,10 @@
         <v>0.47399999999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="15" customHeight="1">
       <c r="A77" s="24"/>
       <c r="B77" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C77" s="29">
         <v>0.54700000000000004</v>
@@ -3971,10 +3963,10 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="15" customHeight="1">
       <c r="A78" s="24"/>
       <c r="B78" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C78" s="29">
         <v>5.2999999999999999E-2</v>
@@ -4005,16 +3997,16 @@
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
-    <col min="5" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="1" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="5" max="6" width="8.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -4022,7 +4014,7 @@
       <c r="D1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="13.5" customHeight="1">
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4036,24 +4028,24 @@
         <v>5</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="I2" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" ht="13.5" customHeight="1">
       <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>8</v>
@@ -4077,12 +4069,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="13.5" customHeight="1">
       <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>11</v>
@@ -4106,47 +4098,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="13.5" customHeight="1">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="13.5" customHeight="1">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="13.5" customHeight="1">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="13.5" customHeight="1">
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="13.5" customHeight="1">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="13.5" customHeight="1">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="13.5" customHeight="1">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="13.5" customHeight="1">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="13.5" customHeight="1">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="G13" s="3"/>
@@ -4169,17 +4161,17 @@
       <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="26" width="8.85546875" customWidth="1"/>
+    <col min="1" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="13.5" customHeight="1">
       <c r="D2" s="5">
         <v>2000</v>
       </c>
@@ -4247,7 +4239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4281,7 +4273,7 @@
       </c>
       <c r="Z3" s="12"/>
     </row>
-    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4323,7 +4315,7 @@
       </c>
       <c r="Z4" s="12"/>
     </row>
-    <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="13.5" customHeight="1">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4357,8 +4349,8 @@
       </c>
       <c r="Z5" s="12"/>
     </row>
-    <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:26" ht="13.5" customHeight="1">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4392,7 +4384,7 @@
       </c>
       <c r="Z7" s="12"/>
     </row>
-    <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="13.5" customHeight="1">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4434,7 +4426,7 @@
       </c>
       <c r="Z8" s="12"/>
     </row>
-    <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="13.5" customHeight="1">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4468,7 +4460,7 @@
       </c>
       <c r="Z9" s="12"/>
     </row>
-    <row r="10" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:26" ht="13.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4488,17 +4480,17 @@
       <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="26" width="8.85546875" customWidth="1"/>
+    <col min="1" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="13.5" customHeight="1">
       <c r="D2" s="7">
         <v>2000</v>
       </c>
@@ -4566,7 +4558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4600,7 +4592,7 @@
       </c>
       <c r="Z3" s="10"/>
     </row>
-    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4640,7 +4632,7 @@
       </c>
       <c r="Z4" s="14"/>
     </row>
-    <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="13.5" customHeight="1">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4674,8 +4666,8 @@
       </c>
       <c r="Z5" s="10"/>
     </row>
-    <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:26" ht="13.5" customHeight="1">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4709,7 +4701,7 @@
       </c>
       <c r="Z7" s="10"/>
     </row>
-    <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="13.5" customHeight="1">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4749,7 +4741,7 @@
       </c>
       <c r="Z8" s="10"/>
     </row>
-    <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="13.5" customHeight="1">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4803,17 +4795,17 @@
       <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="25" width="8.85546875" customWidth="1"/>
+    <col min="1" max="25" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -4881,7 +4873,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4916,7 +4908,7 @@
       </c>
       <c r="Y3" s="10"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4951,15 +4943,15 @@
       </c>
       <c r="Y4" s="10"/>
     </row>
-    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="8" spans="1:25" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -5027,7 +5019,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5060,7 +5052,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5093,15 +5085,15 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="13" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="14" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="15" spans="1:25" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -5169,7 +5161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:25" ht="13.5" customHeight="1">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5202,7 +5194,7 @@
       </c>
       <c r="Y17" s="10"/>
     </row>
-    <row r="18" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:25" ht="13.5" customHeight="1">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5251,21 +5243,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y41"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AA31" sqref="AA31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="25" width="8.85546875" customWidth="1"/>
+    <col min="1" max="25" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -5333,7 +5325,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5366,7 +5358,7 @@
       </c>
       <c r="Y3" s="15"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5399,15 +5391,15 @@
       </c>
       <c r="Y4" s="15"/>
     </row>
-    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="8" spans="1:25" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -5475,7 +5467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1">
       <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
@@ -5507,15 +5499,15 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="12" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="13" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="14" spans="1:25" ht="13.5" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="13.5" customHeight="1">
       <c r="C15" s="5">
         <v>2000</v>
       </c>
@@ -5583,7 +5575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
@@ -5623,15 +5615,15 @@
       </c>
       <c r="Y16" s="6"/>
     </row>
-    <row r="17" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="18" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="19" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="20" spans="1:25" ht="13.5" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="13.5" customHeight="1">
       <c r="C21" s="5">
         <v>2000</v>
       </c>
@@ -5699,7 +5691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="13.5" customHeight="1">
       <c r="B22" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5732,7 +5724,7 @@
       </c>
       <c r="Y22" s="15"/>
     </row>
-    <row r="23" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="13.5" customHeight="1">
       <c r="B23" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5765,15 +5757,15 @@
       </c>
       <c r="Y23" s="15"/>
     </row>
-    <row r="24" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="25" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="26" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="27" spans="1:25" ht="13.5" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="13.5" customHeight="1">
       <c r="C28" s="5">
         <v>2000</v>
       </c>
@@ -5841,7 +5833,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="B29" s="5" t="s">
         <v>14</v>
       </c>
@@ -5854,21 +5846,13 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
-      <c r="L29" s="10">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="M29" s="10">
-        <v>0.82099999999999995</v>
-      </c>
-      <c r="N29" s="10">
-        <v>0.82299999999999995</v>
-      </c>
-      <c r="O29" s="10">
-        <v>0.85799999999999998</v>
-      </c>
-      <c r="P29" s="10">
-        <v>0.86</v>
-      </c>
+      <c r="L29" s="6">
+        <v>200</v>
+      </c>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
       <c r="S29" s="6"/>
@@ -5881,15 +5865,15 @@
       </c>
       <c r="Y29" s="6"/>
     </row>
-    <row r="30" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="31" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="32" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="33" spans="1:25" ht="13.5" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" ht="13.5" customHeight="1">
       <c r="C34" s="5">
         <v>2000</v>
       </c>
@@ -5957,7 +5941,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" ht="13.5" customHeight="1">
       <c r="B35" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -6014,15 +5998,15 @@
       </c>
       <c r="Y35" s="9"/>
     </row>
-    <row r="36" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="37" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="38" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="39" spans="1:25" ht="13.5" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" ht="13.5" customHeight="1">
       <c r="C40" s="5">
         <v>2000</v>
       </c>
@@ -6090,7 +6074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" ht="13.5" customHeight="1">
       <c r="B41" s="5" t="s">
         <v>14</v>
       </c>
@@ -6125,6 +6109,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
@@ -6139,21 +6124,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="25" width="8.85546875" customWidth="1"/>
+    <col min="1" max="25" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -6221,7 +6206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -6251,15 +6236,15 @@
       </c>
       <c r="Y3" s="9"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="5" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="13.5" customHeight="1">
       <c r="C8" s="5">
         <v>2000</v>
       </c>
@@ -6327,7 +6312,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
@@ -6357,15 +6342,15 @@
       </c>
       <c r="Y9" s="9"/>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="11" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="12" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="13" spans="1:25" ht="13.5" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="13.5" customHeight="1">
       <c r="C14" s="5">
         <v>2000</v>
       </c>
@@ -6433,7 +6418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="13.5" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
@@ -6463,15 +6448,15 @@
       </c>
       <c r="Y15" s="9"/>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="17" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="18" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="19" spans="1:25" ht="13.5" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="13.5" customHeight="1">
       <c r="C20" s="5">
         <v>2000</v>
       </c>
@@ -6539,7 +6524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="13.5" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
@@ -6569,15 +6554,15 @@
       </c>
       <c r="Y21" s="9"/>
     </row>
-    <row r="22" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="23" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="24" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="25" spans="1:25" ht="13.5" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" ht="13.5" customHeight="1">
       <c r="C26" s="7">
         <v>2000</v>
       </c>
@@ -6645,7 +6630,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="13.5" customHeight="1">
       <c r="B27" s="7" t="s">
         <v>14</v>
       </c>
@@ -6675,15 +6660,15 @@
       </c>
       <c r="Y27" s="9"/>
     </row>
-    <row r="28" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="29" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="30" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="C32" s="5">
         <v>2000</v>
       </c>
@@ -6751,7 +6736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" ht="13.5" customHeight="1">
       <c r="B33" s="5" t="s">
         <v>14</v>
       </c>
@@ -6781,15 +6766,15 @@
       </c>
       <c r="Y33" s="9"/>
     </row>
-    <row r="34" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="35" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="36" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="37" spans="1:25" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="13.5" customHeight="1">
       <c r="C38" s="5">
         <v>2000</v>
       </c>
@@ -6857,7 +6842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="13.5" customHeight="1">
       <c r="B39" s="5" t="s">
         <v>14</v>
       </c>
@@ -6887,9 +6872,9 @@
       </c>
       <c r="Y39" s="9"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" ht="14">
       <c r="A43" s="34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B43" s="31"/>
       <c r="C43" s="31"/>
@@ -6916,7 +6901,7 @@
       <c r="X43" s="31"/>
       <c r="Y43" s="31"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" ht="14">
       <c r="A44" s="31"/>
       <c r="B44" s="31"/>
       <c r="C44" s="35">
@@ -6987,7 +6972,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" ht="14">
       <c r="A45" s="31"/>
       <c r="B45" s="35" t="s">
         <v>30</v>
@@ -7018,12 +7003,12 @@
       </c>
       <c r="Y45" s="37"/>
     </row>
-    <row r="46" spans="1:25" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:25" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:25" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" ht="12"/>
+    <row r="47" spans="1:25" ht="12"/>
+    <row r="48" spans="1:25" ht="12"/>
+    <row r="49" spans="1:25" ht="14">
       <c r="A49" s="40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B49" s="31"/>
       <c r="C49" s="31"/>
@@ -7050,7 +7035,7 @@
       <c r="X49" s="31"/>
       <c r="Y49" s="31"/>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" ht="14">
       <c r="A50" s="31"/>
       <c r="B50" s="31"/>
       <c r="C50" s="35">
@@ -7121,7 +7106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" ht="14">
       <c r="A51" s="31"/>
       <c r="B51" s="35" t="s">
         <v>30</v>
@@ -7152,12 +7137,12 @@
       </c>
       <c r="Y51" s="37"/>
     </row>
-    <row r="52" spans="1:25" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="1:25" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:25" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" ht="12"/>
+    <row r="53" spans="1:25" ht="12"/>
+    <row r="54" spans="1:25" ht="12"/>
+    <row r="55" spans="1:25" ht="15" customHeight="1">
       <c r="A55" s="40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B55" s="31"/>
       <c r="C55" s="31"/>
@@ -7184,7 +7169,7 @@
       <c r="X55" s="31"/>
       <c r="Y55" s="31"/>
     </row>
-    <row r="56" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" ht="15" customHeight="1">
       <c r="A56" s="31"/>
       <c r="B56" s="31"/>
       <c r="C56" s="35">
@@ -7255,7 +7240,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" ht="15" customHeight="1">
       <c r="A57" s="31"/>
       <c r="B57" s="35" t="s">
         <v>30</v>
@@ -7305,11 +7290,11 @@
       <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="14">
       <c r="A1" s="34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -7336,7 +7321,7 @@
       <c r="X1" s="31"/>
       <c r="Y1" s="31"/>
     </row>
-    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="14">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="35">
@@ -7407,10 +7392,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="14">
       <c r="A3" s="31"/>
       <c r="B3" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" s="33"/>
       <c r="D3" s="33"/>
@@ -7440,10 +7425,10 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="14">
       <c r="A4" s="31"/>
       <c r="B4" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -7473,9 +7458,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="14">
       <c r="A8" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" s="31"/>
       <c r="C8" s="31"/>
@@ -7502,7 +7487,7 @@
       <c r="X8" s="31"/>
       <c r="Y8" s="31"/>
     </row>
-    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="14">
       <c r="A9" s="31"/>
       <c r="B9" s="31"/>
       <c r="C9" s="35">
@@ -7573,10 +7558,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="14">
       <c r="A10" s="31"/>
       <c r="B10" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
@@ -7606,10 +7591,10 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="14">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
@@ -7639,9 +7624,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="14">
       <c r="A15" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
@@ -7668,7 +7653,7 @@
       <c r="X15" s="31"/>
       <c r="Y15" s="31"/>
     </row>
-    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="14">
       <c r="A16" s="31"/>
       <c r="B16" s="31"/>
       <c r="C16" s="35">
@@ -7739,10 +7724,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="14">
       <c r="A17" s="31"/>
       <c r="B17" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
@@ -7772,10 +7757,10 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="14">
       <c r="A18" s="31"/>
       <c r="B18" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
@@ -7805,9 +7790,9 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="14">
       <c r="A22" s="34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B22" s="31"/>
       <c r="C22" s="31"/>
@@ -7834,7 +7819,7 @@
       <c r="X22" s="31"/>
       <c r="Y22" s="31"/>
     </row>
-    <row r="23" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="14">
       <c r="A23" s="31"/>
       <c r="B23" s="31"/>
       <c r="C23" s="35">
@@ -7905,10 +7890,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="14">
       <c r="A24" s="31"/>
       <c r="B24" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
@@ -7938,10 +7923,10 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="14">
       <c r="A25" s="31"/>
       <c r="B25" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="33"/>
       <c r="D25" s="33"/>
@@ -7971,9 +7956,9 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="14">
       <c r="A29" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B29" s="31"/>
       <c r="C29" s="31"/>
@@ -8000,7 +7985,7 @@
       <c r="X29" s="31"/>
       <c r="Y29" s="31"/>
     </row>
-    <row r="30" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="14">
       <c r="A30" s="31"/>
       <c r="B30" s="31"/>
       <c r="C30" s="35">
@@ -8071,7 +8056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="14">
       <c r="A31" s="31"/>
       <c r="B31" s="35" t="s">
         <v>30</v>
@@ -8104,9 +8089,9 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" ht="14">
       <c r="A35" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B35" s="31"/>
       <c r="C35" s="31"/>
@@ -8133,7 +8118,7 @@
       <c r="X35" s="31"/>
       <c r="Y35" s="31"/>
     </row>
-    <row r="36" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" ht="14">
       <c r="A36" s="31"/>
       <c r="B36" s="31"/>
       <c r="C36" s="35">
@@ -8204,7 +8189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" ht="14">
       <c r="A37" s="31"/>
       <c r="B37" s="35" t="s">
         <v>30</v>
@@ -8237,9 +8222,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" ht="14">
       <c r="A41" s="34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B41" s="31"/>
       <c r="C41" s="31"/>
@@ -8266,7 +8251,7 @@
       <c r="X41" s="31"/>
       <c r="Y41" s="31"/>
     </row>
-    <row r="42" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" ht="14">
       <c r="A42" s="31"/>
       <c r="B42" s="31"/>
       <c r="C42" s="35">
@@ -8337,7 +8322,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" ht="14">
       <c r="A43" s="31"/>
       <c r="B43" s="35" t="s">
         <v>30</v>
@@ -8370,9 +8355,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" ht="14">
       <c r="A47" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B47" s="31"/>
       <c r="C47" s="31"/>
@@ -8399,7 +8384,7 @@
       <c r="X47" s="31"/>
       <c r="Y47" s="31"/>
     </row>
-    <row r="48" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" ht="14">
       <c r="A48" s="31"/>
       <c r="B48" s="31"/>
       <c r="C48" s="35">
@@ -8470,7 +8455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" ht="14">
       <c r="A49" s="31"/>
       <c r="B49" s="35" t="s">
         <v>30</v>
@@ -8503,9 +8488,9 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" ht="14">
       <c r="A53" s="34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B53" s="31"/>
       <c r="C53" s="31"/>
@@ -8532,7 +8517,7 @@
       <c r="X53" s="31"/>
       <c r="Y53" s="31"/>
     </row>
-    <row r="54" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" ht="14">
       <c r="A54" s="31"/>
       <c r="B54" s="31"/>
       <c r="C54" s="35">
@@ -8603,7 +8588,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" ht="14">
       <c r="A55" s="31"/>
       <c r="B55" s="35" t="s">
         <v>30</v>
@@ -8636,9 +8621,9 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="59" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" ht="14">
       <c r="A59" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B59" s="31"/>
       <c r="C59" s="31"/>
@@ -8665,7 +8650,7 @@
       <c r="X59" s="31"/>
       <c r="Y59" s="31"/>
     </row>
-    <row r="60" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" ht="14">
       <c r="A60" s="31"/>
       <c r="B60" s="31"/>
       <c r="C60" s="35">
@@ -8736,7 +8721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" ht="14">
       <c r="A61" s="31"/>
       <c r="B61" s="35" t="s">
         <v>30</v>
@@ -8788,17 +8773,17 @@
       <selection activeCell="AA53" sqref="AA53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="25" width="8.85546875" customWidth="1"/>
+    <col min="1" max="25" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -8866,7 +8851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -8899,7 +8884,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -8932,15 +8917,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="8" spans="1:25" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -9008,7 +8993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9042,7 +9027,7 @@
         <v>12.000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9076,15 +9061,15 @@
         <v>6.0000000000000009</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="13" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="14" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="15" spans="1:25" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="13.5" customHeight="1">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -9152,7 +9137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="13.5" customHeight="1">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9185,7 +9170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="13.5" customHeight="1">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9218,15 +9203,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="20" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="21" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="22" spans="1:25" ht="13.5" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="13.5" customHeight="1">
       <c r="C23" s="5">
         <v>2000</v>
       </c>
@@ -9294,7 +9279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="13.5" customHeight="1">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9327,7 +9312,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="13.5" customHeight="1">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9360,15 +9345,15 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="27" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="28" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" ht="13.5" customHeight="1">
       <c r="C30" s="5">
         <v>2000</v>
       </c>
@@ -9436,7 +9421,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="B31" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9469,7 +9454,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="B32" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9502,15 +9487,15 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="34" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="35" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="36" spans="1:25" ht="13.5" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" ht="13.5" customHeight="1">
       <c r="C37" s="5">
         <v>2000</v>
       </c>
@@ -9578,7 +9563,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="13.5" customHeight="1">
       <c r="B38" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9611,7 +9596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="13.5" customHeight="1">
       <c r="B39" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9644,15 +9629,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="41" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="42" spans="1:25" ht="13.5" customHeight="1"/>
+    <row r="43" spans="1:25" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" ht="13.5" customHeight="1">
       <c r="C44" s="5">
         <v>2000</v>
       </c>
@@ -9720,7 +9705,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" ht="13.5" customHeight="1">
       <c r="B45" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>

</xml_diff>

<commit_message>
add propsupp to Optional Indicators
</commit_message>
<xml_diff>
--- a/tests/simple.xlsx
+++ b/tests/simple.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="121">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>PLHIV in care on treatment (%)</t>
+  </si>
+  <si>
+    <t>People on ART with viral suppression (%)</t>
   </si>
   <si>
     <t>Linkage to care from diagnosis within 1 month (%)</t>
@@ -868,15 +871,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -885,8 +888,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="7124040"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="7123680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -913,15 +916,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -930,8 +933,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="7124040"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="7123680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -958,15 +961,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -975,8 +978,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="7124040"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="7123680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1003,15 +1006,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1020,8 +1023,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="7124040"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="7123680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1048,15 +1051,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1065,8 +1068,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="7124040"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="7123680"/>
         </a:xfrm>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
@@ -1095,15 +1098,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1112,8 +1115,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="7314480"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="7314120"/>
         </a:xfrm>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
@@ -1142,15 +1145,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1159,8 +1162,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="8438400"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="8438040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1187,15 +1190,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1204,8 +1207,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="8438400"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="8438040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1232,15 +1235,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1249,8 +1252,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="8438400"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="8438040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1277,15 +1280,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1294,8 +1297,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="8438400"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="8438040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1322,15 +1325,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1339,8 +1342,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="9771840"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="9771480"/>
         </a:xfrm>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
@@ -1369,15 +1372,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>84600</xdr:rowOff>
+      <xdr:rowOff>84240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1386,8 +1389,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="8000280"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="7999920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1414,15 +1417,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>84600</xdr:rowOff>
+      <xdr:rowOff>84240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1431,8 +1434,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="8000280"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="7999920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1459,15 +1462,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>84600</xdr:rowOff>
+      <xdr:rowOff>84240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1476,8 +1479,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="8000280"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="7999920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1504,15 +1507,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>84600</xdr:rowOff>
+      <xdr:rowOff>84240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1521,8 +1524,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="8000280"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="7999920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1549,15 +1552,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>186480</xdr:rowOff>
+      <xdr:rowOff>186120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1566,8 +1569,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="10286640"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="10286280"/>
         </a:xfrm>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
@@ -1596,15 +1599,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1613,8 +1616,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="9810000"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="9809640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1641,15 +1644,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1658,8 +1661,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="9810000"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="9809640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1686,15 +1689,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1703,8 +1706,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="9810000"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="9809640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1731,15 +1734,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1748,8 +1751,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="9810000"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="9809640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1776,15 +1779,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1793,8 +1796,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="11728800" cy="9810000"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="12632760" cy="9809640"/>
         </a:xfrm>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
@@ -1831,8 +1834,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="104.474489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="112.841836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1889,12 +1892,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="25" min="1" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="1" style="0" width="11.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.16836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2033,7 +2037,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2172,7 +2176,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2299,14 +2303,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.3214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="14.6785714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.8316326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.16836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2353,7 +2358,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2400,7 +2405,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -2445,7 +2450,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -2478,7 +2483,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -2503,7 +2508,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -2536,7 +2541,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -2591,14 +2596,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.3622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.1428571428572"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2614,7 +2619,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="29" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C3" s="30" t="n">
         <v>0.0004</v>
@@ -2628,7 +2633,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C4" s="30" t="n">
         <v>0.0008</v>
@@ -2642,7 +2647,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C5" s="30" t="n">
         <v>0.0138</v>
@@ -2656,7 +2661,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C6" s="30" t="n">
         <v>0.0011</v>
@@ -2670,7 +2675,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C7" s="30" t="n">
         <v>0.008</v>
@@ -2684,7 +2689,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C8" s="30" t="n">
         <v>0.367</v>
@@ -2698,7 +2703,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C9" s="30" t="n">
         <v>0.205</v>
@@ -2721,7 +2726,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2737,7 +2742,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C15" s="22" t="n">
         <v>26.03</v>
@@ -2751,7 +2756,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C16" s="22" t="n">
         <v>1</v>
@@ -2765,7 +2770,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C17" s="22" t="n">
         <v>1</v>
@@ -2779,7 +2784,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="29" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C18" s="22" t="n">
         <v>1</v>
@@ -2793,7 +2798,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C19" s="22" t="n">
         <v>3.49</v>
@@ -2807,7 +2812,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C20" s="22" t="n">
         <v>7.17</v>
@@ -2830,7 +2835,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2846,7 +2851,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C26" s="20" t="n">
         <v>4.14</v>
@@ -2860,7 +2865,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C27" s="20" t="n">
         <v>1.05</v>
@@ -2874,7 +2879,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C28" s="20" t="n">
         <v>0.33</v>
@@ -2888,7 +2893,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C29" s="20" t="n">
         <v>0.27</v>
@@ -2902,7 +2907,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C30" s="20" t="n">
         <v>0.67</v>
@@ -2925,7 +2930,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2941,7 +2946,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="29" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C36" s="20" t="n">
         <v>0.45</v>
@@ -2955,7 +2960,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C37" s="20" t="n">
         <v>0.7</v>
@@ -2969,7 +2974,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="29" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C38" s="20" t="n">
         <v>0.47</v>
@@ -2983,7 +2988,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C39" s="20" t="n">
         <v>1.52</v>
@@ -3006,7 +3011,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3022,7 +3027,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C45" s="30" t="n">
         <v>0.0036</v>
@@ -3036,7 +3041,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C46" s="30" t="n">
         <v>0.0036</v>
@@ -3050,7 +3055,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C47" s="30" t="n">
         <v>0.0058</v>
@@ -3064,7 +3069,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="29" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C48" s="30" t="n">
         <v>0.0088</v>
@@ -3078,7 +3083,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C49" s="30" t="n">
         <v>0.059</v>
@@ -3092,7 +3097,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C50" s="30" t="n">
         <v>0.323</v>
@@ -3106,7 +3111,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="29" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C51" s="30" t="n">
         <v>0.23</v>
@@ -3120,7 +3125,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C52" s="30" t="n">
         <v>2.17</v>
@@ -3143,7 +3148,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3159,7 +3164,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="29" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C58" s="20" t="n">
         <v>0.95</v>
@@ -3176,7 +3181,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="29" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C59" s="20" t="n">
         <v>0.58</v>
@@ -3193,7 +3198,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="29" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C60" s="20" t="n">
         <v>0</v>
@@ -3210,7 +3215,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="29" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C61" s="20" t="n">
         <v>2.65</v>
@@ -3227,7 +3232,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="29" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C62" s="20" t="n">
         <v>0.54</v>
@@ -3244,7 +3249,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B63" s="29" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C63" s="20" t="n">
         <v>0.9</v>
@@ -3261,7 +3266,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B64" s="29" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C64" s="20" t="n">
         <v>0.73</v>
@@ -3278,7 +3283,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="29" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C65" s="20" t="n">
         <v>0.5</v>
@@ -3295,7 +3300,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B66" s="29" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C66" s="20" t="n">
         <v>0.92</v>
@@ -3312,7 +3317,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="18" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3328,7 +3333,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B72" s="29" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C72" s="22" t="n">
         <v>0.146</v>
@@ -3342,7 +3347,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B73" s="29" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C73" s="22" t="n">
         <v>0.008</v>
@@ -3356,7 +3361,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B74" s="29" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C74" s="22" t="n">
         <v>0.02</v>
@@ -3370,7 +3375,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B75" s="29" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C75" s="22" t="n">
         <v>0.07</v>
@@ -3384,7 +3389,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B76" s="29" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C76" s="22" t="n">
         <v>0.265</v>
@@ -3398,7 +3403,7 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="29" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C77" s="22" t="n">
         <v>0.547</v>
@@ -3412,7 +3417,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C78" s="22" t="n">
         <v>0.053</v>
@@ -3448,11 +3453,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.3214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.3622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.3214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.1428571428572"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.1224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.16836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3571,7 +3577,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="26" min="1" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="26" min="1" style="0" width="11.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="9.16836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3892,7 +3899,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="26" min="1" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="26" min="1" style="0" width="11.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="9.16836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4209,7 +4217,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="25" min="1" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="1" style="0" width="11.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.16836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4659,7 +4668,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="25" min="1" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="1" style="0" width="11.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.16836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5625,15 +5635,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y65536"/>
+  <dimension ref="A1:AI65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J61" activeCellId="0" sqref="J61"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J63" activeCellId="0" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="25" min="1" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="1" style="0" width="11.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.16836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6669,6 +6680,155 @@
       </c>
       <c r="Y57" s="20"/>
     </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C62" s="19" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D62" s="19" t="n">
+        <v>2001</v>
+      </c>
+      <c r="E62" s="19" t="n">
+        <v>2002</v>
+      </c>
+      <c r="F62" s="19" t="n">
+        <v>2003</v>
+      </c>
+      <c r="G62" s="19" t="n">
+        <v>2004</v>
+      </c>
+      <c r="H62" s="19" t="n">
+        <v>2005</v>
+      </c>
+      <c r="I62" s="19" t="n">
+        <v>2006</v>
+      </c>
+      <c r="J62" s="19" t="n">
+        <v>2007</v>
+      </c>
+      <c r="K62" s="19" t="n">
+        <v>2008</v>
+      </c>
+      <c r="L62" s="19" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M62" s="19" t="n">
+        <v>2010</v>
+      </c>
+      <c r="N62" s="19" t="n">
+        <v>2011</v>
+      </c>
+      <c r="O62" s="19" t="n">
+        <v>2012</v>
+      </c>
+      <c r="P62" s="19" t="n">
+        <v>2013</v>
+      </c>
+      <c r="Q62" s="19" t="n">
+        <v>2014</v>
+      </c>
+      <c r="R62" s="19" t="n">
+        <v>2015</v>
+      </c>
+      <c r="S62" s="19" t="n">
+        <v>2016</v>
+      </c>
+      <c r="T62" s="19" t="n">
+        <v>2017</v>
+      </c>
+      <c r="U62" s="19" t="n">
+        <v>2018</v>
+      </c>
+      <c r="V62" s="19" t="n">
+        <v>2019</v>
+      </c>
+      <c r="W62" s="19" t="n">
+        <v>2020</v>
+      </c>
+      <c r="X62" s="19" t="n">
+        <v>2021</v>
+      </c>
+      <c r="Y62" s="19" t="n">
+        <v>2022</v>
+      </c>
+      <c r="Z62" s="19" t="n">
+        <v>2023</v>
+      </c>
+      <c r="AA62" s="19" t="n">
+        <v>2024</v>
+      </c>
+      <c r="AB62" s="19" t="n">
+        <v>2025</v>
+      </c>
+      <c r="AC62" s="19" t="n">
+        <v>2026</v>
+      </c>
+      <c r="AD62" s="19" t="n">
+        <v>2027</v>
+      </c>
+      <c r="AE62" s="19" t="n">
+        <v>2028</v>
+      </c>
+      <c r="AF62" s="19" t="n">
+        <v>2029</v>
+      </c>
+      <c r="AG62" s="19" t="n">
+        <v>2030</v>
+      </c>
+      <c r="AI62" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="20"/>
+      <c r="I63" s="20"/>
+      <c r="J63" s="20"/>
+      <c r="K63" s="20"/>
+      <c r="L63" s="20"/>
+      <c r="M63" s="20"/>
+      <c r="N63" s="20"/>
+      <c r="O63" s="20"/>
+      <c r="P63" s="20"/>
+      <c r="Q63" s="20"/>
+      <c r="R63" s="20"/>
+      <c r="S63" s="20"/>
+      <c r="T63" s="20"/>
+      <c r="U63" s="20"/>
+      <c r="V63" s="20"/>
+      <c r="W63" s="20"/>
+      <c r="X63" s="20"/>
+      <c r="Y63" s="20"/>
+      <c r="Z63" s="20"/>
+      <c r="AA63" s="20"/>
+      <c r="AB63" s="20"/>
+      <c r="AC63" s="20"/>
+      <c r="AD63" s="20"/>
+      <c r="AE63" s="20"/>
+      <c r="AF63" s="20"/>
+      <c r="AG63" s="20"/>
+      <c r="AH63" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI63" s="20" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6688,18 +6848,18 @@
   </sheetPr>
   <dimension ref="A1:Y65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6836,7 +6996,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6973,7 +7133,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7110,7 +7270,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7248,7 +7408,7 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7353,7 +7513,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7458,7 +7618,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7604,12 +7764,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="25" min="1" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="1" style="0" width="11.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.16836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7748,7 +7909,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7889,7 +8050,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8028,7 +8189,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8167,7 +8328,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8306,7 +8467,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8445,7 +8606,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8551,7 +8712,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
changes spreadsheets and pars but problem with pars
</commit_message>
<xml_diff>
--- a/tests/simple.xlsx
+++ b/tests/simple.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="988" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23760" windowHeight="11360" tabRatio="988" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,12 @@
     <sheet name="Partnerships &amp; transitions" sheetId="11" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -128,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="124">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -277,12 +282,6 @@
     <t>People on ART with viral suppression (%)</t>
   </si>
   <si>
-    <t>Linkage to care from diagnosis within 1 month (%)</t>
-  </si>
-  <si>
-    <t>Linkage to care rate (%/year)</t>
-  </si>
-  <si>
     <t>Percentage of people who receive ART in the year who stop taking ART (%/year)</t>
   </si>
   <si>
@@ -503,6 +502,9 @@
   </si>
   <si>
     <t>People lost to follow up who are still in care (%)</t>
+  </si>
+  <si>
+    <t>Average time taken to be linked to care (years)</t>
   </si>
 </sst>
 </file>
@@ -515,7 +517,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -627,6 +629,22 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -708,7 +726,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="126">
+  <cellStyleXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -835,8 +853,10 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -934,12 +954,15 @@
     <xf numFmtId="10" fontId="4" fillId="6" borderId="1" xfId="117" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="4" fontId="16" fillId="9" borderId="1" xfId="121" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="16" fillId="9" borderId="1" xfId="121" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="126">
+  <cellStyles count="128">
     <cellStyle name="Comma 2" xfId="2"/>
     <cellStyle name="Comma 2 2" xfId="118"/>
     <cellStyle name="Comma 2 3" xfId="11"/>
@@ -950,6 +973,7 @@
     <cellStyle name="Comma 5" xfId="111"/>
     <cellStyle name="Explanatory Text 2" xfId="4"/>
     <cellStyle name="Explanatory Text 3" xfId="115"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="22"/>
     <cellStyle name="Followed Hyperlink 11" xfId="23"/>
     <cellStyle name="Followed Hyperlink 12" xfId="24"/>
@@ -1047,6 +1071,7 @@
     <cellStyle name="Followed Hyperlink 96" xfId="108"/>
     <cellStyle name="Followed Hyperlink 97" xfId="109"/>
     <cellStyle name="Followed Hyperlink 98" xfId="110"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Normal 2 2" xfId="116"/>
@@ -2922,39 +2947,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="121.85546875"/>
-    <col min="2" max="1025" width="11.85546875"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:1" ht="12.75" customHeight="1">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="53"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="53"/>
-    </row>
-    <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
+      <c r="A2" s="55"/>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="55"/>
+    </row>
+    <row r="4" spans="1:1" ht="14">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="67.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="14">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="140">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -2965,6 +2986,11 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2972,21 +2998,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="25" width="11.85546875"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -3054,7 +3077,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3087,7 +3110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3120,12 +3143,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -3193,7 +3216,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1">
       <c r="B10" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3226,7 +3249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1">
       <c r="B11" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3259,12 +3282,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="13.5" customHeight="1">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -3332,7 +3355,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:25" ht="13.5" customHeight="1">
       <c r="B17" s="5" t="s">
         <v>32</v>
       </c>
@@ -3367,6 +3390,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3374,25 +3402,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="11.85546875"/>
-    <col min="3" max="4" width="17.140625"/>
-    <col min="5" max="6" width="11.85546875"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13.5" customHeight="1">
       <c r="C2" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3402,7 +3425,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13.5" customHeight="1">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3412,7 +3435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="13.5" customHeight="1">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3420,26 +3443,26 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13.5" customHeight="1">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="13.5" customHeight="1">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="13.5" customHeight="1">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="13.5" customHeight="1">
       <c r="C9" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3449,7 +3472,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="13.5" customHeight="1">
       <c r="B10" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3459,7 +3482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="13.5" customHeight="1">
       <c r="B11" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3467,26 +3490,26 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="13.5" customHeight="1">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="13.5" customHeight="1">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="13.5" customHeight="1">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="13.5" customHeight="1">
       <c r="C16" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3496,7 +3519,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="13.5" customHeight="1">
       <c r="B17" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3504,7 +3527,7 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="13.5" customHeight="1">
       <c r="B18" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3512,26 +3535,26 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="13.5" customHeight="1">
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="13.5" customHeight="1">
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="13.5" customHeight="1">
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="13.5" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="13.5" customHeight="1">
       <c r="C23" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3541,7 +3564,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="13.5" customHeight="1">
       <c r="B24" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3549,7 +3572,7 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="13.5" customHeight="1">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3557,14 +3580,14 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="13.5" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="13.5" customHeight="1">
       <c r="C30" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3574,7 +3597,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="13.5" customHeight="1">
       <c r="B31" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3582,14 +3605,14 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="35" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="13.5" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="13.5" customHeight="1">
       <c r="C36" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3599,7 +3622,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="13.5" customHeight="1">
       <c r="B37" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3607,7 +3630,7 @@
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="13.5" customHeight="1">
       <c r="B38" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3615,14 +3638,14 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="42" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="13.5" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="13.5" customHeight="1">
       <c r="C43" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3632,7 +3655,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="13.5" customHeight="1">
       <c r="B44" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3640,7 +3663,7 @@
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="13.5" customHeight="1">
       <c r="B45" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3651,6 +3674,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3658,28 +3686,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15:E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="43"/>
-    <col min="2" max="2" width="55.140625" style="43"/>
-    <col min="3" max="1025" width="11.85546875" style="43"/>
-    <col min="1026" max="16384" width="9.140625" style="43"/>
+    <col min="1" max="16384" width="8.83203125" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="13.5" customHeight="1">
       <c r="A1" s="50" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
       <c r="D1" s="48"/>
       <c r="E1" s="48"/>
     </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.5" customHeight="1">
       <c r="A2" s="48"/>
       <c r="B2" s="48"/>
       <c r="C2" s="49" t="s">
@@ -3692,10 +3717,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.5" customHeight="1">
       <c r="A3" s="48"/>
       <c r="B3" s="51" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C3" s="52">
         <v>4.0000000000000002E-4</v>
@@ -3707,10 +3732,10 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.5" customHeight="1">
       <c r="A4" s="48"/>
       <c r="B4" s="51" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" s="52">
         <v>8.0000000000000004E-4</v>
@@ -3722,10 +3747,10 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.5" customHeight="1">
       <c r="A5" s="48"/>
       <c r="B5" s="51" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5" s="52">
         <v>1.1000000000000001E-3</v>
@@ -3737,10 +3762,10 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.5" customHeight="1">
       <c r="A6" s="48"/>
       <c r="B6" s="51" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" s="52">
         <v>1.38E-2</v>
@@ -3752,10 +3777,10 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.5" customHeight="1">
       <c r="A7" s="48"/>
       <c r="B7" s="51" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="52">
         <v>8.0000000000000002E-3</v>
@@ -3767,10 +3792,10 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.5" customHeight="1">
       <c r="A8" s="48"/>
       <c r="B8" s="51" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C8" s="52">
         <v>0.36699999999999999</v>
@@ -3782,10 +3807,10 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.5" customHeight="1">
       <c r="A9" s="48"/>
       <c r="B9" s="51" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C9" s="52">
         <v>0.20499999999999999</v>
@@ -3797,21 +3822,21 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.5" customHeight="1">
       <c r="B10" s="41"/>
     </row>
-    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="13.5" customHeight="1">
       <c r="B11" s="41"/>
     </row>
-    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="13.5" customHeight="1">
       <c r="B12" s="41"/>
     </row>
-    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="13.5" customHeight="1">
       <c r="A13" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="13.5" customHeight="1">
       <c r="C14" s="39" t="s">
         <v>22</v>
       </c>
@@ -3822,23 +3847,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="13.5" customHeight="1">
       <c r="B15" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" s="54">
+        <v>81</v>
+      </c>
+      <c r="C15" s="53">
         <v>5.6</v>
       </c>
-      <c r="D15" s="54">
+      <c r="D15" s="53">
         <v>3.3</v>
       </c>
-      <c r="E15" s="54">
+      <c r="E15" s="53">
         <v>9.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="13.5" customHeight="1">
       <c r="B16" s="40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C16" s="45">
         <v>1</v>
@@ -3850,9 +3875,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="13.5" customHeight="1">
       <c r="B17" s="40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C17" s="45">
         <v>1</v>
@@ -3864,9 +3889,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="13.5" customHeight="1">
       <c r="B18" s="40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C18" s="45">
         <v>1</v>
@@ -3878,9 +3903,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="13.5" customHeight="1">
       <c r="B19" s="40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C19" s="45">
         <v>3.49</v>
@@ -3892,9 +3917,9 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="13.5" customHeight="1">
       <c r="B20" s="40" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C20" s="45">
         <v>7.17</v>
@@ -3906,21 +3931,21 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="13.5" customHeight="1">
       <c r="B21" s="41"/>
     </row>
-    <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="13.5" customHeight="1">
       <c r="B22" s="41"/>
     </row>
-    <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="13.5" customHeight="1">
       <c r="B23" s="41"/>
     </row>
-    <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="13.5" customHeight="1">
       <c r="A24" s="38" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="13.5" customHeight="1">
       <c r="C25" s="39" t="s">
         <v>22</v>
       </c>
@@ -3931,9 +3956,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="13.5" customHeight="1">
       <c r="B26" s="40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C26" s="46">
         <v>4.1399999999999997</v>
@@ -3945,9 +3970,9 @@
         <v>9.76</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="13.5" customHeight="1">
       <c r="B27" s="40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C27" s="46">
         <v>1.05</v>
@@ -3959,9 +3984,9 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="13.5" customHeight="1">
       <c r="B28" s="40" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C28" s="46">
         <v>0.33</v>
@@ -3973,9 +3998,9 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="13.5" customHeight="1">
       <c r="B29" s="40" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C29" s="46">
         <v>0.27</v>
@@ -3987,9 +4012,9 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="13.5" customHeight="1">
       <c r="B30" s="40" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C30" s="46">
         <v>0.67</v>
@@ -4001,25 +4026,25 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="13.5" customHeight="1">
       <c r="B31" s="42"/>
       <c r="C31" s="41"/>
       <c r="D31" s="41"/>
       <c r="E31" s="41"/>
       <c r="F31" s="41"/>
     </row>
-    <row r="32" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="13.5" customHeight="1">
       <c r="B32" s="41"/>
     </row>
-    <row r="33" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="13.5" customHeight="1">
       <c r="B33" s="41"/>
     </row>
-    <row r="34" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="13.5" customHeight="1">
       <c r="A34" s="38" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="13.5" customHeight="1">
       <c r="C35" s="39" t="s">
         <v>22</v>
       </c>
@@ -4030,9 +4055,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="13.5" customHeight="1">
       <c r="B36" s="40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C36" s="46">
         <v>0.45</v>
@@ -4044,9 +4069,9 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="13.5" customHeight="1">
       <c r="B37" s="40" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C37" s="46">
         <v>0.7</v>
@@ -4058,9 +4083,9 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="13.5" customHeight="1">
       <c r="B38" s="40" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C38" s="46">
         <v>0.47</v>
@@ -4072,9 +4097,9 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="13.5" customHeight="1">
       <c r="B39" s="40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C39" s="46">
         <v>1.52</v>
@@ -4086,21 +4111,21 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="13.5" customHeight="1">
       <c r="B40" s="41"/>
     </row>
-    <row r="41" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="13.5" customHeight="1">
       <c r="B41" s="41"/>
     </row>
-    <row r="42" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="13.5" customHeight="1">
       <c r="B42" s="41"/>
     </row>
-    <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="13.5" customHeight="1">
       <c r="A43" s="38" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="13.5" customHeight="1">
       <c r="C44" s="39" t="s">
         <v>22</v>
       </c>
@@ -4111,9 +4136,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="13.5" customHeight="1">
       <c r="B45" s="40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C45" s="44">
         <v>3.5999999999999999E-3</v>
@@ -4125,9 +4150,9 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="13.5" customHeight="1">
       <c r="B46" s="40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C46" s="44">
         <v>3.5999999999999999E-3</v>
@@ -4139,9 +4164,9 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="13.5" customHeight="1">
       <c r="B47" s="40" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C47" s="44">
         <v>5.7999999999999996E-3</v>
@@ -4153,9 +4178,9 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="13.5" customHeight="1">
       <c r="B48" s="40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C48" s="44">
         <v>8.8000000000000005E-3</v>
@@ -4167,9 +4192,9 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="13.5" customHeight="1">
       <c r="B49" s="40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C49" s="44">
         <v>5.8999999999999997E-2</v>
@@ -4181,9 +4206,9 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="13.5" customHeight="1">
       <c r="B50" s="40" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C50" s="44">
         <v>0.32300000000000001</v>
@@ -4195,9 +4220,9 @@
         <v>0.432</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="13.5" customHeight="1">
       <c r="B51" s="40" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C51" s="44">
         <v>0.23</v>
@@ -4209,9 +4234,9 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="13.5" customHeight="1">
       <c r="B52" s="40" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C52" s="44">
         <v>2.17</v>
@@ -4223,21 +4248,21 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="13.5" customHeight="1">
       <c r="B53" s="41"/>
     </row>
-    <row r="54" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="13.5" customHeight="1">
       <c r="B54" s="41"/>
     </row>
-    <row r="55" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="13.5" customHeight="1">
       <c r="B55" s="41"/>
     </row>
-    <row r="56" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="13.5" customHeight="1">
       <c r="A56" s="38" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="13.5" customHeight="1">
       <c r="C57" s="39" t="s">
         <v>22</v>
       </c>
@@ -4248,9 +4273,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="13.5" customHeight="1">
       <c r="B58" s="40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C58" s="46">
         <v>0.95</v>
@@ -4265,9 +4290,9 @@
       <c r="H58" s="47"/>
       <c r="I58" s="47"/>
     </row>
-    <row r="59" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="13.5" customHeight="1">
       <c r="B59" s="40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C59" s="46">
         <v>0.57999999999999996</v>
@@ -4282,9 +4307,9 @@
       <c r="H59" s="47"/>
       <c r="I59" s="47"/>
     </row>
-    <row r="60" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="13.5" customHeight="1">
       <c r="B60" s="40" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C60" s="46">
         <v>0</v>
@@ -4299,9 +4324,9 @@
       <c r="H60" s="47"/>
       <c r="I60" s="47"/>
     </row>
-    <row r="61" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="13.5" customHeight="1">
       <c r="B61" s="40" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C61" s="46">
         <v>2.65</v>
@@ -4316,9 +4341,9 @@
       <c r="H61" s="47"/>
       <c r="I61" s="47"/>
     </row>
-    <row r="62" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="13.5" customHeight="1">
       <c r="B62" s="40" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C62" s="46">
         <v>0.54</v>
@@ -4333,9 +4358,9 @@
       <c r="H62" s="47"/>
       <c r="I62" s="47"/>
     </row>
-    <row r="63" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="13.5" customHeight="1">
       <c r="B63" s="40" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C63" s="46">
         <v>0.9</v>
@@ -4350,9 +4375,9 @@
       <c r="H63" s="47"/>
       <c r="I63" s="47"/>
     </row>
-    <row r="64" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="13.5" customHeight="1">
       <c r="B64" s="40" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C64" s="46">
         <v>0.73</v>
@@ -4367,9 +4392,9 @@
       <c r="H64" s="47"/>
       <c r="I64" s="47"/>
     </row>
-    <row r="65" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="13.5" customHeight="1">
       <c r="B65" s="40" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C65" s="46">
         <v>0.5</v>
@@ -4384,9 +4409,9 @@
       <c r="H65" s="47"/>
       <c r="I65" s="47"/>
     </row>
-    <row r="66" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="13.5" customHeight="1">
       <c r="B66" s="40" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C66" s="46">
         <v>0.92</v>
@@ -4398,19 +4423,19 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="13.5" customHeight="1">
       <c r="B67" s="41"/>
     </row>
-    <row r="70" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="13.5" customHeight="1">
       <c r="A70" s="29" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B70" s="36"/>
       <c r="C70" s="36"/>
       <c r="D70" s="36"/>
       <c r="E70" s="36"/>
     </row>
-    <row r="71" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="13.5" customHeight="1">
       <c r="A71" s="36"/>
       <c r="B71" s="36"/>
       <c r="C71" s="30" t="s">
@@ -4423,10 +4448,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="13.5" customHeight="1">
       <c r="A72" s="36"/>
       <c r="B72" s="31" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C72" s="37">
         <v>0.4</v>
@@ -4438,10 +4463,10 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="13.5" customHeight="1">
       <c r="A73" s="36"/>
       <c r="B73" s="31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C73" s="37">
         <v>0.4</v>
@@ -4453,10 +4478,10 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="13.5" customHeight="1">
       <c r="A74" s="36"/>
       <c r="B74" s="31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C74" s="37">
         <v>0.4</v>
@@ -4468,37 +4493,37 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="13.5" customHeight="1">
       <c r="A75" s="28"/>
       <c r="B75" s="28"/>
       <c r="C75" s="28"/>
       <c r="D75" s="28"/>
       <c r="E75" s="28"/>
     </row>
-    <row r="76" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="13.5" customHeight="1">
       <c r="A76" s="28"/>
       <c r="B76" s="28"/>
       <c r="C76" s="28"/>
       <c r="D76" s="28"/>
       <c r="E76" s="28"/>
     </row>
-    <row r="77" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="15" customHeight="1">
       <c r="A77" s="28"/>
       <c r="B77" s="28"/>
       <c r="C77" s="28"/>
       <c r="D77" s="28"/>
       <c r="E77" s="28"/>
     </row>
-    <row r="78" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="15" customHeight="1">
       <c r="A78" s="32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B78" s="28"/>
       <c r="C78" s="28"/>
       <c r="D78" s="28"/>
       <c r="E78" s="28"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9">
       <c r="A79" s="28"/>
       <c r="B79" s="28"/>
       <c r="C79" s="33" t="s">
@@ -4511,10 +4536,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9">
       <c r="A80" s="28"/>
       <c r="B80" s="34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C80" s="35">
         <v>0.14599999999999999</v>
@@ -4526,10 +4551,10 @@
         <v>0.20499999999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="28"/>
       <c r="B81" s="34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C81" s="35">
         <v>8.0000000000000002E-3</v>
@@ -4541,10 +4566,10 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5">
       <c r="A82" s="28"/>
       <c r="B82" s="34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C82" s="35">
         <v>0.02</v>
@@ -4556,10 +4581,10 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="28"/>
       <c r="B83" s="34" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C83" s="35">
         <v>7.0000000000000007E-2</v>
@@ -4571,10 +4596,10 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="13.5" customHeight="1">
       <c r="A84" s="28"/>
       <c r="B84" s="34" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C84" s="35">
         <v>0.26500000000000001</v>
@@ -4586,10 +4611,10 @@
         <v>0.47399999999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="13.5" customHeight="1">
       <c r="A85" s="28"/>
       <c r="B85" s="34" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C85" s="35">
         <v>0.54700000000000004</v>
@@ -4601,10 +4626,10 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" s="28"/>
       <c r="B86" s="34" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C86" s="35">
         <v>5.2999999999999999E-2</v>
@@ -4618,7 +4643,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4626,20 +4656,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="11.85546875"/>
-    <col min="3" max="3" width="21.140625"/>
-    <col min="4" max="4" width="55.140625"/>
-    <col min="5" max="6" width="11.85546875"/>
-    <col min="7" max="7" width="17.140625"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -4647,7 +4670,7 @@
       <c r="D1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="13.5" customHeight="1">
       <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
@@ -4673,7 +4696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="13.5" customHeight="1">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -4702,7 +4725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="13.5" customHeight="1">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -4734,6 +4757,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4741,21 +4769,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="26" width="11.85546875"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="13.5" customHeight="1">
       <c r="D2" s="5">
         <v>2000</v>
       </c>
@@ -4823,7 +4848,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="13.5" customHeight="1">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4857,7 +4882,7 @@
       </c>
       <c r="Z3" s="9"/>
     </row>
-    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="13.5" customHeight="1">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4899,7 +4924,7 @@
       </c>
       <c r="Z4" s="9"/>
     </row>
-    <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="13.5" customHeight="1">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4933,7 +4958,7 @@
       </c>
       <c r="Z5" s="9"/>
     </row>
-    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="13.5" customHeight="1">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4967,7 +4992,7 @@
       </c>
       <c r="Z7" s="9"/>
     </row>
-    <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="13.5" customHeight="1">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5009,7 +5034,7 @@
       </c>
       <c r="Z8" s="9"/>
     </row>
-    <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="13.5" customHeight="1">
       <c r="B9" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5047,6 +5072,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5054,21 +5084,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="26" width="11.85546875"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="13.5" customHeight="1">
       <c r="D2" s="5">
         <v>2000</v>
       </c>
@@ -5136,7 +5163,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="13.5" customHeight="1">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5170,7 +5197,7 @@
       </c>
       <c r="Z3" s="11"/>
     </row>
-    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="13.5" customHeight="1">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5210,7 +5237,7 @@
       </c>
       <c r="Z4" s="12"/>
     </row>
-    <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="13.5" customHeight="1">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5244,7 +5271,7 @@
       </c>
       <c r="Z5" s="11"/>
     </row>
-    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="13.5" customHeight="1">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5278,7 +5305,7 @@
       </c>
       <c r="Z7" s="11"/>
     </row>
-    <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="13.5" customHeight="1">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5318,7 +5345,7 @@
       </c>
       <c r="Z8" s="11"/>
     </row>
-    <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="13.5" customHeight="1">
       <c r="B9" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5356,6 +5383,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5363,21 +5395,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="25" width="11.85546875"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -5445,7 +5474,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5480,7 +5509,7 @@
       </c>
       <c r="Y3" s="11"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5515,12 +5544,12 @@
       </c>
       <c r="Y4" s="11"/>
     </row>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -5588,7 +5617,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1">
       <c r="B10" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5621,7 +5650,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1">
       <c r="B11" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5654,12 +5683,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -5727,7 +5756,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:25" ht="13.5" customHeight="1">
       <c r="B17" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5760,7 +5789,7 @@
       </c>
       <c r="Y17" s="11"/>
     </row>
-    <row r="18" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:25" ht="13.5" customHeight="1">
       <c r="B18" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5798,6 +5827,11 @@
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5805,21 +5839,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y47"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="25" width="11.85546875"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -5887,7 +5918,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5920,7 +5951,7 @@
       </c>
       <c r="Y3" s="13"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5953,12 +5984,12 @@
       </c>
       <c r="Y4" s="13"/>
     </row>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -6026,7 +6057,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1">
       <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
@@ -6058,12 +6089,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="13.5" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="13.5" customHeight="1">
       <c r="C15" s="5">
         <v>2000</v>
       </c>
@@ -6131,7 +6162,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
@@ -6171,12 +6202,12 @@
       </c>
       <c r="Y16" s="6"/>
     </row>
-    <row r="20" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="13.5" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="13.5" customHeight="1">
       <c r="C21" s="5">
         <v>2000</v>
       </c>
@@ -6244,7 +6275,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="13.5" customHeight="1">
       <c r="B22" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -6277,7 +6308,7 @@
       </c>
       <c r="Y22" s="13"/>
     </row>
-    <row r="23" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="13.5" customHeight="1">
       <c r="B23" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -6310,12 +6341,12 @@
       </c>
       <c r="Y23" s="13"/>
     </row>
-    <row r="27" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="13.5" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" ht="13.5" customHeight="1">
       <c r="C28" s="5">
         <v>2000</v>
       </c>
@@ -6383,7 +6414,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="B29" s="5" t="s">
         <v>32</v>
       </c>
@@ -6415,12 +6446,12 @@
       </c>
       <c r="Y29" s="6"/>
     </row>
-    <row r="33" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" ht="13.5" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" ht="13.5" customHeight="1">
       <c r="C34" s="5">
         <v>2000</v>
       </c>
@@ -6488,7 +6519,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" ht="13.5" customHeight="1">
       <c r="B35" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -6545,12 +6576,12 @@
       </c>
       <c r="Y35" s="15"/>
     </row>
-    <row r="39" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="13.5" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" ht="13.5" customHeight="1">
       <c r="C40" s="5">
         <v>2000</v>
       </c>
@@ -6618,7 +6649,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" ht="13.5" customHeight="1">
       <c r="B41" s="5" t="s">
         <v>32</v>
       </c>
@@ -6651,12 +6682,12 @@
         <v>0.12180000000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" ht="14">
       <c r="A45" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" ht="14">
       <c r="C46" s="18">
         <v>2000</v>
       </c>
@@ -6724,7 +6755,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" ht="14">
       <c r="B47" s="18" t="s">
         <v>30</v>
       </c>
@@ -6761,6 +6792,11 @@
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6768,21 +6804,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="25" width="11.85546875"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -6850,7 +6883,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>32</v>
       </c>
@@ -6880,12 +6913,12 @@
       </c>
       <c r="Y3" s="15"/>
     </row>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="13.5" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="13.5" customHeight="1">
       <c r="C8" s="5">
         <v>2000</v>
       </c>
@@ -6953,7 +6986,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>32</v>
       </c>
@@ -6983,12 +7016,12 @@
       </c>
       <c r="Y9" s="15"/>
     </row>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="13.5" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="13.5" customHeight="1">
       <c r="C14" s="5">
         <v>2000</v>
       </c>
@@ -7056,7 +7089,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="13.5" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
@@ -7086,12 +7119,12 @@
       </c>
       <c r="Y15" s="15"/>
     </row>
-    <row r="19" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="13.5" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="13.5" customHeight="1">
       <c r="C20" s="5">
         <v>2000</v>
       </c>
@@ -7159,7 +7192,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="13.5" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>32</v>
       </c>
@@ -7189,12 +7222,12 @@
       </c>
       <c r="Y21" s="15"/>
     </row>
-    <row r="25" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="13.5" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="13.5" customHeight="1">
       <c r="C26" s="5">
         <v>2000</v>
       </c>
@@ -7262,7 +7295,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="13.5" customHeight="1">
       <c r="B27" s="5" t="s">
         <v>32</v>
       </c>
@@ -7292,12 +7325,12 @@
       </c>
       <c r="Y27" s="15"/>
     </row>
-    <row r="31" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="C32" s="5">
         <v>2000</v>
       </c>
@@ -7365,7 +7398,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" ht="13.5" customHeight="1">
       <c r="B33" s="5" t="s">
         <v>32</v>
       </c>
@@ -7395,12 +7428,12 @@
       </c>
       <c r="Y33" s="15"/>
     </row>
-    <row r="37" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="13.5" customHeight="1">
       <c r="C38" s="5">
         <v>2000</v>
       </c>
@@ -7468,7 +7501,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="13.5" customHeight="1">
       <c r="B39" s="5" t="s">
         <v>32</v>
       </c>
@@ -7498,15 +7531,15 @@
       </c>
       <c r="Y39" s="15"/>
     </row>
-    <row r="40" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" ht="15" customHeight="1"/>
+    <row r="41" spans="1:25" ht="15" customHeight="1"/>
+    <row r="42" spans="1:25" ht="15" customHeight="1"/>
+    <row r="43" spans="1:25" ht="14">
       <c r="A43" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" ht="14">
       <c r="C44" s="18">
         <v>2000</v>
       </c>
@@ -7574,7 +7607,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" ht="14">
       <c r="B45" s="18" t="s">
         <v>30</v>
       </c>
@@ -7604,12 +7637,12 @@
       </c>
       <c r="Y45" s="19"/>
     </row>
-    <row r="49" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:35" ht="14">
       <c r="A49" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" ht="14">
       <c r="C50" s="18">
         <v>2000</v>
       </c>
@@ -7677,7 +7710,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" ht="14">
       <c r="B51" s="18" t="s">
         <v>30</v>
       </c>
@@ -7707,12 +7740,12 @@
       </c>
       <c r="Y51" s="19"/>
     </row>
-    <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" ht="15" customHeight="1">
       <c r="A55" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" ht="15" customHeight="1">
       <c r="C56" s="18">
         <v>2000</v>
       </c>
@@ -7780,7 +7813,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:35" ht="15" customHeight="1">
       <c r="B57" s="18" t="s">
         <v>30</v>
       </c>
@@ -7810,12 +7843,12 @@
       </c>
       <c r="Y57" s="19"/>
     </row>
-    <row r="61" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:35" ht="14">
       <c r="A61" s="17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:35" ht="14">
       <c r="C62" s="18">
         <v>2000</v>
       </c>
@@ -7913,7 +7946,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="63" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:35" ht="14">
       <c r="B63" s="18" t="s">
         <v>30</v>
       </c>
@@ -7955,32 +7988,34 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="1048576" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048576" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y43"/>
+  <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1025" width="11.85546875"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="14">
       <c r="A1" s="17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="14">
       <c r="C2" s="18">
         <v>2000</v>
       </c>
@@ -8048,7 +8083,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="14">
       <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
@@ -8076,11 +8111,11 @@
       <c r="X3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Y3" s="19">
+      <c r="Y3" s="54">
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="14">
       <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
@@ -8108,16 +8143,16 @@
       <c r="X4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Y4" s="19">
+      <c r="Y4" s="54">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="14">
       <c r="A8" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="14">
       <c r="C9" s="18">
         <v>2000</v>
       </c>
@@ -8185,7 +8220,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="14">
       <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
@@ -8214,10 +8249,10 @@
         <v>21</v>
       </c>
       <c r="Y10" s="19">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="14">
       <c r="B11" s="5" t="s">
         <v>16</v>
       </c>
@@ -8246,15 +8281,15 @@
         <v>21</v>
       </c>
       <c r="Y11" s="19">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="14">
       <c r="A15" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="14">
       <c r="C16" s="18">
         <v>2000</v>
       </c>
@@ -8322,7 +8357,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="14">
       <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
@@ -8354,7 +8389,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="14">
       <c r="B18" s="5" t="s">
         <v>16</v>
       </c>
@@ -8386,12 +8421,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="14">
       <c r="A22" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="14">
       <c r="C23" s="18">
         <v>2000</v>
       </c>
@@ -8459,388 +8494,256 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
+    <row r="24" spans="1:25" ht="14">
+      <c r="B24" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="19"/>
+      <c r="W24" s="19"/>
       <c r="X24" s="20" t="s">
         <v>21</v>
       </c>
       <c r="Y24" s="19">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="20" t="s">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="14">
+      <c r="A28" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" ht="14">
+      <c r="C29" s="18">
+        <v>2000</v>
+      </c>
+      <c r="D29" s="18">
+        <v>2001</v>
+      </c>
+      <c r="E29" s="18">
+        <v>2002</v>
+      </c>
+      <c r="F29" s="18">
+        <v>2003</v>
+      </c>
+      <c r="G29" s="18">
+        <v>2004</v>
+      </c>
+      <c r="H29" s="18">
+        <v>2005</v>
+      </c>
+      <c r="I29" s="18">
+        <v>2006</v>
+      </c>
+      <c r="J29" s="18">
+        <v>2007</v>
+      </c>
+      <c r="K29" s="18">
+        <v>2008</v>
+      </c>
+      <c r="L29" s="18">
+        <v>2009</v>
+      </c>
+      <c r="M29" s="18">
+        <v>2010</v>
+      </c>
+      <c r="N29" s="18">
+        <v>2011</v>
+      </c>
+      <c r="O29" s="18">
+        <v>2012</v>
+      </c>
+      <c r="P29" s="18">
+        <v>2013</v>
+      </c>
+      <c r="Q29" s="18">
+        <v>2014</v>
+      </c>
+      <c r="R29" s="18">
+        <v>2015</v>
+      </c>
+      <c r="S29" s="18">
+        <v>2016</v>
+      </c>
+      <c r="T29" s="18">
+        <v>2017</v>
+      </c>
+      <c r="U29" s="18">
+        <v>2018</v>
+      </c>
+      <c r="V29" s="18">
+        <v>2019</v>
+      </c>
+      <c r="W29" s="18">
+        <v>2020</v>
+      </c>
+      <c r="Y29" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" ht="14">
+      <c r="B30" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="21"/>
+      <c r="U30" s="21"/>
+      <c r="V30" s="21"/>
+      <c r="W30" s="21"/>
+      <c r="X30" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Y25" s="19">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="Y30" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" ht="14">
+      <c r="A34" s="17" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="C30" s="18">
+    <row r="35" spans="1:25" ht="14">
+      <c r="C35" s="18">
         <v>2000</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D35" s="18">
         <v>2001</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E35" s="18">
         <v>2002</v>
       </c>
-      <c r="F30" s="18">
+      <c r="F35" s="18">
         <v>2003</v>
       </c>
-      <c r="G30" s="18">
+      <c r="G35" s="18">
         <v>2004</v>
       </c>
-      <c r="H30" s="18">
+      <c r="H35" s="18">
         <v>2005</v>
       </c>
-      <c r="I30" s="18">
+      <c r="I35" s="18">
         <v>2006</v>
       </c>
-      <c r="J30" s="18">
+      <c r="J35" s="18">
         <v>2007</v>
       </c>
-      <c r="K30" s="18">
+      <c r="K35" s="18">
         <v>2008</v>
       </c>
-      <c r="L30" s="18">
+      <c r="L35" s="18">
         <v>2009</v>
       </c>
-      <c r="M30" s="18">
+      <c r="M35" s="18">
         <v>2010</v>
       </c>
-      <c r="N30" s="18">
+      <c r="N35" s="18">
         <v>2011</v>
       </c>
-      <c r="O30" s="18">
+      <c r="O35" s="18">
         <v>2012</v>
       </c>
-      <c r="P30" s="18">
+      <c r="P35" s="18">
         <v>2013</v>
       </c>
-      <c r="Q30" s="18">
+      <c r="Q35" s="18">
         <v>2014</v>
       </c>
-      <c r="R30" s="18">
+      <c r="R35" s="18">
         <v>2015</v>
       </c>
-      <c r="S30" s="18">
+      <c r="S35" s="18">
         <v>2016</v>
       </c>
-      <c r="T30" s="18">
+      <c r="T35" s="18">
         <v>2017</v>
       </c>
-      <c r="U30" s="18">
+      <c r="U35" s="18">
         <v>2018</v>
       </c>
-      <c r="V30" s="18">
+      <c r="V35" s="18">
         <v>2019</v>
       </c>
-      <c r="W30" s="18">
+      <c r="W35" s="18">
         <v>2020</v>
       </c>
-      <c r="Y30" s="18" t="s">
+      <c r="Y35" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="B31" s="18" t="s">
+    <row r="36" spans="1:25" ht="14">
+      <c r="B36" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="19"/>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
-      <c r="S31" s="19"/>
-      <c r="T31" s="19"/>
-      <c r="U31" s="19"/>
-      <c r="V31" s="19"/>
-      <c r="W31" s="19"/>
-      <c r="X31" s="20" t="s">
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
+      <c r="U36" s="19"/>
+      <c r="V36" s="19"/>
+      <c r="W36" s="19"/>
+      <c r="X36" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Y31" s="19">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="C36" s="18">
-        <v>2000</v>
-      </c>
-      <c r="D36" s="18">
-        <v>2001</v>
-      </c>
-      <c r="E36" s="18">
-        <v>2002</v>
-      </c>
-      <c r="F36" s="18">
-        <v>2003</v>
-      </c>
-      <c r="G36" s="18">
-        <v>2004</v>
-      </c>
-      <c r="H36" s="18">
-        <v>2005</v>
-      </c>
-      <c r="I36" s="18">
-        <v>2006</v>
-      </c>
-      <c r="J36" s="18">
-        <v>2007</v>
-      </c>
-      <c r="K36" s="18">
-        <v>2008</v>
-      </c>
-      <c r="L36" s="18">
-        <v>2009</v>
-      </c>
-      <c r="M36" s="18">
-        <v>2010</v>
-      </c>
-      <c r="N36" s="18">
-        <v>2011</v>
-      </c>
-      <c r="O36" s="18">
-        <v>2012</v>
-      </c>
-      <c r="P36" s="18">
-        <v>2013</v>
-      </c>
-      <c r="Q36" s="18">
-        <v>2014</v>
-      </c>
-      <c r="R36" s="18">
-        <v>2015</v>
-      </c>
-      <c r="S36" s="18">
-        <v>2016</v>
-      </c>
-      <c r="T36" s="18">
-        <v>2017</v>
-      </c>
-      <c r="U36" s="18">
-        <v>2018</v>
-      </c>
-      <c r="V36" s="18">
-        <v>2019</v>
-      </c>
-      <c r="W36" s="18">
-        <v>2020</v>
-      </c>
-      <c r="Y36" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="B37" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="21"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="21"/>
-      <c r="N37" s="21"/>
-      <c r="O37" s="21"/>
-      <c r="P37" s="21"/>
-      <c r="Q37" s="21"/>
-      <c r="R37" s="21"/>
-      <c r="S37" s="21"/>
-      <c r="T37" s="21"/>
-      <c r="U37" s="21"/>
-      <c r="V37" s="21"/>
-      <c r="W37" s="21"/>
-      <c r="X37" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y37" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="C42" s="18">
-        <v>2000</v>
-      </c>
-      <c r="D42" s="18">
-        <v>2001</v>
-      </c>
-      <c r="E42" s="18">
-        <v>2002</v>
-      </c>
-      <c r="F42" s="18">
-        <v>2003</v>
-      </c>
-      <c r="G42" s="18">
-        <v>2004</v>
-      </c>
-      <c r="H42" s="18">
-        <v>2005</v>
-      </c>
-      <c r="I42" s="18">
-        <v>2006</v>
-      </c>
-      <c r="J42" s="18">
-        <v>2007</v>
-      </c>
-      <c r="K42" s="18">
-        <v>2008</v>
-      </c>
-      <c r="L42" s="18">
-        <v>2009</v>
-      </c>
-      <c r="M42" s="18">
-        <v>2010</v>
-      </c>
-      <c r="N42" s="18">
-        <v>2011</v>
-      </c>
-      <c r="O42" s="18">
-        <v>2012</v>
-      </c>
-      <c r="P42" s="18">
-        <v>2013</v>
-      </c>
-      <c r="Q42" s="18">
-        <v>2014</v>
-      </c>
-      <c r="R42" s="18">
-        <v>2015</v>
-      </c>
-      <c r="S42" s="18">
-        <v>2016</v>
-      </c>
-      <c r="T42" s="18">
-        <v>2017</v>
-      </c>
-      <c r="U42" s="18">
-        <v>2018</v>
-      </c>
-      <c r="V42" s="18">
-        <v>2019</v>
-      </c>
-      <c r="W42" s="18">
-        <v>2020</v>
-      </c>
-      <c r="Y42" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="B43" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="19"/>
-      <c r="M43" s="19"/>
-      <c r="N43" s="19"/>
-      <c r="O43" s="19"/>
-      <c r="P43" s="19"/>
-      <c r="Q43" s="19"/>
-      <c r="R43" s="19"/>
-      <c r="S43" s="19"/>
-      <c r="T43" s="19"/>
-      <c r="U43" s="19"/>
-      <c r="V43" s="19"/>
-      <c r="W43" s="19"/>
-      <c r="X43" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y43" s="19">
+      <c r="Y36" s="19">
         <v>0.95</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8848,21 +8751,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="25" width="11.85546875"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -8930,7 +8830,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -8963,7 +8863,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -8996,12 +8896,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -9069,7 +8969,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1">
       <c r="B10" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9103,7 +9003,7 @@
         <v>12.000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1">
       <c r="B11" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9137,12 +9037,12 @@
         <v>6.0000000000000009</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="13.5" customHeight="1">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -9210,7 +9110,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="13.5" customHeight="1">
       <c r="B17" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9243,7 +9143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="13.5" customHeight="1">
       <c r="B18" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9276,12 +9176,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="13.5" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="13.5" customHeight="1">
       <c r="C23" s="5">
         <v>2000</v>
       </c>
@@ -9349,7 +9249,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="13.5" customHeight="1">
       <c r="B24" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9382,7 +9282,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="13.5" customHeight="1">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9415,12 +9315,12 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" ht="13.5" customHeight="1">
       <c r="C30" s="5">
         <v>2000</v>
       </c>
@@ -9488,7 +9388,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="13.5" customHeight="1">
       <c r="B31" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9521,7 +9421,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="B32" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9554,12 +9454,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" ht="13.5" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" ht="13.5" customHeight="1">
       <c r="C37" s="5">
         <v>2000</v>
       </c>
@@ -9627,7 +9527,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="13.5" customHeight="1">
       <c r="B38" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9660,7 +9560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="13.5" customHeight="1">
       <c r="B39" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9693,12 +9593,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" ht="13.5" customHeight="1">
       <c r="C44" s="5">
         <v>2000</v>
       </c>
@@ -9766,7 +9666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" ht="13.5" customHeight="1">
       <c r="B45" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9799,12 +9699,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" ht="13.5" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" ht="13.5" customHeight="1">
       <c r="C50" s="5">
         <v>2000</v>
       </c>
@@ -9872,7 +9772,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" ht="13.5" customHeight="1">
       <c r="B51" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9910,5 +9810,10 @@
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ok, fixed problem with numvlmon
</commit_message>
<xml_diff>
--- a/tests/simple.xlsx
+++ b/tests/simple.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="988" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="555" yWindow="555" windowWidth="25035" windowHeight="15495" tabRatio="988" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Partnerships &amp; transitions" sheetId="11" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1119,12 +1119,12 @@
     <xf numFmtId="167" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="4" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="236">
     <cellStyle name="Comma 2" xfId="2"/>
@@ -1724,7 +1724,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1779,7 +1779,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1834,7 +1834,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1889,7 +1889,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1944,7 +1944,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1999,7 +1999,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2054,7 +2054,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2109,7 +2109,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2164,7 +2164,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2219,7 +2219,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2274,7 +2274,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2329,7 +2329,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3294,7 +3294,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3349,7 +3349,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3404,7 +3404,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3459,7 +3459,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3514,7 +3514,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3569,7 +3569,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3624,7 +3624,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3679,7 +3679,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4323,55 +4323,55 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="80.6640625" customWidth="1"/>
+    <col min="1" max="1" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="12.75" customHeight="1">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="66" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="12.75" customHeight="1">
-      <c r="A2" s="63"/>
-    </row>
-    <row r="3" spans="1:1" ht="12.75" customHeight="1">
-      <c r="A3" s="63"/>
-    </row>
-    <row r="4" spans="1:1">
+    <row r="2" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="66"/>
+    </row>
+    <row r="3" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="66"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="60"/>
     </row>
-    <row r="5" spans="1:1" ht="67.5" customHeight="1">
+    <row r="5" spans="1:1" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="60" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="60"/>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="60" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="60"/>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="60" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="60"/>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="60" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="60"/>
     </row>
   </sheetData>
@@ -4396,14 +4396,14 @@
       <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4">
         <v>2000</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4504,7 +4504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4537,12 +4537,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1">
+    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="4">
         <v>2000</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4643,7 +4643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4676,12 +4676,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1">
+    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="4">
         <v>2000</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:25" ht="13.5" customHeight="1">
+    <row r="17" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>28</v>
       </c>
@@ -4800,16 +4800,16 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.5" customHeight="1">
+    <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" ht="13.5" customHeight="1">
+    <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4819,7 +4819,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.5" customHeight="1">
+    <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4829,7 +4829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.5" customHeight="1">
+    <row r="4" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4837,26 +4837,26 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="13.5" customHeight="1">
+    <row r="5" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" ht="13.5" customHeight="1">
+    <row r="6" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="13.5" customHeight="1">
+    <row r="7" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" ht="13.5" customHeight="1">
+    <row r="8" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="13.5" customHeight="1">
+    <row r="9" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4866,7 +4866,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13.5" customHeight="1">
+    <row r="10" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4876,7 +4876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.5" customHeight="1">
+    <row r="11" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4884,26 +4884,26 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" ht="13.5" customHeight="1">
+    <row r="12" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="13.5" customHeight="1">
+    <row r="13" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="13.5" customHeight="1">
+    <row r="14" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="13.5" customHeight="1">
+    <row r="15" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1">
+    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4913,7 +4913,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="13.5" customHeight="1">
+    <row r="17" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4921,7 +4921,7 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:4" ht="13.5" customHeight="1">
+    <row r="18" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4929,26 +4929,26 @@
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:4" ht="13.5" customHeight="1">
+    <row r="19" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="13.5" customHeight="1">
+    <row r="20" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" ht="13.5" customHeight="1">
+    <row r="21" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="13.5" customHeight="1">
+    <row r="22" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" ht="13.5" customHeight="1">
+    <row r="23" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4958,7 +4958,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="13.5" customHeight="1">
+    <row r="24" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4966,7 +4966,7 @@
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:4" ht="13.5" customHeight="1">
+    <row r="25" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4974,14 +4974,14 @@
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
     </row>
-    <row r="29" spans="1:4" ht="13.5" customHeight="1">
+    <row r="29" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="13.5" customHeight="1">
+    <row r="30" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4991,7 +4991,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="13.5" customHeight="1">
+    <row r="31" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4999,14 +4999,14 @@
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
     </row>
-    <row r="35" spans="1:4" ht="13.5" customHeight="1">
+    <row r="35" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" ht="13.5" customHeight="1">
+    <row r="36" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5016,7 +5016,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="13.5" customHeight="1">
+    <row r="37" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5024,7 +5024,7 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:4" ht="13.5" customHeight="1">
+    <row r="38" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5032,14 +5032,14 @@
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="42" spans="1:4" ht="13.5" customHeight="1">
+    <row r="42" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" ht="13.5" customHeight="1">
+    <row r="43" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5049,7 +5049,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="13.5" customHeight="1">
+    <row r="44" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5057,7 +5057,7 @@
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
     </row>
-    <row r="45" spans="1:4" ht="13.5" customHeight="1">
+    <row r="45" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5080,17 +5080,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1">
+    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>59</v>
       </c>
@@ -5099,7 +5099,7 @@
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1">
+    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="B2" s="33"/>
       <c r="C2" s="34" t="s">
@@ -5112,7 +5112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1">
+    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33"/>
       <c r="B3" s="36" t="s">
         <v>60</v>
@@ -5127,7 +5127,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1">
+    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
       <c r="B4" s="36" t="s">
         <v>61</v>
@@ -5142,7 +5142,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1">
+    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33"/>
       <c r="B5" s="36" t="s">
         <v>62</v>
@@ -5157,7 +5157,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1">
+    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33"/>
       <c r="B6" s="36" t="s">
         <v>63</v>
@@ -5172,7 +5172,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1">
+    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33"/>
       <c r="B7" s="36" t="s">
         <v>64</v>
@@ -5187,7 +5187,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1">
+    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
       <c r="B8" s="36" t="s">
         <v>65</v>
@@ -5202,7 +5202,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1">
+    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
       <c r="B9" s="36" t="s">
         <v>66</v>
@@ -5217,33 +5217,33 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1">
+    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="39"/>
       <c r="B10" s="40"/>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
       <c r="E10" s="39"/>
     </row>
-    <row r="11" spans="1:5" ht="13.5" customHeight="1">
+    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="39"/>
       <c r="B11" s="40"/>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
       <c r="E11" s="39"/>
     </row>
-    <row r="12" spans="1:5" ht="13.5" customHeight="1">
+    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="39"/>
       <c r="B12" s="40"/>
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
       <c r="E12" s="39"/>
     </row>
-    <row r="13" spans="1:5" ht="13.5" customHeight="1">
+    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1">
+    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="17" t="s">
         <v>18</v>
       </c>
@@ -5254,7 +5254,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1">
+    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="38" t="s">
         <v>68</v>
       </c>
@@ -5268,7 +5268,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="13.5" customHeight="1">
+    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="38" t="s">
         <v>69</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="13.5" customHeight="1">
+    <row r="17" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="38" t="s">
         <v>70</v>
       </c>
@@ -5296,7 +5296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="13.5" customHeight="1">
+    <row r="18" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="38" t="s">
         <v>71</v>
       </c>
@@ -5310,7 +5310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.5" customHeight="1">
+    <row r="19" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38" t="s">
         <v>72</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="13.5" customHeight="1">
+    <row r="20" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="38" t="s">
         <v>73</v>
       </c>
@@ -5338,33 +5338,33 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="13.5" customHeight="1">
+    <row r="21" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="39"/>
       <c r="B21" s="40"/>
       <c r="C21" s="39"/>
       <c r="D21" s="39"/>
       <c r="E21" s="39"/>
     </row>
-    <row r="22" spans="1:7" ht="13.5" customHeight="1">
+    <row r="22" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="39"/>
       <c r="B22" s="40"/>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
       <c r="E22" s="39"/>
     </row>
-    <row r="23" spans="1:7" ht="13.5" customHeight="1">
+    <row r="23" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="39"/>
       <c r="B23" s="40"/>
       <c r="C23" s="39"/>
       <c r="D23" s="39"/>
       <c r="E23" s="39"/>
     </row>
-    <row r="24" spans="1:7" ht="13.5" customHeight="1">
+    <row r="24" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13.5" customHeight="1">
+    <row r="25" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="17" t="s">
         <v>18</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="13.5" customHeight="1">
+    <row r="26" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="38" t="s">
         <v>74</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13.5" customHeight="1">
+    <row r="27" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="38" t="s">
         <v>70</v>
       </c>
@@ -5404,7 +5404,7 @@
       </c>
       <c r="G27" s="43"/>
     </row>
-    <row r="28" spans="1:7" ht="13.5" customHeight="1">
+    <row r="28" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="38" t="s">
         <v>75</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="13.5" customHeight="1">
+    <row r="29" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="38" t="s">
         <v>76</v>
       </c>
@@ -5432,7 +5432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="13.5" customHeight="1">
+    <row r="30" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="38" t="s">
         <v>77</v>
       </c>
@@ -5446,33 +5446,33 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="13.5" customHeight="1">
+    <row r="31" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="39"/>
       <c r="B31" s="40"/>
       <c r="C31" s="39"/>
       <c r="D31" s="39"/>
       <c r="E31" s="39"/>
     </row>
-    <row r="32" spans="1:7" ht="13.5" customHeight="1">
+    <row r="32" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="39"/>
       <c r="B32" s="40"/>
       <c r="C32" s="39"/>
       <c r="D32" s="39"/>
       <c r="E32" s="39"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="39"/>
       <c r="B33" s="40"/>
       <c r="C33" s="39"/>
       <c r="D33" s="39"/>
       <c r="E33" s="39"/>
     </row>
-    <row r="34" spans="1:9" ht="14">
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="14">
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="C35" s="17" t="s">
         <v>18</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="14">
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" s="38" t="s">
         <v>78</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>7.28</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14">
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B37" s="38" t="s">
         <v>79</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>3.42</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="14">
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B38" s="38" t="s">
         <v>80</v>
       </c>
@@ -5525,7 +5525,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="14">
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="38" t="s">
         <v>81</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="32" customFormat="1" ht="13.5" customHeight="1">
+    <row r="40" spans="1:9" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="28"/>
       <c r="B40" s="38" t="s">
         <v>105</v>
@@ -5554,47 +5554,47 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="32" customFormat="1" ht="13.5" customHeight="1">
+    <row r="41" spans="1:9" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="C41" s="64">
+      <c r="C41" s="63">
         <v>2</v>
       </c>
-      <c r="D41" s="65">
+      <c r="D41" s="64">
         <v>1.5</v>
       </c>
-      <c r="E41" s="65">
+      <c r="E41" s="64">
         <v>2.5</v>
       </c>
-      <c r="F41" s="66"/>
-      <c r="G41" s="66"/>
-      <c r="H41" s="66"/>
-      <c r="I41" s="66"/>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="F41" s="65"/>
+      <c r="G41" s="65"/>
+      <c r="H41" s="65"/>
+      <c r="I41" s="65"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="39"/>
       <c r="B42" s="40"/>
       <c r="C42" s="39"/>
       <c r="D42" s="39"/>
       <c r="E42" s="39"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="39"/>
       <c r="B43" s="40"/>
       <c r="C43" s="39"/>
       <c r="D43" s="39"/>
       <c r="E43" s="39"/>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="39"/>
       <c r="B44" s="40"/>
       <c r="C44" s="39"/>
       <c r="D44" s="39"/>
       <c r="E44" s="39"/>
     </row>
-    <row r="45" spans="1:9" s="32" customFormat="1" ht="13.5" customHeight="1">
+    <row r="45" spans="1:9" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="26" t="s">
         <v>109</v>
       </c>
@@ -5603,7 +5603,7 @@
       <c r="D45" s="28"/>
       <c r="E45" s="28"/>
     </row>
-    <row r="46" spans="1:9" s="32" customFormat="1" ht="13.5" customHeight="1">
+    <row r="46" spans="1:9" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="28"/>
       <c r="B46" s="28"/>
       <c r="C46" s="27" t="s">
@@ -5616,7 +5616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="32" customFormat="1" ht="13.5" customHeight="1">
+    <row r="47" spans="1:9" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="28"/>
       <c r="B47" s="38" t="s">
         <v>70</v>
@@ -5631,7 +5631,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="32" customFormat="1" ht="13.5" customHeight="1">
+    <row r="48" spans="1:9" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="28"/>
       <c r="B48" s="38" t="s">
         <v>78</v>
@@ -5646,7 +5646,7 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1">
+    <row r="49" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="28"/>
       <c r="B49" s="38" t="s">
         <v>75</v>
@@ -5661,7 +5661,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1">
+    <row r="50" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="28"/>
       <c r="B50" s="38" t="s">
         <v>79</v>
@@ -5676,7 +5676,7 @@
         <v>0.82699999999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1">
+    <row r="51" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="28"/>
       <c r="B51" s="38" t="s">
         <v>76</v>
@@ -5691,7 +5691,7 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1">
+    <row r="52" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="28"/>
       <c r="B52" s="38" t="s">
         <v>80</v>
@@ -5706,7 +5706,7 @@
         <v>0.68600000000000005</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1">
+    <row r="53" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="28"/>
       <c r="B53" s="38" t="s">
         <v>77</v>
@@ -5721,7 +5721,7 @@
         <v>0.72299999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1">
+    <row r="54" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="28"/>
       <c r="B54" s="38" t="s">
         <v>81</v>
@@ -5736,7 +5736,7 @@
         <v>0.56299999999999994</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1">
+    <row r="55" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="28"/>
       <c r="B55" s="38" t="s">
         <v>110</v>
@@ -5751,33 +5751,33 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="32" customFormat="1" ht="15" customHeight="1">
+    <row r="56" spans="1:5" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="25"/>
       <c r="B56" s="25"/>
       <c r="C56" s="25"/>
       <c r="D56" s="25"/>
       <c r="E56" s="25"/>
     </row>
-    <row r="57" spans="1:5" s="32" customFormat="1" ht="15" customHeight="1">
+    <row r="57" spans="1:5" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="25"/>
       <c r="B57" s="25"/>
       <c r="C57" s="25"/>
       <c r="D57" s="25"/>
       <c r="E57" s="25"/>
     </row>
-    <row r="58" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1">
+    <row r="58" spans="1:5" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="25"/>
       <c r="B58" s="25"/>
       <c r="C58" s="25"/>
       <c r="D58" s="25"/>
       <c r="E58" s="25"/>
     </row>
-    <row r="59" spans="1:5" ht="13.5" customHeight="1">
+    <row r="59" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="13.5" customHeight="1">
+    <row r="60" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="17" t="s">
         <v>18</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="13.5" customHeight="1">
+    <row r="61" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="38" t="s">
         <v>68</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="13.5" customHeight="1">
+    <row r="62" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="38" t="s">
         <v>69</v>
       </c>
@@ -5816,7 +5816,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="13.5" customHeight="1">
+    <row r="63" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="38" t="s">
         <v>83</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="13.5" customHeight="1">
+    <row r="64" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="38" t="s">
         <v>71</v>
       </c>
@@ -5844,7 +5844,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="13.5" customHeight="1">
+    <row r="65" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="38" t="s">
         <v>72</v>
       </c>
@@ -5859,7 +5859,7 @@
       </c>
       <c r="F65" s="39"/>
     </row>
-    <row r="66" spans="1:9" ht="13.5" customHeight="1">
+    <row r="66" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="38" t="s">
         <v>73</v>
       </c>
@@ -5874,7 +5874,7 @@
       </c>
       <c r="F66" s="39"/>
     </row>
-    <row r="67" spans="1:9" ht="13.5" customHeight="1">
+    <row r="67" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="38" t="s">
         <v>106</v>
       </c>
@@ -5889,7 +5889,7 @@
       </c>
       <c r="F67" s="39"/>
     </row>
-    <row r="68" spans="1:9" ht="13.5" customHeight="1">
+    <row r="68" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="38" t="s">
         <v>107</v>
       </c>
@@ -5904,7 +5904,7 @@
       </c>
       <c r="F68" s="39"/>
     </row>
-    <row r="69" spans="1:9" ht="13.5" customHeight="1">
+    <row r="69" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="38" t="s">
         <v>84</v>
       </c>
@@ -5919,7 +5919,7 @@
       </c>
       <c r="F69" s="39"/>
     </row>
-    <row r="70" spans="1:9" ht="13.5" customHeight="1">
+    <row r="70" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="39"/>
       <c r="B70" s="40"/>
       <c r="C70" s="39"/>
@@ -5927,7 +5927,7 @@
       <c r="E70" s="39"/>
       <c r="F70" s="39"/>
     </row>
-    <row r="71" spans="1:9" ht="13.5" customHeight="1">
+    <row r="71" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="39"/>
       <c r="B71" s="40"/>
       <c r="C71" s="39"/>
@@ -5938,7 +5938,7 @@
       <c r="H71" s="39"/>
       <c r="I71" s="39"/>
     </row>
-    <row r="72" spans="1:9" ht="13.5" customHeight="1">
+    <row r="72" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="39"/>
       <c r="B72" s="40"/>
       <c r="C72" s="39"/>
@@ -5949,7 +5949,7 @@
       <c r="H72" s="39"/>
       <c r="I72" s="39"/>
     </row>
-    <row r="73" spans="1:9" ht="13.5" customHeight="1">
+    <row r="73" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="16" t="s">
         <v>85</v>
       </c>
@@ -5958,7 +5958,7 @@
       <c r="H73" s="39"/>
       <c r="I73" s="39"/>
     </row>
-    <row r="74" spans="1:9" ht="13.5" customHeight="1">
+    <row r="74" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C74" s="17" t="s">
         <v>18</v>
       </c>
@@ -5973,7 +5973,7 @@
       <c r="H74" s="39"/>
       <c r="I74" s="39"/>
     </row>
-    <row r="75" spans="1:9" ht="13.5" customHeight="1">
+    <row r="75" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="38" t="s">
         <v>86</v>
       </c>
@@ -5991,7 +5991,7 @@
       <c r="H75" s="45"/>
       <c r="I75" s="45"/>
     </row>
-    <row r="76" spans="1:9" ht="13.5" customHeight="1">
+    <row r="76" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="38" t="s">
         <v>87</v>
       </c>
@@ -6009,7 +6009,7 @@
       <c r="H76" s="45"/>
       <c r="I76" s="45"/>
     </row>
-    <row r="77" spans="1:9" ht="13.5" customHeight="1">
+    <row r="77" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="38" t="s">
         <v>88</v>
       </c>
@@ -6024,7 +6024,7 @@
       </c>
       <c r="F77" s="39"/>
     </row>
-    <row r="78" spans="1:9" ht="13.5" customHeight="1">
+    <row r="78" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="38" t="s">
         <v>89</v>
       </c>
@@ -6042,7 +6042,7 @@
       <c r="H78" s="45"/>
       <c r="I78" s="45"/>
     </row>
-    <row r="79" spans="1:9" ht="13.5" customHeight="1">
+    <row r="79" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="38" t="s">
         <v>90</v>
       </c>
@@ -6060,7 +6060,7 @@
       <c r="H79" s="45"/>
       <c r="I79" s="45"/>
     </row>
-    <row r="80" spans="1:9" ht="13.5" customHeight="1">
+    <row r="80" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="38" t="s">
         <v>91</v>
       </c>
@@ -6078,7 +6078,7 @@
       <c r="H80" s="45"/>
       <c r="I80" s="45"/>
     </row>
-    <row r="81" spans="1:9" ht="13.5" customHeight="1">
+    <row r="81" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="38" t="s">
         <v>92</v>
       </c>
@@ -6096,7 +6096,7 @@
       <c r="H81" s="45"/>
       <c r="I81" s="45"/>
     </row>
-    <row r="82" spans="1:9" ht="13.5" customHeight="1">
+    <row r="82" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="38" t="s">
         <v>93</v>
       </c>
@@ -6114,7 +6114,7 @@
       <c r="H82" s="45"/>
       <c r="I82" s="45"/>
     </row>
-    <row r="83" spans="1:9" ht="14">
+    <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B83" s="38" t="s">
         <v>94</v>
       </c>
@@ -6132,7 +6132,7 @@
       <c r="H83" s="39"/>
       <c r="I83" s="39"/>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="39"/>
       <c r="B84" s="40"/>
       <c r="C84" s="39"/>
@@ -6143,7 +6143,7 @@
       <c r="H84" s="39"/>
       <c r="I84" s="39"/>
     </row>
-    <row r="85" spans="1:9" ht="15" customHeight="1">
+    <row r="85" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="46"/>
       <c r="B85" s="47"/>
       <c r="C85" s="48"/>
@@ -6154,7 +6154,7 @@
       <c r="H85" s="48"/>
       <c r="I85" s="39"/>
     </row>
-    <row r="86" spans="1:9" ht="14">
+    <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="48"/>
       <c r="B86" s="47"/>
       <c r="C86" s="49"/>
@@ -6165,7 +6165,7 @@
       <c r="H86" s="48"/>
       <c r="I86" s="39"/>
     </row>
-    <row r="87" spans="1:9" ht="14">
+    <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="29" t="s">
         <v>95</v>
       </c>
@@ -6177,7 +6177,7 @@
       <c r="G87" s="50"/>
       <c r="H87" s="50"/>
     </row>
-    <row r="88" spans="1:9" ht="14">
+    <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="50"/>
       <c r="B88" s="50"/>
       <c r="C88" s="30" t="s">
@@ -6193,7 +6193,7 @@
       <c r="G88" s="50"/>
       <c r="H88" s="50"/>
     </row>
-    <row r="89" spans="1:9" ht="14">
+    <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="50"/>
       <c r="B89" s="31" t="s">
         <v>96</v>
@@ -6211,7 +6211,7 @@
       <c r="G89" s="50"/>
       <c r="H89" s="50"/>
     </row>
-    <row r="90" spans="1:9" ht="14">
+    <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="50"/>
       <c r="B90" s="31" t="s">
         <v>97</v>
@@ -6229,7 +6229,7 @@
       <c r="G90" s="50"/>
       <c r="H90" s="50"/>
     </row>
-    <row r="91" spans="1:9" ht="13.5" customHeight="1">
+    <row r="91" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="50"/>
       <c r="B91" s="31" t="s">
         <v>98</v>
@@ -6247,7 +6247,7 @@
       <c r="G91" s="50"/>
       <c r="H91" s="50"/>
     </row>
-    <row r="92" spans="1:9" ht="13.5" customHeight="1">
+    <row r="92" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="50"/>
       <c r="B92" s="31" t="s">
         <v>99</v>
@@ -6265,7 +6265,7 @@
       <c r="G92" s="50"/>
       <c r="H92" s="50"/>
     </row>
-    <row r="93" spans="1:9" ht="14">
+    <row r="93" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="50"/>
       <c r="B93" s="31" t="s">
         <v>100</v>
@@ -6283,7 +6283,7 @@
       <c r="G93" s="50"/>
       <c r="H93" s="50"/>
     </row>
-    <row r="94" spans="1:9" ht="14">
+    <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="50"/>
       <c r="B94" s="31" t="s">
         <v>101</v>
@@ -6301,7 +6301,7 @@
       <c r="G94" s="50"/>
       <c r="H94" s="50"/>
     </row>
-    <row r="95" spans="1:9" ht="14">
+    <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="50"/>
       <c r="B95" s="31" t="s">
         <v>102</v>
@@ -6319,17 +6319,17 @@
       <c r="G95" s="50"/>
       <c r="H95" s="50"/>
     </row>
-    <row r="96" spans="1:9" ht="14">
+    <row r="96" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="F96" s="50"/>
       <c r="G96" s="50"/>
       <c r="H96" s="50"/>
     </row>
-    <row r="97" spans="6:8" ht="14">
+    <row r="97" spans="6:8" ht="15" x14ac:dyDescent="0.25">
       <c r="F97" s="50"/>
       <c r="G97" s="50"/>
       <c r="H97" s="50"/>
     </row>
-    <row r="98" spans="6:8" ht="14">
+    <row r="98" spans="6:8" ht="15" x14ac:dyDescent="0.25">
       <c r="F98" s="50"/>
       <c r="G98" s="50"/>
       <c r="H98" s="50"/>
@@ -6353,9 +6353,9 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.5" customHeight="1">
+    <row r="1" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6363,7 +6363,7 @@
       <c r="D1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="13.5" customHeight="1">
+    <row r="2" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="13.5" customHeight="1">
+    <row r="3" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -6406,7 +6406,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13.5" customHeight="1">
+    <row r="4" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -6448,14 +6448,14 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.5" customHeight="1">
+    <row r="1" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="13.5" customHeight="1">
+    <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="4">
         <v>2000</v>
       </c>
@@ -6523,7 +6523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13.5" customHeight="1">
+    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -6557,7 +6557,7 @@
       </c>
       <c r="Z3" s="8"/>
     </row>
-    <row r="4" spans="1:26" ht="13.5" customHeight="1">
+    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -6599,7 +6599,7 @@
       </c>
       <c r="Z4" s="8"/>
     </row>
-    <row r="5" spans="1:26" ht="13.5" customHeight="1">
+    <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -6633,7 +6633,7 @@
       </c>
       <c r="Z5" s="8"/>
     </row>
-    <row r="7" spans="1:26" ht="13.5" customHeight="1">
+    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -6667,7 +6667,7 @@
       </c>
       <c r="Z7" s="8"/>
     </row>
-    <row r="8" spans="1:26" ht="13.5" customHeight="1">
+    <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -6709,7 +6709,7 @@
       </c>
       <c r="Z8" s="8"/>
     </row>
-    <row r="9" spans="1:26" ht="13.5" customHeight="1">
+    <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -6765,14 +6765,14 @@
       <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.5" customHeight="1">
+    <row r="1" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="13.5" customHeight="1">
+    <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="4">
         <v>2000</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13.5" customHeight="1">
+    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -6874,7 +6874,7 @@
       </c>
       <c r="Z3" s="10"/>
     </row>
-    <row r="4" spans="1:26" ht="13.5" customHeight="1">
+    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -6914,7 +6914,7 @@
       </c>
       <c r="Z4" s="11"/>
     </row>
-    <row r="5" spans="1:26" ht="13.5" customHeight="1">
+    <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -6948,7 +6948,7 @@
       </c>
       <c r="Z5" s="10"/>
     </row>
-    <row r="7" spans="1:26" ht="13.5" customHeight="1">
+    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -6982,7 +6982,7 @@
       </c>
       <c r="Z7" s="10"/>
     </row>
-    <row r="8" spans="1:26" ht="13.5" customHeight="1">
+    <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -7022,7 +7022,7 @@
       </c>
       <c r="Z8" s="10"/>
     </row>
-    <row r="9" spans="1:26" ht="13.5" customHeight="1">
+    <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -7076,14 +7076,14 @@
       <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4">
         <v>2000</v>
       </c>
@@ -7151,7 +7151,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -7186,7 +7186,7 @@
       </c>
       <c r="Y3" s="10"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -7221,12 +7221,12 @@
       </c>
       <c r="Y4" s="10"/>
     </row>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1">
+    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="4">
         <v>2000</v>
       </c>
@@ -7294,7 +7294,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -7327,7 +7327,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -7360,12 +7360,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1">
+    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="4">
         <v>2000</v>
       </c>
@@ -7433,7 +7433,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:25" ht="13.5" customHeight="1">
+    <row r="17" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -7466,7 +7466,7 @@
       </c>
       <c r="Y17" s="10"/>
     </row>
-    <row r="18" spans="2:25" ht="13.5" customHeight="1">
+    <row r="18" spans="2:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -7516,18 +7516,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4">
         <v>2000</v>
       </c>
@@ -7595,7 +7595,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -7628,7 +7628,7 @@
       </c>
       <c r="Y3" s="12"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -7661,12 +7661,12 @@
       </c>
       <c r="Y4" s="12"/>
     </row>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1">
+    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="4">
         <v>2000</v>
       </c>
@@ -7734,7 +7734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>26</v>
       </c>
@@ -7766,12 +7766,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1">
+    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1">
+    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="4">
         <v>2000</v>
       </c>
@@ -7839,7 +7839,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>28</v>
       </c>
@@ -7879,12 +7879,12 @@
       </c>
       <c r="Y16" s="5"/>
     </row>
-    <row r="20" spans="1:25" ht="14">
+    <row r="20" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="61" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="14">
+    <row r="21" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="C21" s="17">
         <v>2000</v>
       </c>
@@ -7952,7 +7952,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="14">
+    <row r="22" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
         <v>28</v>
       </c>
@@ -7988,12 +7988,12 @@
       </c>
       <c r="Y22" s="55"/>
     </row>
-    <row r="26" spans="1:25" ht="13.5" customHeight="1">
+    <row r="26" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="13.5" customHeight="1">
+    <row r="27" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="4">
         <v>2000</v>
       </c>
@@ -8061,7 +8061,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="13.5" customHeight="1">
+    <row r="28" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -8094,7 +8094,7 @@
       </c>
       <c r="Y28" s="12"/>
     </row>
-    <row r="29" spans="1:25" ht="13.5" customHeight="1">
+    <row r="29" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -8127,12 +8127,12 @@
       </c>
       <c r="Y29" s="12"/>
     </row>
-    <row r="33" spans="1:25" ht="13.5" customHeight="1">
+    <row r="33" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="13.5" customHeight="1">
+    <row r="34" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="4">
         <v>2000</v>
       </c>
@@ -8200,7 +8200,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="13.5" customHeight="1">
+    <row r="35" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>28</v>
       </c>
@@ -8232,12 +8232,12 @@
       </c>
       <c r="Y35" s="5"/>
     </row>
-    <row r="39" spans="1:25" ht="13.5" customHeight="1">
+    <row r="39" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="13.5" customHeight="1">
+    <row r="40" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="4">
         <v>2000</v>
       </c>
@@ -8305,7 +8305,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="13.5" customHeight="1">
+    <row r="41" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -8362,12 +8362,12 @@
       </c>
       <c r="Y41" s="14"/>
     </row>
-    <row r="45" spans="1:25" ht="13.5" customHeight="1">
+    <row r="45" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="13.5" customHeight="1">
+    <row r="46" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="4">
         <v>2000</v>
       </c>
@@ -8435,7 +8435,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="13.5" customHeight="1">
+    <row r="47" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
         <v>28</v>
       </c>
@@ -8489,14 +8489,14 @@
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4">
         <v>2000</v>
       </c>
@@ -8564,7 +8564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>28</v>
       </c>
@@ -8596,12 +8596,12 @@
       </c>
       <c r="Y3" s="14"/>
     </row>
-    <row r="7" spans="1:25" ht="13.5" customHeight="1">
+    <row r="7" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1">
+    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="4">
         <v>2000</v>
       </c>
@@ -8669,7 +8669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
@@ -8699,12 +8699,12 @@
       </c>
       <c r="Y9" s="14"/>
     </row>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1">
+    <row r="13" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="13.5" customHeight="1">
+    <row r="14" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="4">
         <v>2000</v>
       </c>
@@ -8772,7 +8772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1">
+    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>28</v>
       </c>
@@ -8802,12 +8802,12 @@
       </c>
       <c r="Y15" s="14"/>
     </row>
-    <row r="19" spans="1:25" ht="13.5" customHeight="1">
+    <row r="19" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="13.5" customHeight="1">
+    <row r="20" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="4">
         <v>2000</v>
       </c>
@@ -8875,7 +8875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="13.5" customHeight="1">
+    <row r="21" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>28</v>
       </c>
@@ -8905,12 +8905,12 @@
       </c>
       <c r="Y21" s="14"/>
     </row>
-    <row r="25" spans="1:25" ht="13.5" customHeight="1">
+    <row r="25" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="13.5" customHeight="1">
+    <row r="26" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="4">
         <v>2000</v>
       </c>
@@ -8978,7 +8978,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="13.5" customHeight="1">
+    <row r="27" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>28</v>
       </c>
@@ -9008,12 +9008,12 @@
       </c>
       <c r="Y27" s="14"/>
     </row>
-    <row r="31" spans="1:25" ht="13.5" customHeight="1">
+    <row r="31" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="13.5" customHeight="1">
+    <row r="32" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="4">
         <v>2000</v>
       </c>
@@ -9081,7 +9081,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="13.5" customHeight="1">
+    <row r="33" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>28</v>
       </c>
@@ -9111,12 +9111,12 @@
       </c>
       <c r="Y33" s="14"/>
     </row>
-    <row r="37" spans="1:25" ht="13.5" customHeight="1">
+    <row r="37" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="13.5" customHeight="1">
+    <row r="38" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="4">
         <v>2000</v>
       </c>
@@ -9184,7 +9184,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="13.5" customHeight="1">
+    <row r="39" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>28</v>
       </c>
@@ -9214,12 +9214,12 @@
       </c>
       <c r="Y39" s="14"/>
     </row>
-    <row r="43" spans="1:25" ht="14">
+    <row r="43" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="51" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="14">
+    <row r="44" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="C44" s="52">
         <v>2000</v>
       </c>
@@ -9287,7 +9287,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="14">
+    <row r="45" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="B45" s="52" t="s">
         <v>26</v>
       </c>
@@ -9317,12 +9317,12 @@
       </c>
       <c r="Y45" s="53"/>
     </row>
-    <row r="49" spans="1:25" ht="14">
+    <row r="49" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="51" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="14">
+    <row r="50" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="C50" s="52">
         <v>2000</v>
       </c>
@@ -9390,7 +9390,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:25" ht="14">
+    <row r="51" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="B51" s="52" t="s">
         <v>26</v>
       </c>
@@ -9420,12 +9420,12 @@
       </c>
       <c r="Y51" s="53"/>
     </row>
-    <row r="55" spans="1:25" ht="14">
+    <row r="55" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="51" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="14">
+    <row r="56" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="C56" s="52">
         <v>2000</v>
       </c>
@@ -9493,7 +9493,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:25" ht="14">
+    <row r="57" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="B57" s="52" t="s">
         <v>26</v>
       </c>
@@ -9523,12 +9523,12 @@
       </c>
       <c r="Y57" s="53"/>
     </row>
-    <row r="61" spans="1:25" ht="14">
+    <row r="61" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="51" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="14">
+    <row r="62" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="C62" s="52">
         <v>2000</v>
       </c>
@@ -9596,7 +9596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="14">
+    <row r="63" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="B63" s="52" t="s">
         <v>26</v>
       </c>
@@ -9626,12 +9626,12 @@
       </c>
       <c r="Y63" s="53"/>
     </row>
-    <row r="67" spans="1:25" ht="14">
+    <row r="67" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="51" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="68" spans="1:25" ht="14">
+    <row r="68" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="C68" s="52">
         <v>2000</v>
       </c>
@@ -9699,7 +9699,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="14">
+    <row r="69" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="B69" s="52" t="s">
         <v>26</v>
       </c>
@@ -9729,7 +9729,7 @@
       </c>
       <c r="Y69" s="53"/>
     </row>
-    <row r="1048546" ht="15" customHeight="1"/>
+    <row r="1048546" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -9745,18 +9745,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V39" sqref="V39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:35" ht="14">
+    <row r="1" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="14">
+    <row r="2" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="C2" s="17">
         <v>2000</v>
       </c>
@@ -9824,7 +9824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="14">
+    <row r="3" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
@@ -9856,7 +9856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="14">
+    <row r="4" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -9888,12 +9888,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="14">
+    <row r="8" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="14">
+    <row r="9" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="C9" s="17">
         <v>2000</v>
       </c>
@@ -9961,7 +9961,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="14">
+    <row r="10" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
         <v>26</v>
       </c>
@@ -9993,7 +9993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="14">
+    <row r="11" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -10029,7 +10029,7 @@
       <c r="AH11" s="17"/>
       <c r="AI11" s="17"/>
     </row>
-    <row r="12" spans="1:35" ht="14">
+    <row r="12" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -10065,7 +10065,7 @@
       <c r="AH12" s="17"/>
       <c r="AI12" s="17"/>
     </row>
-    <row r="13" spans="1:35" ht="14">
+    <row r="13" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -10101,12 +10101,12 @@
       <c r="AH13" s="17"/>
       <c r="AI13" s="17"/>
     </row>
-    <row r="14" spans="1:35" ht="14">
+    <row r="14" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="14">
+    <row r="15" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="C15" s="17">
         <v>2000</v>
       </c>
@@ -10174,7 +10174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="14">
+    <row r="16" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -10206,7 +10206,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="14">
+    <row r="17" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>12</v>
       </c>
@@ -10238,12 +10238,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="14">
+    <row r="21" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="14">
+    <row r="22" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="C22" s="17">
         <v>2000</v>
       </c>
@@ -10311,7 +10311,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:35" ht="14">
+    <row r="23" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
         <v>26</v>
       </c>
@@ -10343,7 +10343,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="1:35" ht="14">
+    <row r="24" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -10379,7 +10379,7 @@
       <c r="AH24" s="17"/>
       <c r="AI24" s="17"/>
     </row>
-    <row r="25" spans="1:35" ht="14">
+    <row r="25" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -10415,7 +10415,7 @@
       <c r="AH25" s="17"/>
       <c r="AI25" s="17"/>
     </row>
-    <row r="26" spans="1:35" ht="14">
+    <row r="26" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -10451,12 +10451,12 @@
       <c r="AH26" s="17"/>
       <c r="AI26" s="17"/>
     </row>
-    <row r="27" spans="1:35" ht="14">
+    <row r="27" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:35" ht="14">
+    <row r="28" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="C28" s="17">
         <v>2000</v>
       </c>
@@ -10524,7 +10524,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:35" ht="14">
+    <row r="29" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
         <v>26</v>
       </c>
@@ -10553,7 +10553,7 @@
         <v>17</v>
       </c>
       <c r="Y29" s="21">
-        <v>1</v>
+        <v>6300</v>
       </c>
     </row>
   </sheetData>
@@ -10575,14 +10575,14 @@
       <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" customHeight="1">
+    <row r="1" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13.5" customHeight="1">
+    <row r="2" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4">
         <v>2000</v>
       </c>
@@ -10650,7 +10650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -10683,7 +10683,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -10716,12 +10716,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1">
+    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.5" customHeight="1">
+    <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="4">
         <v>2000</v>
       </c>
@@ -10789,7 +10789,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" customHeight="1">
+    <row r="10" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -10823,7 +10823,7 @@
         <v>12.000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -10857,12 +10857,12 @@
         <v>6.0000000000000009</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.5" customHeight="1">
+    <row r="15" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1">
+    <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="4">
         <v>2000</v>
       </c>
@@ -10930,7 +10930,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="13.5" customHeight="1">
+    <row r="17" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -10963,7 +10963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="13.5" customHeight="1">
+    <row r="18" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -10996,12 +10996,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="13.5" customHeight="1">
+    <row r="22" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="13.5" customHeight="1">
+    <row r="23" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="4">
         <v>2000</v>
       </c>
@@ -11069,7 +11069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="13.5" customHeight="1">
+    <row r="24" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -11102,7 +11102,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="13.5" customHeight="1">
+    <row r="25" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -11135,12 +11135,12 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="13.5" customHeight="1">
+    <row r="29" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="13.5" customHeight="1">
+    <row r="30" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="4">
         <v>2000</v>
       </c>
@@ -11208,7 +11208,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="13.5" customHeight="1">
+    <row r="31" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -11241,7 +11241,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="13.5" customHeight="1">
+    <row r="32" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -11274,12 +11274,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="13.5" customHeight="1">
+    <row r="36" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="13.5" customHeight="1">
+    <row r="37" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="4">
         <v>2000</v>
       </c>
@@ -11347,7 +11347,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="13.5" customHeight="1">
+    <row r="38" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -11380,7 +11380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="13.5" customHeight="1">
+    <row r="39" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -11413,12 +11413,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="13.5" customHeight="1">
+    <row r="43" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="13.5" customHeight="1">
+    <row r="44" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44" s="4">
         <v>2000</v>
       </c>
@@ -11486,7 +11486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="13.5" customHeight="1">
+    <row r="45" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>

</xml_diff>

<commit_message>
Remove doubled up rows in simple.xlsx
</commit_message>
<xml_diff>
--- a/tests/simple.xlsx
+++ b/tests/simple.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rowan.martin-hughes\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1516963-EB2F-4F08-81F7-5112DAE4B779}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB424A0-C6A5-444E-9800-1135465DED67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="988" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5055" windowWidth="29040" windowHeight="15990" tabRatio="988" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="Partnerships &amp; transitions" sheetId="11" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y55" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
+    <comment ref="Y48" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="130">
   <si>
     <t>Populations</t>
   </si>
@@ -1362,10 +1362,10 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="356" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="12" borderId="0" xfId="356" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="357">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -3363,8 +3363,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>112455</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>36255</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3417,8 +3417,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>112455</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>36255</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3471,8 +3471,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>112455</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>36255</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3525,8 +3525,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>112455</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>36255</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3580,7 +3580,7 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>182880</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>33645</xdr:rowOff>
+      <xdr:rowOff>147945</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3630,8 +3630,8 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>588495</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>158270</xdr:rowOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>110645</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3687,8 +3687,8 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>588495</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>158270</xdr:rowOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>110645</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3744,7 +3744,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3793,7 +3793,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3842,8 +3842,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>117475</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3903,8 +3903,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>117475</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3964,8 +3964,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>117475</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4025,8 +4025,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>117475</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4086,8 +4086,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>117475</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4147,8 +4147,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>117475</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4208,8 +4208,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>117475</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4269,8 +4269,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>117475</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5000,15 +5000,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="82" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="81"/>
+      <c r="A2" s="82"/>
     </row>
     <row r="3" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="81"/>
+      <c r="A3" s="82"/>
     </row>
     <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="64"/>
@@ -5797,7 +5797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
@@ -8207,10 +8207,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Y55"/>
+  <dimension ref="A1:Y48"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:AZ30"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8850,12 +8850,12 @@
       </c>
       <c r="Y30" s="12"/>
     </row>
-    <row r="34" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="4">
         <v>2000</v>
       </c>
@@ -8923,409 +8923,270 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="str">
-        <f>Populations!$C$3</f>
-        <v>M 15-49</v>
-      </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
-      <c r="P36" s="12"/>
-      <c r="Q36" s="12">
-        <v>0</v>
-      </c>
-      <c r="R36" s="12"/>
-      <c r="S36" s="12"/>
-      <c r="T36" s="12"/>
-      <c r="U36" s="12"/>
-      <c r="V36" s="12"/>
-      <c r="W36" s="12"/>
+    <row r="36" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5">
+        <v>200</v>
+      </c>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="5"/>
+      <c r="V36" s="5"/>
+      <c r="W36" s="5"/>
       <c r="X36" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="Y36" s="12"/>
-    </row>
-    <row r="37" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="str">
+      <c r="Y36" s="5"/>
+    </row>
+    <row r="40" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="4">
+        <v>2000</v>
+      </c>
+      <c r="D41" s="4">
+        <v>2001</v>
+      </c>
+      <c r="E41" s="4">
+        <v>2002</v>
+      </c>
+      <c r="F41" s="4">
+        <v>2003</v>
+      </c>
+      <c r="G41" s="4">
+        <v>2004</v>
+      </c>
+      <c r="H41" s="4">
+        <v>2005</v>
+      </c>
+      <c r="I41" s="4">
+        <v>2006</v>
+      </c>
+      <c r="J41" s="4">
+        <v>2007</v>
+      </c>
+      <c r="K41" s="4">
+        <v>2008</v>
+      </c>
+      <c r="L41" s="4">
+        <v>2009</v>
+      </c>
+      <c r="M41" s="4">
+        <v>2010</v>
+      </c>
+      <c r="N41" s="4">
+        <v>2011</v>
+      </c>
+      <c r="O41" s="4">
+        <v>2012</v>
+      </c>
+      <c r="P41" s="4">
+        <v>2013</v>
+      </c>
+      <c r="Q41" s="4">
+        <v>2014</v>
+      </c>
+      <c r="R41" s="4">
+        <v>2015</v>
+      </c>
+      <c r="S41" s="4">
+        <v>2016</v>
+      </c>
+      <c r="T41" s="4">
+        <v>2017</v>
+      </c>
+      <c r="U41" s="4">
+        <v>2018</v>
+      </c>
+      <c r="V41" s="4">
+        <v>2019</v>
+      </c>
+      <c r="W41" s="4">
+        <v>2020</v>
+      </c>
+      <c r="Y41" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="12"/>
-      <c r="Q37" s="12">
-        <v>0</v>
-      </c>
-      <c r="R37" s="12"/>
-      <c r="S37" s="12"/>
-      <c r="T37" s="12"/>
-      <c r="U37" s="12"/>
-      <c r="V37" s="12"/>
-      <c r="W37" s="12"/>
-      <c r="X37" s="7" t="s">
+      <c r="C42" s="14">
+        <v>4.5925296336727497E-2</v>
+      </c>
+      <c r="D42" s="14">
+        <v>4.53240226108024E-2</v>
+      </c>
+      <c r="E42" s="14">
+        <v>4.52581785313017E-2</v>
+      </c>
+      <c r="F42" s="14">
+        <v>4.5643569591584499E-2</v>
+      </c>
+      <c r="G42" s="14">
+        <v>4.6393022020567498E-2</v>
+      </c>
+      <c r="H42" s="14">
+        <v>4.73805326183886E-2</v>
+      </c>
+      <c r="I42" s="14">
+        <v>4.8776034491919598E-2</v>
+      </c>
+      <c r="J42" s="14">
+        <v>5.0081489017354597E-2</v>
+      </c>
+      <c r="K42" s="14">
+        <v>5.1207019154705699E-2</v>
+      </c>
+      <c r="L42" s="14">
+        <v>5.2116086916866103E-2</v>
+      </c>
+      <c r="M42" s="14">
+        <v>5.2784489362924701E-2</v>
+      </c>
+      <c r="N42" s="14">
+        <v>5.21151813595171E-2</v>
+      </c>
+      <c r="O42" s="14">
+        <v>5.2484499496074803E-2</v>
+      </c>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="14"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="14"/>
+      <c r="X42" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="Y37" s="12"/>
-    </row>
-    <row r="41" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C42" s="4">
+      <c r="Y42" s="14"/>
+    </row>
+    <row r="46" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="4">
         <v>2000</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D47" s="4">
         <v>2001</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E47" s="4">
         <v>2002</v>
       </c>
-      <c r="F42" s="4">
+      <c r="F47" s="4">
         <v>2003</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G47" s="4">
         <v>2004</v>
       </c>
-      <c r="H42" s="4">
+      <c r="H47" s="4">
         <v>2005</v>
       </c>
-      <c r="I42" s="4">
+      <c r="I47" s="4">
         <v>2006</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J47" s="4">
         <v>2007</v>
       </c>
-      <c r="K42" s="4">
+      <c r="K47" s="4">
         <v>2008</v>
       </c>
-      <c r="L42" s="4">
+      <c r="L47" s="4">
         <v>2009</v>
       </c>
-      <c r="M42" s="4">
+      <c r="M47" s="4">
         <v>2010</v>
       </c>
-      <c r="N42" s="4">
+      <c r="N47" s="4">
         <v>2011</v>
       </c>
-      <c r="O42" s="4">
+      <c r="O47" s="4">
         <v>2012</v>
       </c>
-      <c r="P42" s="4">
+      <c r="P47" s="4">
         <v>2013</v>
       </c>
-      <c r="Q42" s="4">
+      <c r="Q47" s="4">
         <v>2014</v>
       </c>
-      <c r="R42" s="4">
+      <c r="R47" s="4">
         <v>2015</v>
       </c>
-      <c r="S42" s="4">
+      <c r="S47" s="4">
         <v>2016</v>
       </c>
-      <c r="T42" s="4">
+      <c r="T47" s="4">
         <v>2017</v>
       </c>
-      <c r="U42" s="4">
+      <c r="U47" s="4">
         <v>2018</v>
       </c>
-      <c r="V42" s="4">
+      <c r="V47" s="4">
         <v>2019</v>
       </c>
-      <c r="W42" s="4">
+      <c r="W47" s="4">
         <v>2020</v>
       </c>
-      <c r="Y42" s="4" t="s">
+      <c r="Y47" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
+    <row r="48" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5">
-        <v>200</v>
-      </c>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="5"/>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="5"/>
-      <c r="U43" s="5"/>
-      <c r="V43" s="5"/>
-      <c r="W43" s="5"/>
-      <c r="X43" s="7" t="s">
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="12"/>
+      <c r="M48" s="12"/>
+      <c r="N48" s="12"/>
+      <c r="O48" s="12"/>
+      <c r="P48" s="12"/>
+      <c r="Q48" s="12"/>
+      <c r="R48" s="12"/>
+      <c r="S48" s="12"/>
+      <c r="T48" s="12"/>
+      <c r="U48" s="12"/>
+      <c r="V48" s="12"/>
+      <c r="W48" s="12"/>
+      <c r="X48" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="Y43" s="5"/>
-    </row>
-    <row r="47" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D48" s="4">
-        <v>2001</v>
-      </c>
-      <c r="E48" s="4">
-        <v>2002</v>
-      </c>
-      <c r="F48" s="4">
-        <v>2003</v>
-      </c>
-      <c r="G48" s="4">
-        <v>2004</v>
-      </c>
-      <c r="H48" s="4">
-        <v>2005</v>
-      </c>
-      <c r="I48" s="4">
-        <v>2006</v>
-      </c>
-      <c r="J48" s="4">
-        <v>2007</v>
-      </c>
-      <c r="K48" s="4">
-        <v>2008</v>
-      </c>
-      <c r="L48" s="4">
-        <v>2009</v>
-      </c>
-      <c r="M48" s="4">
-        <v>2010</v>
-      </c>
-      <c r="N48" s="4">
-        <v>2011</v>
-      </c>
-      <c r="O48" s="4">
-        <v>2012</v>
-      </c>
-      <c r="P48" s="4">
-        <v>2013</v>
-      </c>
-      <c r="Q48" s="4">
-        <v>2014</v>
-      </c>
-      <c r="R48" s="4">
-        <v>2015</v>
-      </c>
-      <c r="S48" s="4">
-        <v>2016</v>
-      </c>
-      <c r="T48" s="4">
-        <v>2017</v>
-      </c>
-      <c r="U48" s="4">
-        <v>2018</v>
-      </c>
-      <c r="V48" s="4">
-        <v>2019</v>
-      </c>
-      <c r="W48" s="4">
-        <v>2020</v>
-      </c>
-      <c r="Y48" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="str">
-        <f>Populations!$C$4</f>
-        <v>F 15-49</v>
-      </c>
-      <c r="C49" s="14">
-        <v>4.5925296336727497E-2</v>
-      </c>
-      <c r="D49" s="14">
-        <v>4.53240226108024E-2</v>
-      </c>
-      <c r="E49" s="14">
-        <v>4.52581785313017E-2</v>
-      </c>
-      <c r="F49" s="14">
-        <v>4.5643569591584499E-2</v>
-      </c>
-      <c r="G49" s="14">
-        <v>4.6393022020567498E-2</v>
-      </c>
-      <c r="H49" s="14">
-        <v>4.73805326183886E-2</v>
-      </c>
-      <c r="I49" s="14">
-        <v>4.8776034491919598E-2</v>
-      </c>
-      <c r="J49" s="14">
-        <v>5.0081489017354597E-2</v>
-      </c>
-      <c r="K49" s="14">
-        <v>5.1207019154705699E-2</v>
-      </c>
-      <c r="L49" s="14">
-        <v>5.2116086916866103E-2</v>
-      </c>
-      <c r="M49" s="14">
-        <v>5.2784489362924701E-2</v>
-      </c>
-      <c r="N49" s="14">
-        <v>5.21151813595171E-2</v>
-      </c>
-      <c r="O49" s="14">
-        <v>5.2484499496074803E-2</v>
-      </c>
-      <c r="P49" s="14"/>
-      <c r="Q49" s="14"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="14"/>
-      <c r="T49" s="14"/>
-      <c r="U49" s="14"/>
-      <c r="V49" s="14"/>
-      <c r="W49" s="14"/>
-      <c r="X49" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y49" s="14"/>
-    </row>
-    <row r="53" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="54" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D54" s="4">
-        <v>2001</v>
-      </c>
-      <c r="E54" s="4">
-        <v>2002</v>
-      </c>
-      <c r="F54" s="4">
-        <v>2003</v>
-      </c>
-      <c r="G54" s="4">
-        <v>2004</v>
-      </c>
-      <c r="H54" s="4">
-        <v>2005</v>
-      </c>
-      <c r="I54" s="4">
-        <v>2006</v>
-      </c>
-      <c r="J54" s="4">
-        <v>2007</v>
-      </c>
-      <c r="K54" s="4">
-        <v>2008</v>
-      </c>
-      <c r="L54" s="4">
-        <v>2009</v>
-      </c>
-      <c r="M54" s="4">
-        <v>2010</v>
-      </c>
-      <c r="N54" s="4">
-        <v>2011</v>
-      </c>
-      <c r="O54" s="4">
-        <v>2012</v>
-      </c>
-      <c r="P54" s="4">
-        <v>2013</v>
-      </c>
-      <c r="Q54" s="4">
-        <v>2014</v>
-      </c>
-      <c r="R54" s="4">
-        <v>2015</v>
-      </c>
-      <c r="S54" s="4">
-        <v>2016</v>
-      </c>
-      <c r="T54" s="4">
-        <v>2017</v>
-      </c>
-      <c r="U54" s="4">
-        <v>2018</v>
-      </c>
-      <c r="V54" s="4">
-        <v>2019</v>
-      </c>
-      <c r="W54" s="4">
-        <v>2020</v>
-      </c>
-      <c r="Y54" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="55" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="12"/>
-      <c r="L55" s="12"/>
-      <c r="M55" s="12"/>
-      <c r="N55" s="12"/>
-      <c r="O55" s="12"/>
-      <c r="P55" s="12"/>
-      <c r="Q55" s="12"/>
-      <c r="R55" s="12"/>
-      <c r="S55" s="12"/>
-      <c r="T55" s="12"/>
-      <c r="U55" s="12"/>
-      <c r="V55" s="12"/>
-      <c r="W55" s="12"/>
-      <c r="X55" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y55" s="15">
+      <c r="Y48" s="15">
         <f>14/100*87/100</f>
         <v>0.12180000000000002</v>
       </c>
@@ -11344,10 +11205,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AI55"/>
+  <dimension ref="A1:AI48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:AZ33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12191,7 +12052,7 @@
     </row>
     <row r="34" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:35" ht="15" x14ac:dyDescent="0.25">
@@ -12263,187 +12124,378 @@
       </c>
     </row>
     <row r="36" spans="1:35" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10"/>
-      <c r="S36" s="10"/>
-      <c r="T36" s="10"/>
-      <c r="U36" s="10"/>
-      <c r="V36" s="10"/>
-      <c r="W36" s="10"/>
+      <c r="B36" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="20"/>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="20"/>
+      <c r="S36" s="20"/>
+      <c r="T36" s="20"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="20"/>
+      <c r="W36" s="20"/>
       <c r="X36" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="Y36" s="37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:35" ht="15" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
-      <c r="Q37" s="10"/>
-      <c r="R37" s="10"/>
-      <c r="S37" s="10"/>
-      <c r="T37" s="10"/>
-      <c r="U37" s="10"/>
-      <c r="V37" s="10"/>
-      <c r="W37" s="10"/>
-      <c r="X37" s="19" t="s">
+      <c r="Y36" s="21">
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="Z40" s="62"/>
+      <c r="AA40" s="62"/>
+      <c r="AB40" s="62"/>
+      <c r="AC40" s="62"/>
+      <c r="AD40" s="62"/>
+      <c r="AE40" s="62"/>
+      <c r="AF40" s="62"/>
+      <c r="AG40" s="62"/>
+      <c r="AH40" s="62"/>
+      <c r="AI40" s="62"/>
+    </row>
+    <row r="41" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+      <c r="C41" s="17">
+        <v>2000</v>
+      </c>
+      <c r="D41" s="17">
+        <v>2001</v>
+      </c>
+      <c r="E41" s="17">
+        <v>2002</v>
+      </c>
+      <c r="F41" s="17">
+        <v>2003</v>
+      </c>
+      <c r="G41" s="17">
+        <v>2004</v>
+      </c>
+      <c r="H41" s="17">
+        <v>2005</v>
+      </c>
+      <c r="I41" s="17">
+        <v>2006</v>
+      </c>
+      <c r="J41" s="17">
+        <v>2007</v>
+      </c>
+      <c r="K41" s="17">
+        <v>2008</v>
+      </c>
+      <c r="L41" s="17">
+        <v>2009</v>
+      </c>
+      <c r="M41" s="17">
+        <v>2010</v>
+      </c>
+      <c r="N41" s="17">
+        <v>2011</v>
+      </c>
+      <c r="O41" s="17">
+        <v>2012</v>
+      </c>
+      <c r="P41" s="17">
+        <v>2013</v>
+      </c>
+      <c r="Q41" s="17">
+        <v>2014</v>
+      </c>
+      <c r="R41" s="17">
+        <v>2015</v>
+      </c>
+      <c r="S41" s="17">
+        <v>2016</v>
+      </c>
+      <c r="T41" s="17">
+        <v>2017</v>
+      </c>
+      <c r="U41" s="17">
+        <v>2018</v>
+      </c>
+      <c r="V41" s="17">
+        <v>2019</v>
+      </c>
+      <c r="W41" s="17">
+        <v>2020</v>
+      </c>
+      <c r="Y41" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z41" s="62"/>
+      <c r="AA41" s="62"/>
+      <c r="AB41" s="62"/>
+      <c r="AC41" s="62"/>
+      <c r="AD41" s="62"/>
+      <c r="AE41" s="62"/>
+      <c r="AF41" s="62"/>
+      <c r="AG41" s="62"/>
+      <c r="AH41" s="62"/>
+      <c r="AI41" s="62"/>
+    </row>
+    <row r="42" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+      <c r="B42" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="20">
+        <v>0</v>
+      </c>
+      <c r="D42" s="79"/>
+      <c r="E42" s="79"/>
+      <c r="F42" s="79"/>
+      <c r="G42" s="79"/>
+      <c r="H42" s="79"/>
+      <c r="I42" s="79"/>
+      <c r="J42" s="79"/>
+      <c r="K42" s="79"/>
+      <c r="L42" s="79"/>
+      <c r="M42" s="79"/>
+      <c r="N42" s="79"/>
+      <c r="O42" s="79"/>
+      <c r="P42" s="79"/>
+      <c r="Q42" s="79"/>
+      <c r="R42" s="79">
+        <v>0.8</v>
+      </c>
+      <c r="S42" s="79"/>
+      <c r="T42" s="79"/>
+      <c r="U42" s="79"/>
+      <c r="V42" s="79"/>
+      <c r="W42" s="79"/>
+      <c r="X42" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="Y37" s="37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:35" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:35" ht="15" x14ac:dyDescent="0.25">
-      <c r="C42" s="17">
+      <c r="Y42" s="21"/>
+      <c r="Z42" s="62"/>
+      <c r="AA42" s="62"/>
+      <c r="AB42" s="62"/>
+      <c r="AC42" s="62"/>
+      <c r="AD42" s="62"/>
+      <c r="AE42" s="62"/>
+      <c r="AF42" s="62"/>
+      <c r="AG42" s="62"/>
+      <c r="AH42" s="62"/>
+      <c r="AI42" s="62"/>
+    </row>
+    <row r="43" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="62"/>
+      <c r="B43" s="62"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="62"/>
+      <c r="G43" s="62"/>
+      <c r="H43" s="62"/>
+      <c r="I43" s="62"/>
+      <c r="J43" s="62"/>
+      <c r="K43" s="62"/>
+      <c r="L43" s="62"/>
+      <c r="M43" s="62"/>
+      <c r="N43" s="62"/>
+      <c r="O43" s="62"/>
+      <c r="P43" s="62"/>
+      <c r="Q43" s="62"/>
+      <c r="R43" s="62"/>
+      <c r="S43" s="62"/>
+      <c r="T43" s="62"/>
+      <c r="U43" s="62"/>
+      <c r="V43" s="62"/>
+      <c r="W43" s="62"/>
+      <c r="X43" s="62"/>
+      <c r="Y43" s="62"/>
+      <c r="Z43" s="62"/>
+      <c r="AA43" s="62"/>
+      <c r="AB43" s="62"/>
+      <c r="AC43" s="62"/>
+      <c r="AD43" s="62"/>
+      <c r="AE43" s="62"/>
+      <c r="AF43" s="62"/>
+      <c r="AG43" s="62"/>
+      <c r="AH43" s="62"/>
+      <c r="AI43" s="62"/>
+    </row>
+    <row r="44" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="62"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="62"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="62"/>
+      <c r="J44" s="62"/>
+      <c r="K44" s="62"/>
+      <c r="L44" s="62"/>
+      <c r="M44" s="62"/>
+      <c r="N44" s="62"/>
+      <c r="O44" s="62"/>
+      <c r="P44" s="62"/>
+      <c r="Q44" s="62"/>
+      <c r="R44" s="62"/>
+      <c r="S44" s="62"/>
+      <c r="T44" s="62"/>
+      <c r="U44" s="62"/>
+      <c r="V44" s="62"/>
+      <c r="W44" s="62"/>
+      <c r="X44" s="62"/>
+      <c r="Y44" s="62"/>
+      <c r="Z44" s="62"/>
+      <c r="AA44" s="62"/>
+      <c r="AB44" s="62"/>
+      <c r="AC44" s="62"/>
+      <c r="AD44" s="62"/>
+      <c r="AE44" s="62"/>
+      <c r="AF44" s="62"/>
+      <c r="AG44" s="62"/>
+      <c r="AH44" s="62"/>
+      <c r="AI44" s="62"/>
+    </row>
+    <row r="45" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="62"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="62"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="62"/>
+      <c r="I45" s="62"/>
+      <c r="J45" s="62"/>
+      <c r="K45" s="62"/>
+      <c r="L45" s="62"/>
+      <c r="M45" s="62"/>
+      <c r="N45" s="62"/>
+      <c r="O45" s="62"/>
+      <c r="P45" s="62"/>
+      <c r="Q45" s="62"/>
+      <c r="R45" s="62"/>
+      <c r="S45" s="62"/>
+      <c r="T45" s="62"/>
+      <c r="U45" s="62"/>
+      <c r="V45" s="62"/>
+      <c r="W45" s="62"/>
+      <c r="X45" s="62"/>
+      <c r="Y45" s="62"/>
+      <c r="Z45" s="62"/>
+      <c r="AA45" s="62"/>
+      <c r="AB45" s="62"/>
+      <c r="AC45" s="62"/>
+      <c r="AD45" s="62"/>
+      <c r="AE45" s="62"/>
+      <c r="AF45" s="62"/>
+      <c r="AG45" s="62"/>
+      <c r="AH45" s="62"/>
+      <c r="AI45" s="62"/>
+    </row>
+    <row r="46" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="Z46" s="62"/>
+      <c r="AA46" s="62"/>
+      <c r="AB46" s="62"/>
+      <c r="AC46" s="62"/>
+      <c r="AD46" s="62"/>
+      <c r="AE46" s="62"/>
+      <c r="AF46" s="62"/>
+      <c r="AG46" s="62"/>
+      <c r="AH46" s="62"/>
+      <c r="AI46" s="62"/>
+    </row>
+    <row r="47" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+      <c r="C47" s="17">
         <v>2000</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D47" s="17">
         <v>2001</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E47" s="17">
         <v>2002</v>
       </c>
-      <c r="F42" s="17">
+      <c r="F47" s="17">
         <v>2003</v>
       </c>
-      <c r="G42" s="17">
+      <c r="G47" s="17">
         <v>2004</v>
       </c>
-      <c r="H42" s="17">
+      <c r="H47" s="17">
         <v>2005</v>
       </c>
-      <c r="I42" s="17">
+      <c r="I47" s="17">
         <v>2006</v>
       </c>
-      <c r="J42" s="17">
+      <c r="J47" s="17">
         <v>2007</v>
       </c>
-      <c r="K42" s="17">
+      <c r="K47" s="17">
         <v>2008</v>
       </c>
-      <c r="L42" s="17">
+      <c r="L47" s="17">
         <v>2009</v>
       </c>
-      <c r="M42" s="17">
+      <c r="M47" s="17">
         <v>2010</v>
       </c>
-      <c r="N42" s="17">
+      <c r="N47" s="17">
         <v>2011</v>
       </c>
-      <c r="O42" s="17">
+      <c r="O47" s="17">
         <v>2012</v>
       </c>
-      <c r="P42" s="17">
+      <c r="P47" s="17">
         <v>2013</v>
       </c>
-      <c r="Q42" s="17">
+      <c r="Q47" s="17">
         <v>2014</v>
       </c>
-      <c r="R42" s="17">
+      <c r="R47" s="17">
         <v>2015</v>
       </c>
-      <c r="S42" s="17">
+      <c r="S47" s="17">
         <v>2016</v>
       </c>
-      <c r="T42" s="17">
+      <c r="T47" s="17">
         <v>2017</v>
       </c>
-      <c r="U42" s="17">
+      <c r="U47" s="17">
         <v>2018</v>
       </c>
-      <c r="V42" s="17">
+      <c r="V47" s="17">
         <v>2019</v>
       </c>
-      <c r="W42" s="17">
+      <c r="W47" s="17">
         <v>2020</v>
       </c>
-      <c r="Y42" s="17" t="s">
+      <c r="Y47" s="17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:35" ht="15" x14ac:dyDescent="0.25">
-      <c r="B43" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
-      <c r="M43" s="20"/>
-      <c r="N43" s="20"/>
-      <c r="O43" s="20"/>
-      <c r="P43" s="20"/>
-      <c r="Q43" s="20"/>
-      <c r="R43" s="20"/>
-      <c r="S43" s="20"/>
-      <c r="T43" s="20"/>
-      <c r="U43" s="20"/>
-      <c r="V43" s="20"/>
-      <c r="W43" s="20"/>
-      <c r="X43" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y43" s="21">
-        <v>6300</v>
-      </c>
-    </row>
-    <row r="47" spans="1:35" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="16"/>
       <c r="Z47" s="62"/>
       <c r="AA47" s="62"/>
       <c r="AB47" s="62"/>
@@ -12456,72 +12508,36 @@
       <c r="AI47" s="62"/>
     </row>
     <row r="48" spans="1:35" ht="15" x14ac:dyDescent="0.25">
-      <c r="C48" s="17">
-        <v>2000</v>
-      </c>
-      <c r="D48" s="17">
-        <v>2001</v>
-      </c>
-      <c r="E48" s="17">
-        <v>2002</v>
-      </c>
-      <c r="F48" s="17">
-        <v>2003</v>
-      </c>
-      <c r="G48" s="17">
-        <v>2004</v>
-      </c>
-      <c r="H48" s="17">
-        <v>2005</v>
-      </c>
-      <c r="I48" s="17">
-        <v>2006</v>
-      </c>
-      <c r="J48" s="17">
-        <v>2007</v>
-      </c>
-      <c r="K48" s="17">
-        <v>2008</v>
-      </c>
-      <c r="L48" s="17">
-        <v>2009</v>
-      </c>
-      <c r="M48" s="17">
-        <v>2010</v>
-      </c>
-      <c r="N48" s="17">
-        <v>2011</v>
-      </c>
-      <c r="O48" s="17">
-        <v>2012</v>
-      </c>
-      <c r="P48" s="17">
-        <v>2013</v>
-      </c>
-      <c r="Q48" s="17">
-        <v>2014</v>
-      </c>
-      <c r="R48" s="17">
-        <v>2015</v>
-      </c>
-      <c r="S48" s="17">
-        <v>2016</v>
-      </c>
-      <c r="T48" s="17">
-        <v>2017</v>
-      </c>
-      <c r="U48" s="17">
-        <v>2018</v>
-      </c>
-      <c r="V48" s="17">
-        <v>2019</v>
-      </c>
-      <c r="W48" s="17">
-        <v>2020</v>
-      </c>
-      <c r="Y48" s="17" t="s">
-        <v>14</v>
-      </c>
+      <c r="B48" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="20"/>
+      <c r="D48" s="79"/>
+      <c r="E48" s="79"/>
+      <c r="F48" s="79"/>
+      <c r="G48" s="79"/>
+      <c r="H48" s="79"/>
+      <c r="I48" s="79"/>
+      <c r="J48" s="79"/>
+      <c r="K48" s="79"/>
+      <c r="L48" s="79"/>
+      <c r="M48" s="79"/>
+      <c r="N48" s="79"/>
+      <c r="O48" s="79"/>
+      <c r="P48" s="79"/>
+      <c r="Q48" s="79"/>
+      <c r="R48" s="79">
+        <v>0.16</v>
+      </c>
+      <c r="S48" s="79"/>
+      <c r="T48" s="79"/>
+      <c r="U48" s="79"/>
+      <c r="V48" s="79"/>
+      <c r="W48" s="79"/>
+      <c r="X48" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y48" s="21"/>
       <c r="Z48" s="62"/>
       <c r="AA48" s="62"/>
       <c r="AB48" s="62"/>
@@ -12532,298 +12548,6 @@
       <c r="AG48" s="62"/>
       <c r="AH48" s="62"/>
       <c r="AI48" s="62"/>
-    </row>
-    <row r="49" spans="1:35" ht="15" x14ac:dyDescent="0.25">
-      <c r="B49" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C49" s="20">
-        <v>0</v>
-      </c>
-      <c r="D49" s="79"/>
-      <c r="E49" s="79"/>
-      <c r="F49" s="79"/>
-      <c r="G49" s="79"/>
-      <c r="H49" s="79"/>
-      <c r="I49" s="79"/>
-      <c r="J49" s="79"/>
-      <c r="K49" s="79"/>
-      <c r="L49" s="79"/>
-      <c r="M49" s="79"/>
-      <c r="N49" s="79"/>
-      <c r="O49" s="79"/>
-      <c r="P49" s="79"/>
-      <c r="Q49" s="79"/>
-      <c r="R49" s="79">
-        <v>0.8</v>
-      </c>
-      <c r="S49" s="79"/>
-      <c r="T49" s="79"/>
-      <c r="U49" s="79"/>
-      <c r="V49" s="79"/>
-      <c r="W49" s="79"/>
-      <c r="X49" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y49" s="21"/>
-      <c r="Z49" s="62"/>
-      <c r="AA49" s="62"/>
-      <c r="AB49" s="62"/>
-      <c r="AC49" s="62"/>
-      <c r="AD49" s="62"/>
-      <c r="AE49" s="62"/>
-      <c r="AF49" s="62"/>
-      <c r="AG49" s="62"/>
-      <c r="AH49" s="62"/>
-      <c r="AI49" s="62"/>
-    </row>
-    <row r="50" spans="1:35" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="62"/>
-      <c r="B50" s="62"/>
-      <c r="C50" s="62"/>
-      <c r="D50" s="62"/>
-      <c r="E50" s="62"/>
-      <c r="F50" s="62"/>
-      <c r="G50" s="62"/>
-      <c r="H50" s="62"/>
-      <c r="I50" s="62"/>
-      <c r="J50" s="62"/>
-      <c r="K50" s="62"/>
-      <c r="L50" s="62"/>
-      <c r="M50" s="62"/>
-      <c r="N50" s="62"/>
-      <c r="O50" s="62"/>
-      <c r="P50" s="62"/>
-      <c r="Q50" s="62"/>
-      <c r="R50" s="62"/>
-      <c r="S50" s="62"/>
-      <c r="T50" s="62"/>
-      <c r="U50" s="62"/>
-      <c r="V50" s="62"/>
-      <c r="W50" s="62"/>
-      <c r="X50" s="62"/>
-      <c r="Y50" s="62"/>
-      <c r="Z50" s="62"/>
-      <c r="AA50" s="62"/>
-      <c r="AB50" s="62"/>
-      <c r="AC50" s="62"/>
-      <c r="AD50" s="62"/>
-      <c r="AE50" s="62"/>
-      <c r="AF50" s="62"/>
-      <c r="AG50" s="62"/>
-      <c r="AH50" s="62"/>
-      <c r="AI50" s="62"/>
-    </row>
-    <row r="51" spans="1:35" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="62"/>
-      <c r="B51" s="62"/>
-      <c r="C51" s="62"/>
-      <c r="D51" s="62"/>
-      <c r="E51" s="62"/>
-      <c r="F51" s="62"/>
-      <c r="G51" s="62"/>
-      <c r="H51" s="62"/>
-      <c r="I51" s="62"/>
-      <c r="J51" s="62"/>
-      <c r="K51" s="62"/>
-      <c r="L51" s="62"/>
-      <c r="M51" s="62"/>
-      <c r="N51" s="62"/>
-      <c r="O51" s="62"/>
-      <c r="P51" s="62"/>
-      <c r="Q51" s="62"/>
-      <c r="R51" s="62"/>
-      <c r="S51" s="62"/>
-      <c r="T51" s="62"/>
-      <c r="U51" s="62"/>
-      <c r="V51" s="62"/>
-      <c r="W51" s="62"/>
-      <c r="X51" s="62"/>
-      <c r="Y51" s="62"/>
-      <c r="Z51" s="62"/>
-      <c r="AA51" s="62"/>
-      <c r="AB51" s="62"/>
-      <c r="AC51" s="62"/>
-      <c r="AD51" s="62"/>
-      <c r="AE51" s="62"/>
-      <c r="AF51" s="62"/>
-      <c r="AG51" s="62"/>
-      <c r="AH51" s="62"/>
-      <c r="AI51" s="62"/>
-    </row>
-    <row r="52" spans="1:35" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="62"/>
-      <c r="B52" s="62"/>
-      <c r="C52" s="62"/>
-      <c r="D52" s="62"/>
-      <c r="E52" s="62"/>
-      <c r="F52" s="62"/>
-      <c r="G52" s="62"/>
-      <c r="H52" s="62"/>
-      <c r="I52" s="62"/>
-      <c r="J52" s="62"/>
-      <c r="K52" s="62"/>
-      <c r="L52" s="62"/>
-      <c r="M52" s="62"/>
-      <c r="N52" s="62"/>
-      <c r="O52" s="62"/>
-      <c r="P52" s="62"/>
-      <c r="Q52" s="62"/>
-      <c r="R52" s="62"/>
-      <c r="S52" s="62"/>
-      <c r="T52" s="62"/>
-      <c r="U52" s="62"/>
-      <c r="V52" s="62"/>
-      <c r="W52" s="62"/>
-      <c r="X52" s="62"/>
-      <c r="Y52" s="62"/>
-      <c r="Z52" s="62"/>
-      <c r="AA52" s="62"/>
-      <c r="AB52" s="62"/>
-      <c r="AC52" s="62"/>
-      <c r="AD52" s="62"/>
-      <c r="AE52" s="62"/>
-      <c r="AF52" s="62"/>
-      <c r="AG52" s="62"/>
-      <c r="AH52" s="62"/>
-      <c r="AI52" s="62"/>
-    </row>
-    <row r="53" spans="1:35" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
-      <c r="Z53" s="62"/>
-      <c r="AA53" s="62"/>
-      <c r="AB53" s="62"/>
-      <c r="AC53" s="62"/>
-      <c r="AD53" s="62"/>
-      <c r="AE53" s="62"/>
-      <c r="AF53" s="62"/>
-      <c r="AG53" s="62"/>
-      <c r="AH53" s="62"/>
-      <c r="AI53" s="62"/>
-    </row>
-    <row r="54" spans="1:35" ht="15" x14ac:dyDescent="0.25">
-      <c r="C54" s="17">
-        <v>2000</v>
-      </c>
-      <c r="D54" s="17">
-        <v>2001</v>
-      </c>
-      <c r="E54" s="17">
-        <v>2002</v>
-      </c>
-      <c r="F54" s="17">
-        <v>2003</v>
-      </c>
-      <c r="G54" s="17">
-        <v>2004</v>
-      </c>
-      <c r="H54" s="17">
-        <v>2005</v>
-      </c>
-      <c r="I54" s="17">
-        <v>2006</v>
-      </c>
-      <c r="J54" s="17">
-        <v>2007</v>
-      </c>
-      <c r="K54" s="17">
-        <v>2008</v>
-      </c>
-      <c r="L54" s="17">
-        <v>2009</v>
-      </c>
-      <c r="M54" s="17">
-        <v>2010</v>
-      </c>
-      <c r="N54" s="17">
-        <v>2011</v>
-      </c>
-      <c r="O54" s="17">
-        <v>2012</v>
-      </c>
-      <c r="P54" s="17">
-        <v>2013</v>
-      </c>
-      <c r="Q54" s="17">
-        <v>2014</v>
-      </c>
-      <c r="R54" s="17">
-        <v>2015</v>
-      </c>
-      <c r="S54" s="17">
-        <v>2016</v>
-      </c>
-      <c r="T54" s="17">
-        <v>2017</v>
-      </c>
-      <c r="U54" s="17">
-        <v>2018</v>
-      </c>
-      <c r="V54" s="17">
-        <v>2019</v>
-      </c>
-      <c r="W54" s="17">
-        <v>2020</v>
-      </c>
-      <c r="Y54" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z54" s="62"/>
-      <c r="AA54" s="62"/>
-      <c r="AB54" s="62"/>
-      <c r="AC54" s="62"/>
-      <c r="AD54" s="62"/>
-      <c r="AE54" s="62"/>
-      <c r="AF54" s="62"/>
-      <c r="AG54" s="62"/>
-      <c r="AH54" s="62"/>
-      <c r="AI54" s="62"/>
-    </row>
-    <row r="55" spans="1:35" ht="15" x14ac:dyDescent="0.25">
-      <c r="B55" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C55" s="20"/>
-      <c r="D55" s="79"/>
-      <c r="E55" s="79"/>
-      <c r="F55" s="79"/>
-      <c r="G55" s="79"/>
-      <c r="H55" s="79"/>
-      <c r="I55" s="79"/>
-      <c r="J55" s="79"/>
-      <c r="K55" s="79"/>
-      <c r="L55" s="79"/>
-      <c r="M55" s="79"/>
-      <c r="N55" s="79"/>
-      <c r="O55" s="79"/>
-      <c r="P55" s="79"/>
-      <c r="Q55" s="79"/>
-      <c r="R55" s="79">
-        <v>0.16</v>
-      </c>
-      <c r="S55" s="79"/>
-      <c r="T55" s="79"/>
-      <c r="U55" s="79"/>
-      <c r="V55" s="79"/>
-      <c r="W55" s="79"/>
-      <c r="X55" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y55" s="21"/>
-      <c r="Z55" s="62"/>
-      <c r="AA55" s="62"/>
-      <c r="AB55" s="62"/>
-      <c r="AC55" s="62"/>
-      <c r="AD55" s="62"/>
-      <c r="AE55" s="62"/>
-      <c r="AF55" s="62"/>
-      <c r="AG55" s="62"/>
-      <c r="AH55" s="62"/>
-      <c r="AI55" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -13885,7 +13609,7 @@
       <c r="X52" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="Y52" s="82">
+      <c r="Y52" s="81">
         <v>0</v>
       </c>
     </row>

</xml_diff>